<commit_message>
LOCAL -  Testing with the file permissions.
</commit_message>
<xml_diff>
--- a/CLASSOPS/Derek/Derek's Log.xlsx
+++ b/CLASSOPS/Derek/Derek's Log.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="141">
   <si>
     <t>Staff Name</t>
   </si>
@@ -995,11 +995,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A38" sqref="A38:XFD38"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1643,56 +1643,6 @@
       <c r="H34" s="25"/>
       <c r="I34" s="25"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="21"/>
-      <c r="B35" s="21"/>
-      <c r="C35" s="22" t="s">
-        <v>115</v>
-      </c>
-      <c r="D35" s="23"/>
-      <c r="E35" s="21"/>
-      <c r="F35" s="23"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B36" s="10">
-        <v>42584</v>
-      </c>
-      <c r="C36" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="D36" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E36" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="F36" s="19" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B37" s="10">
-        <v>42584</v>
-      </c>
-      <c r="C37" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="D37" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="E37" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="F37" s="19" t="s">
-        <v>117</v>
-      </c>
-    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0"/>
   <sortState ref="A427:G515">
@@ -1700,13 +1650,13 @@
     <sortCondition ref="D427:D515"/>
   </sortState>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A22:A23 B6 B2 A7:A8 B9 A10:A16 B17 A18:A20 B21 A3:A5 B24 A25:A27 B28 B32 A29:A31 A33:A34 B35 A36:A1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A22:A23 B6 B2 A7:A8 B9 A10:A16 B17 A18:A20 B21 A3:A5 B24 A25:A27 B28 B32 A29:A31 A33:A1048576">
       <formula1>Task_type</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6 E2 D22:D23 D7:D8 E9 D10:D16 E17 D18:D20 E21 D3:D5 E24 D25:D27 E28 E32 D29:D31 D33:D34 E35 D36:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6 E2 D22:D23 D7:D8 E9 D10:D16 E17 D18:D20 E21 D3:D5 E24 D25:D27 E28 E32 D29:D31 D33:D1048576">
       <formula1>Building</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 A2 A9 A17 A21 A24 A28 A32 A35">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 A2 A9 A17 A21 A24 A28 A32">
       <formula1>Staff_Name</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Off by one bug fixed in the range. Update the files
</commit_message>
<xml_diff>
--- a/CLASSOPS/Derek/Derek's Log.xlsx
+++ b/CLASSOPS/Derek/Derek's Log.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="143">
   <si>
     <t>Staff Name</t>
   </si>
@@ -471,6 +471,9 @@
   </si>
   <si>
     <t>Turn off PC and projector. Leave equipment in room. Lock room. Key for room in Founders 164 storeroom.</t>
+  </si>
+  <si>
+    <t>FRIDAY</t>
   </si>
 </sst>
 </file>
@@ -603,7 +606,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -691,6 +694,21 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -998,11 +1016,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:I42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F44" sqref="F44"/>
+      <selection pane="bottomLeft" activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1743,6 +1761,36 @@
         <v>127</v>
       </c>
       <c r="F40" s="29" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="36"/>
+      <c r="B41" s="37"/>
+      <c r="C41" s="38" t="s">
+        <v>142</v>
+      </c>
+      <c r="D41" s="36"/>
+      <c r="E41" s="39"/>
+      <c r="F41" s="40"/>
+    </row>
+    <row r="42" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B42" s="26">
+        <v>42587</v>
+      </c>
+      <c r="C42" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E42" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="F42" s="29" t="s">
         <v>141</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Spell checked and permission changed
</commit_message>
<xml_diff>
--- a/CLASSOPS/Derek/Derek's Log.xlsx
+++ b/CLASSOPS/Derek/Derek's Log.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="147">
   <si>
     <t>Staff Name</t>
   </si>
@@ -474,6 +474,18 @@
   </si>
   <si>
     <t>FRIDAY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">152 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pick up mic and clip and mic stand - return to Founders 156A storeroom. Leave mic cables and matts. Turn off amp. </t>
+  </si>
+  <si>
+    <t>152</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pick up wireless keyboard and return to Founders 156A storeroom. </t>
   </si>
 </sst>
 </file>
@@ -1016,11 +1028,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I45"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C48" sqref="C48"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1842,6 +1854,76 @@
       </c>
       <c r="F45" s="29" t="s">
         <v>118</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="36"/>
+      <c r="B46" s="37"/>
+      <c r="C46" s="38" t="s">
+        <v>142</v>
+      </c>
+      <c r="D46" s="36"/>
+      <c r="E46" s="39"/>
+      <c r="F46" s="40"/>
+    </row>
+    <row r="47" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B47" s="10">
+        <v>42594</v>
+      </c>
+      <c r="C47" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="D47" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E47" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="F47" s="19" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B48" s="10">
+        <v>42594</v>
+      </c>
+      <c r="C48" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="D48" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E48" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="F48" s="19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B49" s="10">
+        <v>42594</v>
+      </c>
+      <c r="C49" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="D49" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E49" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="F49" s="19" t="s">
+        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reworked the print method to print out all the logs at the end of the execution of the application.
</commit_message>
<xml_diff>
--- a/CLASSOPS/Derek/Derek's Log.xlsx
+++ b/CLASSOPS/Derek/Derek's Log.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="151">
   <si>
     <t>Staff Name</t>
   </si>
@@ -486,6 +486,18 @@
   </si>
   <si>
     <t xml:space="preserve">Pick up wireless keyboard and return to Founders 156A storeroom. </t>
+  </si>
+  <si>
+    <t>1705</t>
+  </si>
+  <si>
+    <t>N927</t>
+  </si>
+  <si>
+    <t>215</t>
+  </si>
+  <si>
+    <t>York Room N927 is opposite Senate Chamber when you step off the elevator. Flat screen TV w/PC in back. Turn off wireless keyboard and store with TV remote in canvas bag before transporting. Door will be locked at 1710 by client if you are late. To Vari 1155.</t>
   </si>
 </sst>
 </file>
@@ -618,7 +630,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -630,38 +642,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -707,20 +689,32 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1028,625 +1022,625 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I49"/>
+  <dimension ref="A1:I53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F52" sqref="F52"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="19" style="10" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" style="9" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" style="11" customWidth="1"/>
-    <col min="6" max="6" width="60.42578125" style="19" customWidth="1"/>
+    <col min="1" max="1" width="27.7109375" style="15" customWidth="1"/>
+    <col min="2" max="2" width="19" style="26" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" style="23" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" style="24" customWidth="1"/>
+    <col min="6" max="6" width="60.42578125" style="25" customWidth="1"/>
     <col min="7" max="16384" width="22.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="27" t="s">
         <v>104</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="33" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="21"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="22" t="s">
+    <row r="2" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="D2" s="23"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="26">
         <v>42570</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="F3" s="25" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="26">
         <v>42570</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="F4" s="25" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="26">
         <v>42570</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="F5" s="19" t="s">
+      <c r="F5" s="25" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="21"/>
-      <c r="B6" s="21"/>
-      <c r="C6" s="22" t="s">
+    <row r="6" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="26">
+      <c r="B7" s="16">
         <v>42571</v>
       </c>
-      <c r="C7" s="27" t="s">
+      <c r="C7" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="D7" s="28" t="s">
+      <c r="D7" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="E7" s="27" t="s">
+      <c r="E7" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="F7" s="29" t="s">
+      <c r="F7" s="19" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="26">
+      <c r="B8" s="16">
         <v>42571</v>
       </c>
-      <c r="C8" s="30" t="s">
+      <c r="C8" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="D8" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="E8" s="25" t="s">
+      <c r="E8" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="F8" s="19" t="s">
+      <c r="F8" s="25" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="21"/>
-      <c r="B9" s="21"/>
-      <c r="C9" s="22" t="s">
+    <row r="9" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="D9" s="23"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="B10" s="26">
+      <c r="B10" s="16">
         <v>42573</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="22" t="s">
         <v>120</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="F10" s="29" t="s">
+      <c r="F10" s="19" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="B11" s="26">
+      <c r="B11" s="16">
         <v>42573</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="F11" s="19" t="s">
+      <c r="F11" s="25" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="B12" s="26">
+      <c r="B12" s="16">
         <v>42573</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E12" s="24" t="s">
         <v>121</v>
       </c>
-      <c r="F12" s="19" t="s">
+      <c r="F12" s="25" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="B13" s="26">
+      <c r="B13" s="16">
         <v>42573</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="24" t="s">
         <v>121</v>
       </c>
-      <c r="F13" s="19" t="s">
+      <c r="F13" s="25" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="B14" s="26">
+      <c r="B14" s="16">
         <v>42573</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="E14" s="24" t="s">
         <v>121</v>
       </c>
-      <c r="F14" s="19" t="s">
+      <c r="F14" s="25" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="B15" s="26">
+      <c r="B15" s="16">
         <v>42573</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="E15" s="11" t="s">
+      <c r="E15" s="24" t="s">
         <v>121</v>
       </c>
-      <c r="F15" s="19" t="s">
+      <c r="F15" s="25" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="26">
+      <c r="B16" s="16">
         <v>42573</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="E16" s="24" t="s">
         <v>121</v>
       </c>
-      <c r="F16" s="19" t="s">
+      <c r="F16" s="25" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="21"/>
-      <c r="B17" s="21"/>
-      <c r="C17" s="22" t="s">
+    <row r="17" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="11"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="D17" s="23"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="21"/>
-    </row>
-    <row r="18" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="25" t="s">
+      <c r="D17" s="13"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+    </row>
+    <row r="18" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="26">
+      <c r="B18" s="16">
         <v>42576</v>
       </c>
-      <c r="C18" s="27" t="s">
+      <c r="C18" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="D18" s="28" t="s">
+      <c r="D18" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="E18" s="27" t="s">
+      <c r="E18" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="F18" s="29" t="s">
+      <c r="F18" s="19" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="25" t="s">
+      <c r="A19" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="26">
+      <c r="B19" s="16">
         <v>42576</v>
       </c>
-      <c r="C19" s="30" t="s">
+      <c r="C19" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="D19" s="25" t="s">
+      <c r="D19" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="E19" s="30" t="s">
+      <c r="E19" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="F19" s="31" t="s">
+      <c r="F19" s="21" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="25" t="s">
+      <c r="A20" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="26">
+      <c r="B20" s="16">
         <v>42576</v>
       </c>
-      <c r="C20" s="30" t="s">
+      <c r="C20" s="20" t="s">
         <v>132</v>
       </c>
-      <c r="D20" s="25" t="s">
+      <c r="D20" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="E20" s="30" t="s">
+      <c r="E20" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="F20" s="19" t="s">
+      <c r="F20" s="25" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="21" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="21"/>
-      <c r="B21" s="21"/>
-      <c r="C21" s="22" t="s">
+    <row r="21" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="11"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="D21" s="23"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="24"/>
-      <c r="H21" s="21"/>
-      <c r="I21" s="21"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="10">
+      <c r="B22" s="26">
         <v>42577</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="D22" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="11" t="s">
+      <c r="E22" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="F22" s="19" t="s">
+      <c r="F22" s="25" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="B23" s="10">
+      <c r="B23" s="26">
         <v>42577</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="D23" s="9" t="s">
+      <c r="D23" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="E23" s="11" t="s">
+      <c r="E23" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="F23" s="19" t="s">
+      <c r="F23" s="25" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="24" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="21"/>
-      <c r="B24" s="21"/>
-      <c r="C24" s="22" t="s">
+    <row r="24" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="11"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="D24" s="23"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="23"/>
-      <c r="G24" s="24"/>
-      <c r="H24" s="21"/>
-      <c r="I24" s="21"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="25" t="s">
+      <c r="A25" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="26">
+      <c r="B25" s="16">
         <v>42578</v>
       </c>
-      <c r="C25" s="27" t="s">
+      <c r="C25" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="D25" s="28" t="s">
+      <c r="D25" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="E25" s="27" t="s">
+      <c r="E25" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="F25" s="29" t="s">
+      <c r="F25" s="19" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="25" t="s">
+      <c r="A26" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="B26" s="26">
+      <c r="B26" s="16">
         <v>42578</v>
       </c>
-      <c r="C26" s="30" t="s">
+      <c r="C26" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="D26" s="25" t="s">
+      <c r="D26" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="E26" s="25" t="s">
+      <c r="E26" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="F26" s="19" t="s">
+      <c r="F26" s="25" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="25" t="s">
+      <c r="A27" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B27" s="26">
+      <c r="B27" s="16">
         <v>42578</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="C27" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="D27" s="25" t="s">
+      <c r="D27" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="E27" s="30" t="s">
+      <c r="E27" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="F27" s="31" t="s">
+      <c r="F27" s="21" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="28" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="21"/>
-      <c r="B28" s="21"/>
-      <c r="C28" s="22" t="s">
+    <row r="28" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="11"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="D28" s="23"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="21"/>
-      <c r="I28" s="21"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="25" t="s">
+      <c r="A29" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B29" s="26">
+      <c r="B29" s="16">
         <v>42579</v>
       </c>
-      <c r="C29" s="12" t="s">
+      <c r="C29" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="D29" s="25" t="s">
+      <c r="D29" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="E29" s="30" t="s">
+      <c r="E29" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="F29" s="31" t="s">
+      <c r="F29" s="21" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="25" t="s">
+      <c r="A30" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B30" s="26">
+      <c r="B30" s="16">
         <v>42579</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="C30" s="22" t="s">
         <v>136</v>
       </c>
-      <c r="D30" s="25" t="s">
+      <c r="D30" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="E30" s="11" t="s">
+      <c r="E30" s="24" t="s">
         <v>137</v>
       </c>
-      <c r="F30" s="19" t="s">
+      <c r="F30" s="25" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="B31" s="26">
+      <c r="B31" s="16">
         <v>42579</v>
       </c>
-      <c r="C31" s="12" t="s">
+      <c r="C31" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="D31" s="9" t="s">
+      <c r="D31" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="E31" s="11" t="s">
+      <c r="E31" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="F31" s="19" t="s">
+      <c r="F31" s="25" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="21"/>
-      <c r="B32" s="21"/>
-      <c r="C32" s="22" t="s">
+      <c r="A32" s="11"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="D32" s="23"/>
-      <c r="E32" s="21"/>
-      <c r="F32" s="23"/>
-      <c r="G32" s="24"/>
-      <c r="H32" s="21"/>
-      <c r="I32" s="21"/>
-    </row>
-    <row r="33" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+      <c r="D32" s="13"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="11"/>
+    </row>
+    <row r="33" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="B33" s="26">
+      <c r="B33" s="16">
         <v>42580</v>
       </c>
-      <c r="C33" s="12" t="s">
+      <c r="C33" s="22" t="s">
         <v>120</v>
       </c>
-      <c r="D33" s="9" t="s">
+      <c r="D33" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="E33" s="11" t="s">
+      <c r="E33" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="F33" s="29" t="s">
+      <c r="F33" s="19" t="s">
         <v>126</v>
       </c>
       <c r="G33" s="3"/>
@@ -1654,276 +1648,346 @@
       <c r="I33" s="3"/>
     </row>
     <row r="34" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
+      <c r="A34" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="B34" s="26">
+      <c r="B34" s="16">
         <v>42580</v>
       </c>
-      <c r="C34" s="32" t="s">
+      <c r="C34" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="D34" s="33" t="s">
+      <c r="D34" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="E34" s="34" t="s">
+      <c r="E34" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="F34" s="35" t="s">
+      <c r="F34" s="25" t="s">
         <v>140</v>
       </c>
-      <c r="G34" s="25"/>
-      <c r="H34" s="25"/>
-      <c r="I34" s="25"/>
+      <c r="G34" s="15"/>
+      <c r="H34" s="15"/>
+      <c r="I34" s="15"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="21"/>
-      <c r="B35" s="21"/>
-      <c r="C35" s="22" t="s">
+      <c r="A35" s="11"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="D35" s="23"/>
-      <c r="E35" s="21"/>
-      <c r="F35" s="23"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="13"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
+      <c r="A36" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B36" s="10">
+      <c r="B36" s="26">
         <v>42584</v>
       </c>
-      <c r="C36" s="12" t="s">
+      <c r="C36" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="D36" s="9" t="s">
+      <c r="D36" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="E36" s="11" t="s">
+      <c r="E36" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="F36" s="19" t="s">
+      <c r="F36" s="25" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
+      <c r="A37" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="B37" s="10">
+      <c r="B37" s="26">
         <v>42584</v>
       </c>
-      <c r="C37" s="12" t="s">
+      <c r="C37" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="D37" s="9" t="s">
+      <c r="D37" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="E37" s="11" t="s">
+      <c r="E37" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="F37" s="19" t="s">
+      <c r="F37" s="25" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="21"/>
-      <c r="B38" s="21"/>
-      <c r="C38" s="22" t="s">
+      <c r="A38" s="11"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="D38" s="23"/>
-      <c r="E38" s="21"/>
-      <c r="F38" s="23"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="13"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="25" t="s">
+      <c r="A39" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B39" s="26">
+      <c r="B39" s="16">
         <v>42585</v>
       </c>
-      <c r="C39" s="27" t="s">
+      <c r="C39" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="D39" s="28" t="s">
+      <c r="D39" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="E39" s="27" t="s">
+      <c r="E39" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="F39" s="29" t="s">
+      <c r="F39" s="19" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
+      <c r="A40" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="B40" s="26">
+      <c r="B40" s="16">
         <v>42585</v>
       </c>
-      <c r="C40" s="12" t="s">
+      <c r="C40" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="D40" s="9" t="s">
+      <c r="D40" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="E40" s="11" t="s">
+      <c r="E40" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="F40" s="29" t="s">
+      <c r="F40" s="19" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="36"/>
-      <c r="B41" s="37"/>
-      <c r="C41" s="38" t="s">
+      <c r="A41" s="11"/>
+      <c r="B41" s="28"/>
+      <c r="C41" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="D41" s="36"/>
-      <c r="E41" s="39"/>
-      <c r="F41" s="40"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="32"/>
+      <c r="F41" s="34"/>
     </row>
     <row r="42" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
+      <c r="A42" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="B42" s="26">
+      <c r="B42" s="16">
         <v>42587</v>
       </c>
-      <c r="C42" s="12" t="s">
+      <c r="C42" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="D42" s="9" t="s">
+      <c r="D42" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="E42" s="11" t="s">
+      <c r="E42" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="F42" s="29" t="s">
+      <c r="F42" s="19" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="36"/>
-      <c r="B43" s="37"/>
-      <c r="C43" s="38" t="s">
+      <c r="A43" s="11"/>
+      <c r="B43" s="28"/>
+      <c r="C43" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="D43" s="36"/>
-      <c r="E43" s="39"/>
-      <c r="F43" s="40"/>
+      <c r="D43" s="11"/>
+      <c r="E43" s="32"/>
+      <c r="F43" s="34"/>
     </row>
     <row r="44" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
+      <c r="A44" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="B44" s="10">
+      <c r="B44" s="26">
         <v>42590</v>
       </c>
-      <c r="C44" s="12" t="s">
+      <c r="C44" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="D44" s="9" t="s">
+      <c r="D44" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="E44" s="11" t="s">
+      <c r="E44" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="F44" s="19" t="s">
+      <c r="F44" s="25" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="25" t="s">
+      <c r="A45" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B45" s="26">
+      <c r="B45" s="16">
         <v>42590</v>
       </c>
-      <c r="C45" s="27" t="s">
+      <c r="C45" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="D45" s="28" t="s">
+      <c r="D45" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="E45" s="27" t="s">
+      <c r="E45" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="F45" s="29" t="s">
+      <c r="F45" s="19" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="36"/>
-      <c r="B46" s="37"/>
-      <c r="C46" s="38" t="s">
+      <c r="A46" s="11"/>
+      <c r="B46" s="28"/>
+      <c r="C46" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="D46" s="36"/>
-      <c r="E46" s="39"/>
-      <c r="F46" s="40"/>
+      <c r="D46" s="11"/>
+      <c r="E46" s="32"/>
+      <c r="F46" s="34"/>
     </row>
     <row r="47" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
+      <c r="A47" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="B47" s="10">
+      <c r="B47" s="26">
         <v>42594</v>
       </c>
-      <c r="C47" s="12" t="s">
+      <c r="C47" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="D47" s="9" t="s">
+      <c r="D47" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="E47" s="11" t="s">
+      <c r="E47" s="24" t="s">
         <v>143</v>
       </c>
-      <c r="F47" s="19" t="s">
+      <c r="F47" s="25" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
+      <c r="A48" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="B48" s="10">
+      <c r="B48" s="26">
         <v>42594</v>
       </c>
-      <c r="C48" s="12" t="s">
+      <c r="C48" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="D48" s="9" t="s">
+      <c r="D48" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="E48" s="11" t="s">
+      <c r="E48" s="24" t="s">
         <v>145</v>
       </c>
-      <c r="F48" s="19" t="s">
+      <c r="F48" s="25" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
+      <c r="A49" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B49" s="10">
+      <c r="B49" s="26">
         <v>42594</v>
       </c>
-      <c r="C49" s="12" t="s">
+      <c r="C49" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="D49" s="9" t="s">
+      <c r="D49" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="E49" s="11" t="s">
+      <c r="E49" s="24" t="s">
         <v>145</v>
       </c>
-      <c r="F49" s="19" t="s">
+      <c r="F49" s="25" t="s">
         <v>146</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="11"/>
+      <c r="B50" s="28"/>
+      <c r="C50" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="D50" s="11"/>
+      <c r="E50" s="32"/>
+      <c r="F50" s="34"/>
+    </row>
+    <row r="51" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="B51" s="26">
+        <v>42597</v>
+      </c>
+      <c r="C51" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="D51" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="E51" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="F51" s="19" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B52" s="26">
+        <v>42597</v>
+      </c>
+      <c r="C52" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="D52" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="E52" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="F52" s="25" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B53" s="26">
+        <v>42597</v>
+      </c>
+      <c r="C53" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="D53" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="E53" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="F53" s="25" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -1962,7 +2026,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.140625" customWidth="1"/>
-    <col min="2" max="2" width="29.7109375" style="18" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" style="10" customWidth="1"/>
     <col min="3" max="3" width="39.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1970,7 +2034,7 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="9" t="s">
         <v>11</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -1981,7 +2045,7 @@
       <c r="A2" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="10" t="s">
         <v>82</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -1992,7 +2056,7 @@
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="10" t="s">
         <v>32</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -2003,7 +2067,7 @@
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="10" t="s">
         <v>27</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -2014,7 +2078,7 @@
       <c r="A5" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="10" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -2025,7 +2089,7 @@
       <c r="A6" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="10" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -2036,7 +2100,7 @@
       <c r="A7" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="10" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -2047,7 +2111,7 @@
       <c r="A8" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="10" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -2058,7 +2122,7 @@
       <c r="A9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="10" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -2069,7 +2133,7 @@
       <c r="A10" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="10" t="s">
         <v>84</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -2080,7 +2144,7 @@
       <c r="A11" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="10" t="s">
         <v>93</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -2091,7 +2155,7 @@
       <c r="A12" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="10" t="s">
         <v>89</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -2102,7 +2166,7 @@
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="10" t="s">
         <v>90</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -2113,7 +2177,7 @@
       <c r="A14" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="10" t="s">
         <v>95</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -2124,7 +2188,7 @@
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="10" t="s">
         <v>87</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -2135,7 +2199,7 @@
       <c r="A16" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="10" t="s">
         <v>54</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -2146,7 +2210,7 @@
       <c r="A17" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="10" t="s">
         <v>13</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -2157,7 +2221,7 @@
       <c r="A18" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="10" t="s">
         <v>50</v>
       </c>
       <c r="C18" s="1" t="s">
@@ -2168,7 +2232,7 @@
       <c r="A19" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="10" t="s">
         <v>91</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -2179,7 +2243,7 @@
       <c r="A20" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="10" t="s">
         <v>86</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -2190,7 +2254,7 @@
       <c r="A21" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="10" t="s">
         <v>92</v>
       </c>
       <c r="C21" s="1" t="s">
@@ -2201,7 +2265,7 @@
       <c r="A22" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="10" t="s">
         <v>83</v>
       </c>
       <c r="C22" s="1" t="s">
@@ -2212,7 +2276,7 @@
       <c r="A23" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B23" s="18" t="s">
+      <c r="B23" s="10" t="s">
         <v>88</v>
       </c>
       <c r="C23" s="1" t="s">
@@ -2223,7 +2287,7 @@
       <c r="A24" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="18" t="s">
+      <c r="B24" s="10" t="s">
         <v>94</v>
       </c>
       <c r="C24" s="1" t="s">
@@ -2234,7 +2298,7 @@
       <c r="A25" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B25" s="18" t="s">
+      <c r="B25" s="10" t="s">
         <v>85</v>
       </c>
       <c r="C25" s="1" t="s">

</xml_diff>

<commit_message>
Minor bug fix that prevents double logging of one event that occurs in the border cases
</commit_message>
<xml_diff>
--- a/CLASSOPS/Derek/Derek's Log.xlsx
+++ b/CLASSOPS/Derek/Derek's Log.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="168">
   <si>
     <t>Staff Name</t>
   </si>
@@ -553,10 +553,22 @@
     <t>014 JCR</t>
   </si>
   <si>
-    <t>Pick up PC and Projector cart. Projector cart has small speaker on it. Pick up portable screen also. Key for room in Founders 164 storeroom. Return equipment to Vanier 040 storeroom.</t>
-  </si>
-  <si>
     <t>Pick up mic, clip, mic cable and mic stand and return to Vanier 040 storeroom.</t>
+  </si>
+  <si>
+    <t>Pick up PC and Projector cart. Projector cart has small speaker on it. Pick up portable screen also. PICK UP 6 MATS. Key for room in Founders 164 storeroom. Return equipment to Vanier 040 storeroom.</t>
+  </si>
+  <si>
+    <t>283B</t>
+  </si>
+  <si>
+    <t>No need to go here. Room is managed by Winters college.</t>
+  </si>
+  <si>
+    <t>117</t>
+  </si>
+  <si>
+    <t>Winters classroom key B15</t>
   </si>
 </sst>
 </file>
@@ -1089,11 +1101,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I72"/>
+  <dimension ref="A1:I76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F75" sqref="F75"/>
+      <pane ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F82" sqref="F82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2360,7 +2372,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" ht="43.15" x14ac:dyDescent="0.3">
       <c r="A71" s="15" t="s">
         <v>89</v>
       </c>
@@ -2377,7 +2389,7 @@
         <v>161</v>
       </c>
       <c r="F71" s="25" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2397,7 +2409,77 @@
         <v>161</v>
       </c>
       <c r="F72" s="25" t="s">
-        <v>163</v>
+        <v>162</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="11"/>
+      <c r="B73" s="28"/>
+      <c r="C73" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="D73" s="11"/>
+      <c r="E73" s="32"/>
+      <c r="F73" s="34"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B74" s="26">
+        <v>42604</v>
+      </c>
+      <c r="C74" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="D74" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="E74" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="F74" s="21" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B75" s="26">
+        <v>42604</v>
+      </c>
+      <c r="C75" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="D75" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="E75" s="24" t="s">
+        <v>166</v>
+      </c>
+      <c r="F75" s="25" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B76" s="26">
+        <v>42604</v>
+      </c>
+      <c r="C76" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="D76" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="E76" s="24" t="s">
+        <v>164</v>
+      </c>
+      <c r="F76" s="25" t="s">
+        <v>165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Files updated and optimization with excel only opening once
</commit_message>
<xml_diff>
--- a/CLASSOPS/Derek/Derek's Log.xlsx
+++ b/CLASSOPS/Derek/Derek's Log.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="90" yWindow="150" windowWidth="14865" windowHeight="10785" tabRatio="440"/>
+    <workbookView xWindow="96" yWindow="156" windowWidth="14868" windowHeight="10788" tabRatio="440"/>
   </bookViews>
   <sheets>
     <sheet name="Logs" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="172">
   <si>
     <t>Staff Name</t>
   </si>
@@ -103,9 +103,6 @@
   </si>
   <si>
     <t>LSB</t>
-  </si>
-  <si>
-    <t>Crestron Logout</t>
   </si>
   <si>
     <t>BSB</t>
@@ -581,6 +578,9 @@
   </si>
   <si>
     <t>Please check room - lock room - key for room in Fdrs 164 storeroom.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Neck mic, desk mic, PC.Turn off audio system etc. Lock booth and Senate doors. N940 keys. </t>
   </si>
 </sst>
 </file>
@@ -1113,22 +1113,22 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I80"/>
+  <dimension ref="A1:I85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F83" sqref="F83"/>
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B85" sqref="B85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="22.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" style="15" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" style="15" customWidth="1"/>
     <col min="2" max="2" width="19" style="26" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" style="22" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="23" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" style="24" customWidth="1"/>
-    <col min="6" max="6" width="60.42578125" style="25" customWidth="1"/>
-    <col min="7" max="16384" width="22.140625" style="3"/>
+    <col min="5" max="5" width="11.6640625" style="24" customWidth="1"/>
+    <col min="6" max="6" width="60.44140625" style="25" customWidth="1"/>
+    <col min="7" max="16384" width="22.109375" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -1136,7 +1136,7 @@
         <v>11</v>
       </c>
       <c r="B1" s="27" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C1" s="30" t="s">
         <v>20</v>
@@ -1148,14 +1148,14 @@
         <v>18</v>
       </c>
       <c r="F1" s="33" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="15" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D2" s="13"/>
       <c r="E2" s="11"/>
@@ -1164,7 +1164,7 @@
       <c r="H2" s="11"/>
       <c r="I2" s="11"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>16</v>
       </c>
@@ -1172,63 +1172,63 @@
         <v>42570</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D3" s="23" t="s">
         <v>22</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F3" s="25" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B4" s="26">
         <v>42570</v>
       </c>
       <c r="C4" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="D4" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="E4" s="24" t="s">
-        <v>109</v>
-      </c>
       <c r="F4" s="25" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B5" s="26">
         <v>42570</v>
       </c>
       <c r="C5" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="D5" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="E5" s="24" t="s">
-        <v>111</v>
-      </c>
       <c r="F5" s="25" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="15" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D6" s="13"/>
       <c r="E6" s="11"/>
@@ -1237,7 +1237,7 @@
       <c r="H6" s="11"/>
       <c r="I6" s="11"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>19</v>
       </c>
@@ -1245,19 +1245,19 @@
         <v>42571</v>
       </c>
       <c r="C7" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="D7" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>114</v>
-      </c>
       <c r="F7" s="19" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>19</v>
       </c>
@@ -1265,23 +1265,23 @@
         <v>42571</v>
       </c>
       <c r="C8" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="D8" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>111</v>
-      </c>
       <c r="F8" s="25" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="15" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D9" s="13"/>
       <c r="E9" s="11"/>
@@ -1290,127 +1290,127 @@
       <c r="H9" s="11"/>
       <c r="I9" s="11"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B10" s="16">
         <v>42573</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E10" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B11" s="16">
         <v>42573</v>
       </c>
       <c r="C11" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="D11" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="E11" s="24" t="s">
-        <v>111</v>
-      </c>
       <c r="F11" s="25" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B12" s="16">
         <v>42573</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E12" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="F12" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="F12" s="25" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B13" s="16">
         <v>42573</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E13" s="24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F13" s="25" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B14" s="16">
         <v>42573</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E14" s="24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F14" s="25" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B15" s="16">
         <v>42573</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E15" s="24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F15" s="25" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
         <v>19</v>
       </c>
@@ -1418,23 +1418,23 @@
         <v>42573</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D16" s="23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E16" s="24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F16" s="25" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="15" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="11"/>
       <c r="B17" s="11"/>
       <c r="C17" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D17" s="13"/>
       <c r="E17" s="11"/>
@@ -1443,7 +1443,7 @@
       <c r="H17" s="11"/>
       <c r="I17" s="11"/>
     </row>
-    <row r="18" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" s="15" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
         <v>19</v>
       </c>
@@ -1451,19 +1451,19 @@
         <v>42576</v>
       </c>
       <c r="C18" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="D18" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="E18" s="17" t="s">
-        <v>114</v>
-      </c>
       <c r="F18" s="19" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
         <v>19</v>
       </c>
@@ -1471,19 +1471,19 @@
         <v>42576</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E19" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="F19" s="21" t="s">
         <v>130</v>
       </c>
-      <c r="F19" s="21" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
         <v>19</v>
       </c>
@@ -1491,23 +1491,23 @@
         <v>42576</v>
       </c>
       <c r="C20" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" s="20" t="s">
         <v>132</v>
       </c>
-      <c r="D20" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="E20" s="20" t="s">
+      <c r="F20" s="25" t="s">
         <v>133</v>
       </c>
-      <c r="F20" s="25" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:9" s="15" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="11"/>
       <c r="B21" s="11"/>
       <c r="C21" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D21" s="13"/>
       <c r="E21" s="11"/>
@@ -1516,7 +1516,7 @@
       <c r="H21" s="11"/>
       <c r="I21" s="11"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
         <v>16</v>
       </c>
@@ -1524,43 +1524,43 @@
         <v>42577</v>
       </c>
       <c r="C22" s="22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D22" s="23" t="s">
         <v>22</v>
       </c>
       <c r="E22" s="24" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F22" s="25" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B23" s="26">
         <v>42577</v>
       </c>
       <c r="C23" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="D23" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="E23" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="D23" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="E23" s="24" t="s">
-        <v>109</v>
-      </c>
       <c r="F23" s="25" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" s="15" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="11"/>
       <c r="B24" s="11"/>
       <c r="C24" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D24" s="13"/>
       <c r="E24" s="11"/>
@@ -1569,7 +1569,7 @@
       <c r="H24" s="11"/>
       <c r="I24" s="11"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
         <v>19</v>
       </c>
@@ -1577,39 +1577,39 @@
         <v>42578</v>
       </c>
       <c r="C25" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="E25" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="D25" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="E25" s="17" t="s">
-        <v>114</v>
-      </c>
       <c r="F25" s="19" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B26" s="16">
         <v>42578</v>
       </c>
       <c r="C26" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="E26" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="D26" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="E26" s="15" t="s">
-        <v>111</v>
-      </c>
       <c r="F26" s="25" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
         <v>19</v>
       </c>
@@ -1617,23 +1617,23 @@
         <v>42578</v>
       </c>
       <c r="C27" s="22" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E27" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="F27" s="21" t="s">
         <v>130</v>
       </c>
-      <c r="F27" s="21" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:9" s="15" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="11"/>
       <c r="B28" s="11"/>
       <c r="C28" s="12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D28" s="13"/>
       <c r="E28" s="11"/>
@@ -1642,7 +1642,7 @@
       <c r="H28" s="11"/>
       <c r="I28" s="11"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
         <v>19</v>
       </c>
@@ -1650,19 +1650,19 @@
         <v>42579</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E29" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="F29" s="21" t="s">
         <v>130</v>
       </c>
-      <c r="F29" s="21" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
         <v>19</v>
       </c>
@@ -1670,43 +1670,43 @@
         <v>42579</v>
       </c>
       <c r="C30" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="E30" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="D30" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="E30" s="24" t="s">
+      <c r="F30" s="25" t="s">
         <v>137</v>
       </c>
-      <c r="F30" s="25" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B31" s="16">
         <v>42579</v>
       </c>
       <c r="C31" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="D31" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="E31" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="D31" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="E31" s="24" t="s">
-        <v>109</v>
-      </c>
       <c r="F31" s="25" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="11"/>
       <c r="B32" s="11"/>
       <c r="C32" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D32" s="13"/>
       <c r="E32" s="11"/>
@@ -1715,24 +1715,24 @@
       <c r="H32" s="11"/>
       <c r="I32" s="11"/>
     </row>
-    <row r="33" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" s="15" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B33" s="16">
         <v>42580</v>
       </c>
       <c r="C33" s="22" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D33" s="23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E33" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F33" s="19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
@@ -1740,38 +1740,38 @@
     </row>
     <row r="34" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B34" s="16">
         <v>42580</v>
       </c>
       <c r="C34" s="22" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D34" s="23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E34" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="F34" s="25" t="s">
         <v>139</v>
-      </c>
-      <c r="F34" s="25" t="s">
-        <v>140</v>
       </c>
       <c r="G34" s="15"/>
       <c r="H34" s="15"/>
       <c r="I34" s="15"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="11"/>
       <c r="B35" s="11"/>
       <c r="C35" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D35" s="13"/>
       <c r="E35" s="11"/>
       <c r="F35" s="13"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="15" t="s">
         <v>16</v>
       </c>
@@ -1779,49 +1779,49 @@
         <v>42584</v>
       </c>
       <c r="C36" s="22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D36" s="23" t="s">
         <v>22</v>
       </c>
       <c r="E36" s="24" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F36" s="25" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B37" s="26">
         <v>42584</v>
       </c>
       <c r="C37" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="D37" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="E37" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="D37" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="E37" s="24" t="s">
-        <v>109</v>
-      </c>
       <c r="F37" s="25" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="11"/>
       <c r="B38" s="11"/>
       <c r="C38" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D38" s="13"/>
       <c r="E38" s="11"/>
       <c r="F38" s="13"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="15" t="s">
         <v>19</v>
       </c>
@@ -1829,43 +1829,43 @@
         <v>42585</v>
       </c>
       <c r="C39" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="D39" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="E39" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="D39" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="E39" s="17" t="s">
-        <v>114</v>
-      </c>
       <c r="F39" s="19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B40" s="16">
         <v>42585</v>
       </c>
       <c r="C40" s="22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D40" s="23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E40" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F40" s="19" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="11"/>
       <c r="B41" s="28"/>
       <c r="C41" s="13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D41" s="11"/>
       <c r="E41" s="32"/>
@@ -1873,29 +1873,29 @@
     </row>
     <row r="42" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B42" s="16">
         <v>42587</v>
       </c>
       <c r="C42" s="22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D42" s="23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E42" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F42" s="19" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="11"/>
       <c r="B43" s="28"/>
       <c r="C43" s="13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D43" s="11"/>
       <c r="E43" s="32"/>
@@ -1903,25 +1903,25 @@
     </row>
     <row r="44" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B44" s="26">
         <v>42590</v>
       </c>
       <c r="C44" s="22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D44" s="23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E44" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F44" s="25" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="15" t="s">
         <v>19</v>
       </c>
@@ -1929,23 +1929,23 @@
         <v>42590</v>
       </c>
       <c r="C45" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="D45" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="E45" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="D45" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="E45" s="17" t="s">
-        <v>114</v>
-      </c>
       <c r="F45" s="19" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="11"/>
       <c r="B46" s="28"/>
       <c r="C46" s="13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D46" s="11"/>
       <c r="E46" s="32"/>
@@ -1953,42 +1953,42 @@
     </row>
     <row r="47" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B47" s="26">
         <v>42594</v>
       </c>
       <c r="C47" s="22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D47" s="23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E47" s="24" t="s">
+        <v>142</v>
+      </c>
+      <c r="F47" s="25" t="s">
         <v>143</v>
-      </c>
-      <c r="F47" s="25" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B48" s="26">
         <v>42594</v>
       </c>
       <c r="C48" s="22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D48" s="23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E48" s="24" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F48" s="25" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1999,23 +1999,23 @@
         <v>42594</v>
       </c>
       <c r="C49" s="22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D49" s="23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E49" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="F49" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="F49" s="25" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="11"/>
       <c r="B50" s="28"/>
       <c r="C50" s="13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D50" s="11"/>
       <c r="E50" s="32"/>
@@ -2023,25 +2023,25 @@
     </row>
     <row r="51" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B51" s="26">
         <v>42597</v>
       </c>
       <c r="C51" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="D51" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="E51" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="D51" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="E51" s="17" t="s">
-        <v>148</v>
-      </c>
       <c r="F51" s="19" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="15" t="s">
         <v>19</v>
       </c>
@@ -2049,19 +2049,19 @@
         <v>42597</v>
       </c>
       <c r="C52" s="22" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D52" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E52" s="24" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F52" s="25" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="15" t="s">
         <v>19</v>
       </c>
@@ -2069,49 +2069,49 @@
         <v>42597</v>
       </c>
       <c r="C53" s="22" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D53" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E53" s="24" t="s">
+        <v>136</v>
+      </c>
+      <c r="F53" s="25" t="s">
         <v>137</v>
       </c>
-      <c r="F53" s="25" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="11"/>
       <c r="B54" s="11"/>
       <c r="C54" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D54" s="13"/>
       <c r="E54" s="11"/>
       <c r="F54" s="13"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B55" s="26">
         <v>42598</v>
       </c>
       <c r="C55" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="D55" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="E55" s="24" t="s">
         <v>151</v>
       </c>
-      <c r="D55" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="E55" s="24" t="s">
+      <c r="F55" s="25" t="s">
         <v>152</v>
       </c>
-      <c r="F55" s="25" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="15" t="s">
         <v>19</v>
       </c>
@@ -2119,19 +2119,19 @@
         <v>42598</v>
       </c>
       <c r="C56" s="22" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D56" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E56" s="24" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F56" s="25" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="15" t="s">
         <v>19</v>
       </c>
@@ -2139,89 +2139,89 @@
         <v>42598</v>
       </c>
       <c r="C57" s="22" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D57" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E57" s="24" t="s">
+        <v>136</v>
+      </c>
+      <c r="F57" s="25" t="s">
         <v>137</v>
       </c>
-      <c r="F57" s="25" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="11"/>
       <c r="B58" s="11"/>
       <c r="C58" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D58" s="13"/>
       <c r="E58" s="11"/>
       <c r="F58" s="13"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B59" s="16">
         <v>42599</v>
       </c>
       <c r="C59" s="17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D59" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E59" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="F59" s="19" t="s">
         <v>155</v>
-      </c>
-      <c r="F59" s="19" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B60" s="16">
         <v>42599</v>
       </c>
       <c r="C60" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="D60" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="E60" s="24" t="s">
         <v>151</v>
       </c>
-      <c r="D60" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="E60" s="24" t="s">
-        <v>152</v>
-      </c>
       <c r="F60" s="25" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B61" s="16">
         <v>42599</v>
       </c>
       <c r="C61" s="22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D61" s="23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E61" s="24" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F61" s="19" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="15" t="s">
         <v>19</v>
       </c>
@@ -2229,19 +2229,19 @@
         <v>42599</v>
       </c>
       <c r="C62" s="22" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D62" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E62" s="24" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F62" s="25" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" s="15" t="s">
         <v>19</v>
       </c>
@@ -2249,23 +2249,23 @@
         <v>42599</v>
       </c>
       <c r="C63" s="22" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D63" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E63" s="24" t="s">
+        <v>136</v>
+      </c>
+      <c r="F63" s="25" t="s">
         <v>137</v>
       </c>
-      <c r="F63" s="25" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:9" s="15" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" s="11"/>
       <c r="B64" s="11"/>
       <c r="C64" s="12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D64" s="13"/>
       <c r="E64" s="11"/>
@@ -2274,47 +2274,47 @@
       <c r="H64" s="11"/>
       <c r="I64" s="11"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B65" s="16">
         <v>42600</v>
       </c>
       <c r="C65" s="22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D65" s="23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E65" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F65" s="25" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A66" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B66" s="16">
         <v>42600</v>
       </c>
       <c r="C66" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="D66" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="E66" s="24" t="s">
         <v>151</v>
       </c>
-      <c r="D66" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="E66" s="24" t="s">
-        <v>152</v>
-      </c>
       <c r="F66" s="25" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A67" s="15" t="s">
         <v>19</v>
       </c>
@@ -2322,19 +2322,19 @@
         <v>42600</v>
       </c>
       <c r="C67" s="22" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D67" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E67" s="24" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F67" s="25" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" s="15" t="s">
         <v>19</v>
       </c>
@@ -2342,23 +2342,23 @@
         <v>42600</v>
       </c>
       <c r="C68" s="22" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D68" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E68" s="24" t="s">
+        <v>136</v>
+      </c>
+      <c r="F68" s="25" t="s">
         <v>137</v>
       </c>
-      <c r="F68" s="25" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="11"/>
       <c r="B69" s="28"/>
       <c r="C69" s="13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D69" s="11"/>
       <c r="E69" s="32"/>
@@ -2366,75 +2366,75 @@
     </row>
     <row r="70" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B70" s="16">
         <v>42601</v>
       </c>
       <c r="C70" s="22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D70" s="23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E70" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F70" s="25" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" ht="43.15" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A71" s="15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B71" s="26">
         <v>42601</v>
       </c>
       <c r="C71" s="22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D71" s="23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E71" s="24" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F71" s="25" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B72" s="26">
         <v>42601</v>
       </c>
       <c r="C72" s="22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D72" s="23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E72" s="24" t="s">
+        <v>160</v>
+      </c>
+      <c r="F72" s="25" t="s">
         <v>161</v>
       </c>
-      <c r="F72" s="25" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="73" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A73" s="11"/>
       <c r="B73" s="28"/>
       <c r="C73" s="13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D73" s="11"/>
       <c r="E73" s="32"/>
       <c r="F73" s="34"/>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A74" s="15" t="s">
         <v>19</v>
       </c>
@@ -2442,19 +2442,19 @@
         <v>42604</v>
       </c>
       <c r="C74" s="22" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D74" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E74" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="F74" s="21" t="s">
         <v>130</v>
       </c>
-      <c r="F74" s="21" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A75" s="15" t="s">
         <v>19</v>
       </c>
@@ -2462,19 +2462,19 @@
         <v>42604</v>
       </c>
       <c r="C75" s="22" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D75" s="23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E75" s="24" t="s">
+        <v>165</v>
+      </c>
+      <c r="F75" s="25" t="s">
         <v>166</v>
       </c>
-      <c r="F75" s="25" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A76" s="15" t="s">
         <v>19</v>
       </c>
@@ -2482,23 +2482,23 @@
         <v>42604</v>
       </c>
       <c r="C76" s="22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D76" s="23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E76" s="24" t="s">
+        <v>163</v>
+      </c>
+      <c r="F76" s="25" t="s">
         <v>164</v>
       </c>
-      <c r="F76" s="25" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A77" s="11"/>
       <c r="B77" s="28"/>
       <c r="C77" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D77" s="11"/>
       <c r="E77" s="32"/>
@@ -2506,25 +2506,25 @@
     </row>
     <row r="78" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B78" s="26">
         <v>42605</v>
       </c>
       <c r="C78" s="22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D78" s="23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E78" s="24" t="s">
+        <v>167</v>
+      </c>
+      <c r="F78" s="25" t="s">
         <v>168</v>
       </c>
-      <c r="F78" s="25" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A79" s="15" t="s">
         <v>19</v>
       </c>
@@ -2532,16 +2532,16 @@
         <v>42605</v>
       </c>
       <c r="C79" s="22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D79" s="23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E79" s="24" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F79" s="25" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="80" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2552,16 +2552,106 @@
         <v>42605</v>
       </c>
       <c r="C80" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="D80" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="E80" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="F80" s="25" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A81" s="11"/>
+      <c r="B81" s="11"/>
+      <c r="C81" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D81" s="13"/>
+      <c r="E81" s="11"/>
+      <c r="F81" s="13"/>
+    </row>
+    <row r="82" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A82" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="B82" s="16">
+        <v>42606</v>
+      </c>
+      <c r="C82" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="D82" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="E82" s="24" t="s">
+        <v>151</v>
+      </c>
+      <c r="F82" s="25" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A83" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B83" s="16">
+        <v>42606</v>
+      </c>
+      <c r="C83" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="D83" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="E83" s="24" t="s">
+        <v>148</v>
+      </c>
+      <c r="F83" s="25" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A84" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B84" s="16">
+        <v>42606</v>
+      </c>
+      <c r="C84" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="D84" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="E84" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="D80" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="E80" s="24" t="s">
-        <v>145</v>
-      </c>
-      <c r="F80" s="25" t="s">
-        <v>171</v>
+      <c r="F84" s="25" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A85" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B85" s="16">
+        <v>42606</v>
+      </c>
+      <c r="C85" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="D85" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="E85" s="24" t="s">
+        <v>163</v>
+      </c>
+      <c r="F85" s="25" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -2571,13 +2661,13 @@
     <sortCondition ref="D427:D515"/>
   </sortState>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A22:A23 B6 B2 A7:A8 B9 A10:A16 B17 A18:A20 B21 A3:A5 B24 A25:A27 B28 B32 A29:A31 A33:A34 B35 A36:A37 B38 A39:A53 B54 A55:A57 B58 A59:A63 B64 A65:A1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A22:A23 B6 B2 A7:A8 B9 A10:A16 B17 A18:A20 B21 A3:A5 B24 A25:A27 B28 B32 A29:A31 A33:A34 B35 A36:A37 B38 A39:A53 B54 A55:A57 B58 A59:A63 B64 A65:A80 B81 A82:A1048576">
       <formula1>Task_type</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6 E2 D22:D23 D7:D8 E9 D10:D16 E17 D18:D20 E21 D3:D5 E24 D25:D27 E28 E32 D29:D31 D33:D34 E35 D36:D37 E38 D39:D53 E54 D55:D57 E58 D59:D63 E64 D65:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6 E2 D22:D23 D7:D8 E9 D10:D16 E17 D18:D20 E21 D3:D5 E24 D25:D27 E28 E32 D29:D31 D33:D34 E35 D36:D37 E38 D39:D53 E54 D55:D57 E58 D59:D63 E64 D65:D80 E81 D82:D1048576">
       <formula1>Building</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 A2 A9 A17 A21 A24 A28 A32 A35 A38 A54 A58 A64">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 A2 A9 A17 A21 A24 A28 A32 A35 A38 A54 A58 A64 A81">
       <formula1>Staff_Name</formula1>
     </dataValidation>
   </dataValidations>
@@ -2593,18 +2683,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C40" sqref="C2:C40"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A38" sqref="A2:A38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.140625" customWidth="1"/>
-    <col min="2" max="2" width="29.7109375" style="10" customWidth="1"/>
-    <col min="3" max="3" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.109375" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="39.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2615,117 +2705,117 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="B8" s="10" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>3</v>
       </c>
@@ -2733,217 +2823,214 @@
         <v>89</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>87</v>
+        <v>53</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>54</v>
+        <v>13</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="B19" s="10" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+    <row r="24" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C27" s="1" t="s">
+      <c r="C29" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C33" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>9</v>
       </c>
@@ -2951,95 +3038,95 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C35" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C36" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C36" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C37" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C37" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="C38" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
       <c r="C39" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
       <c r="C40" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="4"/>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="5"/>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" s="5"/>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" s="5"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" s="5"/>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" s="5"/>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" s="5"/>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" s="6"/>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" s="7"/>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" s="8"/>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57" s="8"/>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" s="8"/>
     </row>
   </sheetData>
-  <sortState ref="C2:C40">
-    <sortCondition ref="C40"/>
+  <sortState ref="A2:A38">
+    <sortCondition ref="A38"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Email login window complete
</commit_message>
<xml_diff>
--- a/CLASSOPS/Derek/Derek's Log.xlsx
+++ b/CLASSOPS/Derek/Derek's Log.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="179">
   <si>
     <t>Staff Name</t>
   </si>
@@ -581,6 +581,27 @@
   </si>
   <si>
     <t xml:space="preserve">Neck mic, desk mic, PC.Turn off audio system etc. Lock booth and Senate doors. N940 keys. </t>
+  </si>
+  <si>
+    <t>Pick up PC and Projector cart and large portable screen also. PICK UP MATS. Return equipment to Vanier 040 storeroom.</t>
+  </si>
+  <si>
+    <t>Lectern mic, stand and cables with large PA system. To Vanier 040.</t>
+  </si>
+  <si>
+    <t>1800</t>
+  </si>
+  <si>
+    <t>001-JCR</t>
+  </si>
+  <si>
+    <t>Lectern mic with small PA etc. Return to Vanier 040.</t>
+  </si>
+  <si>
+    <t>May include portable screen. All to Vanier 040.</t>
+  </si>
+  <si>
+    <t>001-DH</t>
   </si>
 </sst>
 </file>
@@ -1113,11 +1134,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I87"/>
+  <dimension ref="A1:I93"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B87" sqref="B87"/>
+      <pane ySplit="1" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E102" sqref="E101:E102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2684,6 +2705,116 @@
         <v>163</v>
       </c>
       <c r="F87" s="25" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A88" s="11"/>
+      <c r="B88" s="28"/>
+      <c r="C88" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="D88" s="11"/>
+      <c r="E88" s="32"/>
+      <c r="F88" s="34"/>
+    </row>
+    <row r="89" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A89" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="B89" s="26">
+        <v>42608</v>
+      </c>
+      <c r="C89" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="D89" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="E89" s="24" t="s">
+        <v>178</v>
+      </c>
+      <c r="F89" s="25" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="B90" s="26">
+        <v>42608</v>
+      </c>
+      <c r="C90" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="D90" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="E90" s="24" t="s">
+        <v>178</v>
+      </c>
+      <c r="F90" s="25" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="B91" s="26">
+        <v>42608</v>
+      </c>
+      <c r="C91" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="D91" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="E91" s="24" t="s">
+        <v>175</v>
+      </c>
+      <c r="F91" s="25" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A92" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="B92" s="26">
+        <v>42608</v>
+      </c>
+      <c r="C92" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="D92" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="E92" s="24" t="s">
+        <v>175</v>
+      </c>
+      <c r="F92" s="25" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A93" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B93" s="26">
+        <v>42608</v>
+      </c>
+      <c r="C93" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="D93" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="E93" s="24" t="s">
+        <v>163</v>
+      </c>
+      <c r="F93" s="25" t="s">
         <v>164</v>
       </c>
     </row>

</xml_diff>

<commit_message>
TEL has been changed to DB
</commit_message>
<xml_diff>
--- a/CLASSOPS/Derek/Derek's Log.xlsx
+++ b/CLASSOPS/Derek/Derek's Log.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="184">
   <si>
     <t>Staff Name</t>
   </si>
@@ -602,6 +602,21 @@
   </si>
   <si>
     <t>001-DH</t>
+  </si>
+  <si>
+    <t>113</t>
+  </si>
+  <si>
+    <t>Flat screen DLP and wireless keyboard. To Vanier 132 storeroom.</t>
+  </si>
+  <si>
+    <t>010-SCR</t>
+  </si>
+  <si>
+    <t>Leave portable screen and network cable, but get carpets. To  Vanier 040 storeroom.</t>
+  </si>
+  <si>
+    <t>305-SCR</t>
   </si>
 </sst>
 </file>
@@ -1134,11 +1149,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I93"/>
+  <dimension ref="A1:I97"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E102" sqref="E101:E102"/>
+      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A102" sqref="A102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2816,6 +2831,76 @@
       </c>
       <c r="F93" s="25" t="s">
         <v>164</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A94" s="11"/>
+      <c r="B94" s="28"/>
+      <c r="C94" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="D94" s="11"/>
+      <c r="E94" s="32"/>
+      <c r="F94" s="34"/>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A95" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="B95" s="26">
+        <v>42611</v>
+      </c>
+      <c r="C95" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="D95" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="E95" s="24" t="s">
+        <v>183</v>
+      </c>
+      <c r="F95" s="25" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A96" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="B96" s="26">
+        <v>42611</v>
+      </c>
+      <c r="C96" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="D96" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="E96" s="24" t="s">
+        <v>179</v>
+      </c>
+      <c r="F96" s="25" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A97" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="B97" s="26">
+        <v>42611</v>
+      </c>
+      <c r="C97" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="D97" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="E97" s="24" t="s">
+        <v>181</v>
+      </c>
+      <c r="F97" s="25" t="s">
+        <v>182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Printing working as intended now
</commit_message>
<xml_diff>
--- a/CLASSOPS/Derek/Derek's Log.xlsx
+++ b/CLASSOPS/Derek/Derek's Log.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="193">
   <si>
     <t>Staff Name</t>
   </si>
@@ -617,6 +617,33 @@
   </si>
   <si>
     <t>305-SCR</t>
+  </si>
+  <si>
+    <t>157B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Door code 11012* </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Door code 10077* </t>
+  </si>
+  <si>
+    <t>1745</t>
+  </si>
+  <si>
+    <t>1645</t>
+  </si>
+  <si>
+    <t>140-SCR</t>
+  </si>
+  <si>
+    <t>2130</t>
+  </si>
+  <si>
+    <t>Door code 7083*  Leave portable screen. Return to Founders 156A.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Portable screen is there. Door code 7083* </t>
   </si>
 </sst>
 </file>
@@ -1149,11 +1176,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I97"/>
+  <dimension ref="A1:I104"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A102" sqref="A102"/>
+      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C107" sqref="C107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2903,6 +2930,136 @@
         <v>182</v>
       </c>
     </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98" s="11"/>
+      <c r="B98" s="28"/>
+      <c r="C98" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="D98" s="11"/>
+      <c r="E98" s="32"/>
+      <c r="F98" s="34"/>
+    </row>
+    <row r="99" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A99" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B99" s="26">
+        <v>42613</v>
+      </c>
+      <c r="C99" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="D99" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="E99" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="F99" s="19" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B100" s="26">
+        <v>42613</v>
+      </c>
+      <c r="C100" s="22" t="s">
+        <v>188</v>
+      </c>
+      <c r="D100" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="E100" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="F100" s="25" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A101" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B101" s="26">
+        <v>42613</v>
+      </c>
+      <c r="C101" s="22" t="s">
+        <v>188</v>
+      </c>
+      <c r="D101" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="E101" s="24" t="s">
+        <v>184</v>
+      </c>
+      <c r="F101" s="25" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="B102" s="26">
+        <v>42613</v>
+      </c>
+      <c r="C102" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="D102" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="E102" s="24" t="s">
+        <v>179</v>
+      </c>
+      <c r="F102" s="25" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="B103" s="26">
+        <v>42613</v>
+      </c>
+      <c r="C103" s="22" t="s">
+        <v>187</v>
+      </c>
+      <c r="D103" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="E103" s="24" t="s">
+        <v>189</v>
+      </c>
+      <c r="F103" s="25" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="B104" s="26">
+        <v>42613</v>
+      </c>
+      <c r="C104" s="22" t="s">
+        <v>190</v>
+      </c>
+      <c r="D104" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="E104" s="24" t="s">
+        <v>189</v>
+      </c>
+      <c r="F104" s="25" t="s">
+        <v>191</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0"/>
   <sortState ref="A427:G515">
@@ -2910,10 +3067,10 @@
     <sortCondition ref="D427:D515"/>
   </sortState>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A22:A23 B6 B2 A7:A8 B9 A10:A16 B17 A18:A20 B21 A3:A5 B24 A25:A27 B28 B32 A29:A31 A33:A34 B35 A36:A37 B38 A39:A53 B54 A55:A57 B58 A59:A63 B64 A65:A80 B81 A82:A85 B86 A87:A1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A22:A23 B6 B2 A7:A8 B9 A10:A16 B17 A18:A20 B21 A3:A5 B24 A25:A27 B28 B32 A29:A31 A33:A34 B35 A36:A37 B38 A39:A53 B54 A55:A57 B58 A59:A63 B64 A65:A80 B81 A82:A85 B86 A87:A103 A104:A1048576">
       <formula1>Task_type</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6 E2 D22:D23 D7:D8 E9 D10:D16 E17 D18:D20 E21 D3:D5 E24 D25:D27 E28 E32 D29:D31 D33:D34 E35 D36:D37 E38 D39:D53 E54 D55:D57 E58 D59:D63 E64 D65:D80 E81 D82:D85 E86 D87:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6 E2 D22:D23 D7:D8 E9 D10:D16 E17 D18:D20 E21 D3:D5 E24 D25:D27 E28 E32 D29:D31 D33:D34 E35 D36:D37 E38 D39:D53 E54 D55:D57 E58 D59:D63 E64 D65:D80 E81 D82:D85 E86 D87:D103 D104:D1048576">
       <formula1>Building</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 A2 A9 A17 A21 A24 A28 A32 A35 A38 A54 A58 A64 A81 A86">

</xml_diff>

<commit_message>
Minor bug fixes and file updates
</commit_message>
<xml_diff>
--- a/CLASSOPS/Derek/Derek's Log.xlsx
+++ b/CLASSOPS/Derek/Derek's Log.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="193">
   <si>
     <t>Staff Name</t>
   </si>
@@ -1176,11 +1176,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I104"/>
+  <dimension ref="A1:I109"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C107" sqref="C107"/>
+      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A109" sqref="A109:XFD109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2945,7 +2945,7 @@
         <v>92</v>
       </c>
       <c r="B99" s="26">
-        <v>42613</v>
+        <v>42612</v>
       </c>
       <c r="C99" s="22" t="s">
         <v>135</v>
@@ -2962,10 +2962,10 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="15" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B100" s="26">
-        <v>42613</v>
+        <v>42612</v>
       </c>
       <c r="C100" s="22" t="s">
         <v>188</v>
@@ -2982,10 +2982,10 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="15" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B101" s="26">
-        <v>42613</v>
+        <v>42612</v>
       </c>
       <c r="C101" s="22" t="s">
         <v>188</v>
@@ -3005,7 +3005,7 @@
         <v>88</v>
       </c>
       <c r="B102" s="26">
-        <v>42613</v>
+        <v>42612</v>
       </c>
       <c r="C102" s="22" t="s">
         <v>131</v>
@@ -3025,7 +3025,7 @@
         <v>82</v>
       </c>
       <c r="B103" s="26">
-        <v>42613</v>
+        <v>42612</v>
       </c>
       <c r="C103" s="22" t="s">
         <v>187</v>
@@ -3045,7 +3045,7 @@
         <v>88</v>
       </c>
       <c r="B104" s="26">
-        <v>42613</v>
+        <v>42612</v>
       </c>
       <c r="C104" s="22" t="s">
         <v>190</v>
@@ -3058,6 +3058,96 @@
       </c>
       <c r="F104" s="25" t="s">
         <v>191</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105" s="11"/>
+      <c r="B105" s="11"/>
+      <c r="C105" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D105" s="13"/>
+      <c r="E105" s="11"/>
+      <c r="F105" s="13"/>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A106" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B106" s="16">
+        <v>42613</v>
+      </c>
+      <c r="C106" s="22" t="s">
+        <v>188</v>
+      </c>
+      <c r="D106" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="E106" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="F106" s="25" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A107" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B107" s="16">
+        <v>42613</v>
+      </c>
+      <c r="C107" s="22" t="s">
+        <v>188</v>
+      </c>
+      <c r="D107" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="E107" s="24" t="s">
+        <v>184</v>
+      </c>
+      <c r="F107" s="25" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="B108" s="16">
+        <v>42613</v>
+      </c>
+      <c r="C108" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="D108" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="E108" s="24" t="s">
+        <v>175</v>
+      </c>
+      <c r="F108" s="25" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A109" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="B109" s="16">
+        <v>42613</v>
+      </c>
+      <c r="C109" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="D109" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="E109" s="24" t="s">
+        <v>175</v>
+      </c>
+      <c r="F109" s="25" t="s">
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -3067,13 +3157,13 @@
     <sortCondition ref="D427:D515"/>
   </sortState>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A22:A23 B6 B2 A7:A8 B9 A10:A16 B17 A18:A20 B21 A3:A5 B24 A25:A27 B28 B32 A29:A31 A33:A34 B35 A36:A37 B38 A39:A53 B54 A55:A57 B58 A59:A63 B64 A65:A80 B81 A82:A85 B86 A87:A103 A104:A1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A22:A23 B6 B2 A7:A8 B9 A10:A16 B17 A18:A20 B21 A3:A5 B24 A25:A27 B28 B32 A29:A31 A33:A34 B35 A36:A37 B38 A39:A53 B54 A55:A57 B58 A59:A63 B64 A65:A80 B81 A82:A85 B86 A87:A104 B105 A106:A1048576">
       <formula1>Task_type</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6 E2 D22:D23 D7:D8 E9 D10:D16 E17 D18:D20 E21 D3:D5 E24 D25:D27 E28 E32 D29:D31 D33:D34 E35 D36:D37 E38 D39:D53 E54 D55:D57 E58 D59:D63 E64 D65:D80 E81 D82:D85 E86 D87:D103 D104:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6 E2 D22:D23 D7:D8 E9 D10:D16 E17 D18:D20 E21 D3:D5 E24 D25:D27 E28 E32 D29:D31 D33:D34 E35 D36:D37 E38 D39:D53 E54 D55:D57 E58 D59:D63 E64 D65:D80 E81 D82:D85 E86 D87:D104 E105 D106:D1048576">
       <formula1>Building</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 A2 A9 A17 A21 A24 A28 A32 A35 A38 A54 A58 A64 A81 A86">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 A2 A9 A17 A21 A24 A28 A32 A35 A38 A54 A58 A64 A81 A86 A105">
       <formula1>Staff_Name</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
MInor bugfixes and file updates
</commit_message>
<xml_diff>
--- a/CLASSOPS/Derek/Derek's Log.xlsx
+++ b/CLASSOPS/Derek/Derek's Log.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="193">
   <si>
     <t>Staff Name</t>
   </si>
@@ -1176,11 +1176,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I109"/>
+  <dimension ref="A1:I111"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A109" sqref="A109:XFD109"/>
+      <pane ySplit="1" topLeftCell="A94" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A111" sqref="A111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2910,7 +2910,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="97" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A97" s="15" t="s">
         <v>88</v>
       </c>
@@ -2930,7 +2930,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="11"/>
       <c r="B98" s="28"/>
       <c r="C98" s="13" t="s">
@@ -2940,7 +2940,7 @@
       <c r="E98" s="32"/>
       <c r="F98" s="34"/>
     </row>
-    <row r="99" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A99" s="15" t="s">
         <v>92</v>
       </c>
@@ -2960,7 +2960,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="15" t="s">
         <v>12</v>
       </c>
@@ -2980,7 +2980,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="15" t="s">
         <v>12</v>
       </c>
@@ -3000,7 +3000,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="15" t="s">
         <v>88</v>
       </c>
@@ -3020,7 +3020,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="15" t="s">
         <v>82</v>
       </c>
@@ -3040,7 +3040,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="104" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="15" t="s">
         <v>88</v>
       </c>
@@ -3060,7 +3060,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="11"/>
       <c r="B105" s="11"/>
       <c r="C105" s="12" t="s">
@@ -3070,7 +3070,7 @@
       <c r="E105" s="11"/>
       <c r="F105" s="13"/>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="15" t="s">
         <v>12</v>
       </c>
@@ -3090,7 +3090,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="15" t="s">
         <v>12</v>
       </c>
@@ -3110,7 +3110,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="108" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="15" t="s">
         <v>88</v>
       </c>
@@ -3130,7 +3130,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="15" t="s">
         <v>86</v>
       </c>
@@ -3148,6 +3148,39 @@
       </c>
       <c r="F109" s="25" t="s">
         <v>176</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="11"/>
+      <c r="B110" s="11"/>
+      <c r="C110" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="D110" s="13"/>
+      <c r="E110" s="11"/>
+      <c r="F110" s="13"/>
+      <c r="G110" s="14"/>
+      <c r="H110" s="11"/>
+      <c r="I110" s="11"/>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A111" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B111" s="26">
+        <v>42614</v>
+      </c>
+      <c r="C111" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="D111" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="E111" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="F111" s="21" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -3157,13 +3190,13 @@
     <sortCondition ref="D427:D515"/>
   </sortState>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A22:A23 B6 B2 A7:A8 B9 A10:A16 B17 A18:A20 B21 A3:A5 B24 A25:A27 B28 B32 A29:A31 A33:A34 B35 A36:A37 B38 A39:A53 B54 A55:A57 B58 A59:A63 B64 A65:A80 B81 A82:A85 B86 A87:A104 B105 A106:A1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A22:A23 B6 B2 A7:A8 B9 A10:A16 B17 A18:A20 B21 A3:A5 B24 A25:A27 B28 B32 A29:A31 A33:A34 B35 A36:A37 B38 A39:A53 B54 A55:A57 B58 A59:A63 B64 A65:A80 B81 A82:A85 B86 A87:A104 B105 A106:A109 B110 A111:A1048576">
       <formula1>Task_type</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6 E2 D22:D23 D7:D8 E9 D10:D16 E17 D18:D20 E21 D3:D5 E24 D25:D27 E28 E32 D29:D31 D33:D34 E35 D36:D37 E38 D39:D53 E54 D55:D57 E58 D59:D63 E64 D65:D80 E81 D82:D85 E86 D87:D104 E105 D106:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6 E2 D22:D23 D7:D8 E9 D10:D16 E17 D18:D20 E21 D3:D5 E24 D25:D27 E28 E32 D29:D31 D33:D34 E35 D36:D37 E38 D39:D53 E54 D55:D57 E58 D59:D63 E64 D65:D80 E81 D82:D85 E86 D87:D104 E105 D106:D109 E110 D111:D1048576">
       <formula1>Building</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 A2 A9 A17 A21 A24 A28 A32 A35 A38 A54 A58 A64 A81 A86 A105">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 A2 A9 A17 A21 A24 A28 A32 A35 A38 A54 A58 A64 A81 A86 A105 A110">
       <formula1>Staff_Name</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
More bug fixes and optmizations
</commit_message>
<xml_diff>
--- a/CLASSOPS/Derek/Derek's Log.xlsx
+++ b/CLASSOPS/Derek/Derek's Log.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="196">
   <si>
     <t>Staff Name</t>
   </si>
@@ -644,6 +644,15 @@
   </si>
   <si>
     <t xml:space="preserve">Portable screen is there. Door code 7083* </t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Lectern mic, stand and cable. To Stedman 114L.</t>
+  </si>
+  <si>
+    <t>1430</t>
   </si>
 </sst>
 </file>
@@ -1176,11 +1185,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I111"/>
+  <dimension ref="A1:I115"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A94" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A111" sqref="A111"/>
+      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A115" sqref="A115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3181,6 +3190,76 @@
       </c>
       <c r="F111" s="21" t="s">
         <v>130</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A112" s="11"/>
+      <c r="B112" s="28"/>
+      <c r="C112" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="D112" s="11"/>
+      <c r="E112" s="32"/>
+      <c r="F112" s="34"/>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A113" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B113" s="26">
+        <v>42615</v>
+      </c>
+      <c r="C113" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="D113" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="E113" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="F113" s="21" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A114" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B114" s="26">
+        <v>42615</v>
+      </c>
+      <c r="C114" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="D114" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="E114" s="24" t="s">
+        <v>165</v>
+      </c>
+      <c r="F114" s="25" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A115" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B115" s="26">
+        <v>42615</v>
+      </c>
+      <c r="C115" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="D115" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="E115" s="24" t="s">
+        <v>193</v>
+      </c>
+      <c r="F115" s="25" t="s">
+        <v>194</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Major bug fix and optimization
</commit_message>
<xml_diff>
--- a/CLASSOPS/Derek/Derek's Log.xlsx
+++ b/CLASSOPS/Derek/Derek's Log.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="211">
   <si>
     <t>Staff Name</t>
   </si>
@@ -653,6 +653,71 @@
   </si>
   <si>
     <t>1430</t>
+  </si>
+  <si>
+    <t>2100</t>
+  </si>
+  <si>
+    <t>Door code 7083*  Neck mic and small PA, to Founders 156A.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Leave all in an lock room. Do not pick up equipment. Needed again tomorrow morning.</t>
+  </si>
+  <si>
+    <t>Return wireless keyboard &amp; projector remote to Founders 156A.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Leave mic cables in place.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Remove lec mic, stand, clip. Turn off PA as usual and lock room. To Founders 156A.</t>
+    </r>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Lec mic, stand and cable. To  Stedman 114L MCR.</t>
+  </si>
+  <si>
+    <t>135</t>
+  </si>
+  <si>
+    <t>258</t>
+  </si>
+  <si>
+    <t>Lec mic, stand and cable, small PA. To  Vanier 040.</t>
+  </si>
+  <si>
+    <t>Nat Taylor Cinema. Lock cinema all doors after shutdown.</t>
+  </si>
+  <si>
+    <t>Lec mic, stand and cable. To Vanier 040.</t>
+  </si>
+  <si>
+    <t>1730</t>
+  </si>
+  <si>
+    <t>2045</t>
   </si>
 </sst>
 </file>
@@ -1185,11 +1250,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I115"/>
+  <dimension ref="A1:I133"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A115" sqref="A115"/>
+      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C150" sqref="C150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3242,7 +3307,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A115" s="15" t="s">
         <v>92</v>
       </c>
@@ -3260,6 +3325,346 @@
       </c>
       <c r="F115" s="25" t="s">
         <v>194</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A116" s="11"/>
+      <c r="B116" s="28"/>
+      <c r="C116" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="D116" s="11"/>
+      <c r="E116" s="32"/>
+      <c r="F116" s="34"/>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A117" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B117" s="26">
+        <v>42619</v>
+      </c>
+      <c r="C117" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="D117" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="E117" s="24" t="s">
+        <v>148</v>
+      </c>
+      <c r="F117" s="25" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B118" s="26">
+        <v>42619</v>
+      </c>
+      <c r="C118" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="D118" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="E118" s="24" t="s">
+        <v>189</v>
+      </c>
+      <c r="F118" s="25" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="B119" s="26">
+        <v>42619</v>
+      </c>
+      <c r="C119" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="D119" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="E119" s="24" t="s">
+        <v>189</v>
+      </c>
+      <c r="F119" s="25" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="B120" s="26">
+        <v>42619</v>
+      </c>
+      <c r="C120" s="22" t="s">
+        <v>196</v>
+      </c>
+      <c r="D120" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="E120" s="24" t="s">
+        <v>175</v>
+      </c>
+      <c r="F120" s="25" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A121" s="11"/>
+      <c r="B121" s="11"/>
+      <c r="C121" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D121" s="13"/>
+      <c r="E121" s="11"/>
+      <c r="F121" s="13"/>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A122" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="B122" s="26">
+        <v>42620</v>
+      </c>
+      <c r="C122" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="D122" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="E122" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="F122" s="25" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A123" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B123" s="26">
+        <v>42620</v>
+      </c>
+      <c r="C123" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="D123" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="E123" s="24" t="s">
+        <v>201</v>
+      </c>
+      <c r="F123" s="25" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A124" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B124" s="26">
+        <v>42620</v>
+      </c>
+      <c r="C124" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="D124" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="E124" s="24" t="s">
+        <v>202</v>
+      </c>
+      <c r="F124" s="25" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A125" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B125" s="26">
+        <v>42620</v>
+      </c>
+      <c r="C125" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="D125" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="E125" s="24" t="s">
+        <v>193</v>
+      </c>
+      <c r="F125" s="25" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="B126" s="26">
+        <v>42620</v>
+      </c>
+      <c r="C126" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="D126" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="E126" s="24" t="s">
+        <v>175</v>
+      </c>
+      <c r="F126" s="25" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A127" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="B127" s="26">
+        <v>42620</v>
+      </c>
+      <c r="C127" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="D127" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="E127" s="24" t="s">
+        <v>175</v>
+      </c>
+      <c r="F127" s="25" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A128" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="B128" s="26">
+        <v>42620</v>
+      </c>
+      <c r="C128" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="D128" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="E128" s="24" t="s">
+        <v>179</v>
+      </c>
+      <c r="F128" s="25" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A129" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B129" s="26">
+        <v>42620</v>
+      </c>
+      <c r="C129" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="D129" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="E129" s="24" t="s">
+        <v>204</v>
+      </c>
+      <c r="F129" s="25" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A130" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B130" s="26">
+        <v>42620</v>
+      </c>
+      <c r="C130" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="D130" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="E130" s="24" t="s">
+        <v>205</v>
+      </c>
+      <c r="F130" s="25" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A131" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B131" s="26">
+        <v>42620</v>
+      </c>
+      <c r="C131" s="22" t="s">
+        <v>209</v>
+      </c>
+      <c r="D131" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="E131" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="F131" s="21" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A132" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B132" s="26">
+        <v>42620</v>
+      </c>
+      <c r="C132" s="22" t="s">
+        <v>210</v>
+      </c>
+      <c r="D132" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="E132" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="F132" s="19" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A133" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="B133" s="26">
+        <v>42620</v>
+      </c>
+      <c r="C133" s="22" t="s">
+        <v>210</v>
+      </c>
+      <c r="D133" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="E133" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="F133" s="25" t="s">
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -3269,13 +3674,13 @@
     <sortCondition ref="D427:D515"/>
   </sortState>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A22:A23 B6 B2 A7:A8 B9 A10:A16 B17 A18:A20 B21 A3:A5 B24 A25:A27 B28 B32 A29:A31 A33:A34 B35 A36:A37 B38 A39:A53 B54 A55:A57 B58 A59:A63 B64 A65:A80 B81 A82:A85 B86 A87:A104 B105 A106:A109 B110 A111:A1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A22:A23 B6 B2 A7:A8 B9 A10:A16 B17 A18:A20 B21 A3:A5 B24 A25:A27 B28 B32 A29:A31 A33:A34 B35 A36:A37 B38 A39:A53 B54 A55:A57 B58 A59:A63 B64 A65:A80 B81 A82:A85 B86 A87:A104 B105 A106:A109 B110 A111:A120 B121 A122:A1048576">
       <formula1>Task_type</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6 E2 D22:D23 D7:D8 E9 D10:D16 E17 D18:D20 E21 D3:D5 E24 D25:D27 E28 E32 D29:D31 D33:D34 E35 D36:D37 E38 D39:D53 E54 D55:D57 E58 D59:D63 E64 D65:D80 E81 D82:D85 E86 D87:D104 E105 D106:D109 E110 D111:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6 E2 D22:D23 D7:D8 E9 D10:D16 E17 D18:D20 E21 D3:D5 E24 D25:D27 E28 E32 D29:D31 D33:D34 E35 D36:D37 E38 D39:D53 E54 D55:D57 E58 D59:D63 E64 D65:D80 E81 D82:D85 E86 D87:D104 E105 D106:D109 E110 D111:D120 E121 D122:D1048576">
       <formula1>Building</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 A2 A9 A17 A21 A24 A28 A32 A35 A38 A54 A58 A64 A81 A86 A105 A110">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 A2 A9 A17 A21 A24 A28 A32 A35 A38 A54 A58 A64 A81 A86 A105 A110 A121">
       <formula1>Staff_Name</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Working on fixing a bug with the clo
</commit_message>
<xml_diff>
--- a/CLASSOPS/Derek/Derek's Log.xlsx
+++ b/CLASSOPS/Derek/Derek's Log.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="229">
   <si>
     <t>Staff Name</t>
   </si>
@@ -130,9 +130,6 @@
   </si>
   <si>
     <t>Christina</t>
-  </si>
-  <si>
-    <t>Clairissa</t>
   </si>
   <si>
     <t>Hasebullah</t>
@@ -718,6 +715,63 @@
   </si>
   <si>
     <t>2045</t>
+  </si>
+  <si>
+    <t>Clair</t>
+  </si>
+  <si>
+    <t>1550</t>
+  </si>
+  <si>
+    <t>S137</t>
+  </si>
+  <si>
+    <t>1820</t>
+  </si>
+  <si>
+    <t>109</t>
+  </si>
+  <si>
+    <t>1850</t>
+  </si>
+  <si>
+    <t>S105</t>
+  </si>
+  <si>
+    <t>S133</t>
+  </si>
+  <si>
+    <t>1005</t>
+  </si>
+  <si>
+    <t>Professor Elena Skliarenko</t>
+  </si>
+  <si>
+    <t>Professor Suzie Young</t>
+  </si>
+  <si>
+    <t>Professor Ken Ogata</t>
+  </si>
+  <si>
+    <t>Instructor Cheryl McPherson</t>
+  </si>
+  <si>
+    <t>Instructor Wendy Braithwaite</t>
+  </si>
+  <si>
+    <t>N146</t>
+  </si>
+  <si>
+    <t>Place overhead transparency projector on the desk, focus and demo the quick lamp change (QLC) feature. OV is there already and stays in 24/7.</t>
+  </si>
+  <si>
+    <t>2030</t>
+  </si>
+  <si>
+    <t>2200</t>
+  </si>
+  <si>
+    <t>118</t>
   </si>
 </sst>
 </file>
@@ -1250,11 +1304,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I133"/>
+  <dimension ref="A1:I145"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C150" sqref="C150"/>
+      <pane ySplit="1" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A145" sqref="A145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1273,7 +1327,7 @@
         <v>11</v>
       </c>
       <c r="B1" s="27" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C1" s="30" t="s">
         <v>20</v>
@@ -1292,7 +1346,7 @@
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D2" s="13"/>
       <c r="E2" s="11"/>
@@ -1309,63 +1363,63 @@
         <v>42570</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D3" s="23" t="s">
         <v>22</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F3" s="25" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B4" s="26">
         <v>42570</v>
       </c>
       <c r="C4" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="D4" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="E4" s="24" t="s">
-        <v>108</v>
-      </c>
       <c r="F4" s="25" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B5" s="26">
         <v>42570</v>
       </c>
       <c r="C5" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="D5" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="E5" s="24" t="s">
-        <v>110</v>
-      </c>
       <c r="F5" s="25" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D6" s="13"/>
       <c r="E6" s="11"/>
@@ -1382,16 +1436,16 @@
         <v>42571</v>
       </c>
       <c r="C7" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E7" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="D7" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>113</v>
-      </c>
       <c r="F7" s="19" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1402,23 +1456,23 @@
         <v>42571</v>
       </c>
       <c r="C8" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="D8" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>110</v>
-      </c>
       <c r="F8" s="25" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D9" s="13"/>
       <c r="E9" s="11"/>
@@ -1429,122 +1483,122 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B10" s="16">
         <v>42573</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E10" s="24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B11" s="16">
         <v>42573</v>
       </c>
       <c r="C11" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="D11" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="E11" s="24" t="s">
-        <v>110</v>
-      </c>
       <c r="F11" s="25" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B12" s="16">
         <v>42573</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E12" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="F12" s="25" t="s">
         <v>120</v>
-      </c>
-      <c r="F12" s="25" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B13" s="16">
         <v>42573</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E13" s="24" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F13" s="25" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B14" s="16">
         <v>42573</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E14" s="24" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F14" s="25" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B15" s="16">
         <v>42573</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E15" s="24" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F15" s="25" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1555,23 +1609,23 @@
         <v>42573</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D16" s="23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E16" s="24" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F16" s="25" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="11"/>
       <c r="B17" s="11"/>
       <c r="C17" s="12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D17" s="13"/>
       <c r="E17" s="11"/>
@@ -1588,16 +1642,16 @@
         <v>42576</v>
       </c>
       <c r="C18" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E18" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="D18" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="E18" s="17" t="s">
-        <v>113</v>
-      </c>
       <c r="F18" s="19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1608,16 +1662,16 @@
         <v>42576</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E19" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="F19" s="21" t="s">
         <v>129</v>
-      </c>
-      <c r="F19" s="21" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1628,23 +1682,23 @@
         <v>42576</v>
       </c>
       <c r="C20" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="E20" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="D20" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="E20" s="20" t="s">
+      <c r="F20" s="25" t="s">
         <v>132</v>
-      </c>
-      <c r="F20" s="25" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="21" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11"/>
       <c r="B21" s="11"/>
       <c r="C21" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D21" s="13"/>
       <c r="E21" s="11"/>
@@ -1661,43 +1715,43 @@
         <v>42577</v>
       </c>
       <c r="C22" s="22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D22" s="23" t="s">
         <v>22</v>
       </c>
       <c r="E22" s="24" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F22" s="25" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B23" s="26">
         <v>42577</v>
       </c>
       <c r="C23" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="D23" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E23" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="D23" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="E23" s="24" t="s">
-        <v>108</v>
-      </c>
       <c r="F23" s="25" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="24" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11"/>
       <c r="B24" s="11"/>
       <c r="C24" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D24" s="13"/>
       <c r="E24" s="11"/>
@@ -1714,36 +1768,36 @@
         <v>42578</v>
       </c>
       <c r="C25" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E25" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="D25" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="E25" s="17" t="s">
-        <v>113</v>
-      </c>
       <c r="F25" s="19" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B26" s="16">
         <v>42578</v>
       </c>
       <c r="C26" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="E26" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="D26" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="E26" s="15" t="s">
-        <v>110</v>
-      </c>
       <c r="F26" s="25" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -1754,23 +1808,23 @@
         <v>42578</v>
       </c>
       <c r="C27" s="22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E27" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="F27" s="21" t="s">
         <v>129</v>
-      </c>
-      <c r="F27" s="21" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="28" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="11"/>
       <c r="B28" s="11"/>
       <c r="C28" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D28" s="13"/>
       <c r="E28" s="11"/>
@@ -1787,16 +1841,16 @@
         <v>42579</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E29" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="F29" s="21" t="s">
         <v>129</v>
-      </c>
-      <c r="F29" s="21" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -1807,43 +1861,43 @@
         <v>42579</v>
       </c>
       <c r="C30" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E30" s="24" t="s">
         <v>135</v>
       </c>
-      <c r="D30" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="E30" s="24" t="s">
+      <c r="F30" s="25" t="s">
         <v>136</v>
-      </c>
-      <c r="F30" s="25" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B31" s="16">
         <v>42579</v>
       </c>
       <c r="C31" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="D31" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E31" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="D31" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="E31" s="24" t="s">
-        <v>108</v>
-      </c>
       <c r="F31" s="25" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="11"/>
       <c r="B32" s="11"/>
       <c r="C32" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D32" s="13"/>
       <c r="E32" s="11"/>
@@ -1854,22 +1908,22 @@
     </row>
     <row r="33" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B33" s="16">
         <v>42580</v>
       </c>
       <c r="C33" s="22" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D33" s="23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E33" s="24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F33" s="19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
@@ -1877,22 +1931,22 @@
     </row>
     <row r="34" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B34" s="16">
         <v>42580</v>
       </c>
       <c r="C34" s="22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D34" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E34" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="F34" s="25" t="s">
         <v>138</v>
-      </c>
-      <c r="F34" s="25" t="s">
-        <v>139</v>
       </c>
       <c r="G34" s="15"/>
       <c r="H34" s="15"/>
@@ -1902,7 +1956,7 @@
       <c r="A35" s="11"/>
       <c r="B35" s="11"/>
       <c r="C35" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D35" s="13"/>
       <c r="E35" s="11"/>
@@ -1916,43 +1970,43 @@
         <v>42584</v>
       </c>
       <c r="C36" s="22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D36" s="23" t="s">
         <v>22</v>
       </c>
       <c r="E36" s="24" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F36" s="25" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B37" s="26">
         <v>42584</v>
       </c>
       <c r="C37" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="D37" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E37" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="D37" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="E37" s="24" t="s">
-        <v>108</v>
-      </c>
       <c r="F37" s="25" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="11"/>
       <c r="B38" s="11"/>
       <c r="C38" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D38" s="13"/>
       <c r="E38" s="11"/>
@@ -1966,43 +2020,43 @@
         <v>42585</v>
       </c>
       <c r="C39" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="D39" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E39" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="D39" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="E39" s="17" t="s">
-        <v>113</v>
-      </c>
       <c r="F39" s="19" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B40" s="16">
         <v>42585</v>
       </c>
       <c r="C40" s="22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D40" s="23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E40" s="24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F40" s="19" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="11"/>
       <c r="B41" s="28"/>
       <c r="C41" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D41" s="11"/>
       <c r="E41" s="32"/>
@@ -2010,29 +2064,29 @@
     </row>
     <row r="42" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B42" s="16">
         <v>42587</v>
       </c>
       <c r="C42" s="22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D42" s="23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E42" s="24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F42" s="19" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="11"/>
       <c r="B43" s="28"/>
       <c r="C43" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D43" s="11"/>
       <c r="E43" s="32"/>
@@ -2040,22 +2094,22 @@
     </row>
     <row r="44" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B44" s="26">
         <v>42590</v>
       </c>
       <c r="C44" s="22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D44" s="23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E44" s="24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F44" s="25" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -2066,23 +2120,23 @@
         <v>42590</v>
       </c>
       <c r="C45" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="D45" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E45" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="D45" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="E45" s="17" t="s">
-        <v>113</v>
-      </c>
       <c r="F45" s="19" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="11"/>
       <c r="B46" s="28"/>
       <c r="C46" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D46" s="11"/>
       <c r="E46" s="32"/>
@@ -2090,42 +2144,42 @@
     </row>
     <row r="47" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B47" s="26">
         <v>42594</v>
       </c>
       <c r="C47" s="22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D47" s="23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E47" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="F47" s="25" t="s">
         <v>142</v>
-      </c>
-      <c r="F47" s="25" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B48" s="26">
         <v>42594</v>
       </c>
       <c r="C48" s="22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D48" s="23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E48" s="24" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F48" s="25" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -2136,23 +2190,23 @@
         <v>42594</v>
       </c>
       <c r="C49" s="22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D49" s="23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E49" s="24" t="s">
+        <v>143</v>
+      </c>
+      <c r="F49" s="25" t="s">
         <v>144</v>
-      </c>
-      <c r="F49" s="25" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="11"/>
       <c r="B50" s="28"/>
       <c r="C50" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D50" s="11"/>
       <c r="E50" s="32"/>
@@ -2160,22 +2214,22 @@
     </row>
     <row r="51" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B51" s="26">
         <v>42597</v>
       </c>
       <c r="C51" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="D51" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E51" s="17" t="s">
         <v>146</v>
       </c>
-      <c r="D51" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="E51" s="17" t="s">
-        <v>147</v>
-      </c>
       <c r="F51" s="19" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
@@ -2186,16 +2240,16 @@
         <v>42597</v>
       </c>
       <c r="C52" s="22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D52" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E52" s="24" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F52" s="25" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -2206,23 +2260,23 @@
         <v>42597</v>
       </c>
       <c r="C53" s="22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D53" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E53" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="F53" s="25" t="s">
         <v>136</v>
-      </c>
-      <c r="F53" s="25" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="11"/>
       <c r="B54" s="11"/>
       <c r="C54" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D54" s="13"/>
       <c r="E54" s="11"/>
@@ -2230,22 +2284,22 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B55" s="26">
         <v>42598</v>
       </c>
       <c r="C55" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="D55" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E55" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="D55" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="E55" s="24" t="s">
+      <c r="F55" s="25" t="s">
         <v>151</v>
-      </c>
-      <c r="F55" s="25" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -2256,16 +2310,16 @@
         <v>42598</v>
       </c>
       <c r="C56" s="22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D56" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E56" s="24" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F56" s="25" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -2276,23 +2330,23 @@
         <v>42598</v>
       </c>
       <c r="C57" s="22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D57" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E57" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="F57" s="25" t="s">
         <v>136</v>
-      </c>
-      <c r="F57" s="25" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="11"/>
       <c r="B58" s="11"/>
       <c r="C58" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D58" s="13"/>
       <c r="E58" s="11"/>
@@ -2300,62 +2354,62 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B59" s="16">
         <v>42599</v>
       </c>
       <c r="C59" s="17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D59" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E59" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="F59" s="19" t="s">
         <v>154</v>
-      </c>
-      <c r="F59" s="19" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B60" s="16">
         <v>42599</v>
       </c>
       <c r="C60" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="D60" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E60" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="D60" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="E60" s="24" t="s">
-        <v>151</v>
-      </c>
       <c r="F60" s="25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B61" s="16">
         <v>42599</v>
       </c>
       <c r="C61" s="22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D61" s="23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E61" s="24" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F61" s="19" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
@@ -2366,16 +2420,16 @@
         <v>42599</v>
       </c>
       <c r="C62" s="22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D62" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E62" s="24" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F62" s="25" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
@@ -2386,23 +2440,23 @@
         <v>42599</v>
       </c>
       <c r="C63" s="22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D63" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E63" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="F63" s="25" t="s">
         <v>136</v>
-      </c>
-      <c r="F63" s="25" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="64" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="11"/>
       <c r="B64" s="11"/>
       <c r="C64" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D64" s="13"/>
       <c r="E64" s="11"/>
@@ -2413,42 +2467,42 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B65" s="16">
         <v>42600</v>
       </c>
       <c r="C65" s="22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D65" s="23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E65" s="24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F65" s="25" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A66" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B66" s="16">
         <v>42600</v>
       </c>
       <c r="C66" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="D66" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E66" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="D66" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="E66" s="24" t="s">
-        <v>151</v>
-      </c>
       <c r="F66" s="25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -2459,16 +2513,16 @@
         <v>42600</v>
       </c>
       <c r="C67" s="22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D67" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E67" s="24" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F67" s="25" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -2479,23 +2533,23 @@
         <v>42600</v>
       </c>
       <c r="C68" s="22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D68" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E68" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="F68" s="25" t="s">
         <v>136</v>
-      </c>
-      <c r="F68" s="25" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="11"/>
       <c r="B69" s="28"/>
       <c r="C69" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D69" s="11"/>
       <c r="E69" s="32"/>
@@ -2503,69 +2557,69 @@
     </row>
     <row r="70" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B70" s="16">
         <v>42601</v>
       </c>
       <c r="C70" s="22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D70" s="23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E70" s="24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F70" s="25" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="43.15" x14ac:dyDescent="0.3">
       <c r="A71" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B71" s="26">
         <v>42601</v>
       </c>
       <c r="C71" s="22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D71" s="23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E71" s="24" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F71" s="25" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B72" s="26">
         <v>42601</v>
       </c>
       <c r="C72" s="22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D72" s="23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E72" s="24" t="s">
+        <v>159</v>
+      </c>
+      <c r="F72" s="25" t="s">
         <v>160</v>
-      </c>
-      <c r="F72" s="25" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="11"/>
       <c r="B73" s="28"/>
       <c r="C73" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D73" s="11"/>
       <c r="E73" s="32"/>
@@ -2579,16 +2633,16 @@
         <v>42604</v>
       </c>
       <c r="C74" s="22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D74" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E74" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="F74" s="21" t="s">
         <v>129</v>
-      </c>
-      <c r="F74" s="21" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -2599,16 +2653,16 @@
         <v>42604</v>
       </c>
       <c r="C75" s="22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D75" s="23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E75" s="24" t="s">
+        <v>164</v>
+      </c>
+      <c r="F75" s="25" t="s">
         <v>165</v>
-      </c>
-      <c r="F75" s="25" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
@@ -2619,23 +2673,23 @@
         <v>42604</v>
       </c>
       <c r="C76" s="22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D76" s="23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E76" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="F76" s="25" t="s">
         <v>163</v>
-      </c>
-      <c r="F76" s="25" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="11"/>
       <c r="B77" s="28"/>
       <c r="C77" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D77" s="11"/>
       <c r="E77" s="32"/>
@@ -2643,22 +2697,22 @@
     </row>
     <row r="78" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B78" s="26">
         <v>42605</v>
       </c>
       <c r="C78" s="22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D78" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E78" s="24" t="s">
+        <v>166</v>
+      </c>
+      <c r="F78" s="25" t="s">
         <v>167</v>
-      </c>
-      <c r="F78" s="25" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -2669,16 +2723,16 @@
         <v>42605</v>
       </c>
       <c r="C79" s="22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D79" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E79" s="24" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F79" s="25" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="80" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2689,23 +2743,23 @@
         <v>42605</v>
       </c>
       <c r="C80" s="22" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D80" s="23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E80" s="24" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F80" s="25" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="11"/>
       <c r="B81" s="11"/>
       <c r="C81" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D81" s="13"/>
       <c r="E81" s="11"/>
@@ -2713,22 +2767,22 @@
     </row>
     <row r="82" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B82" s="16">
         <v>42606</v>
       </c>
       <c r="C82" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="D82" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E82" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="D82" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="E82" s="24" t="s">
-        <v>151</v>
-      </c>
       <c r="F82" s="25" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
@@ -2739,16 +2793,16 @@
         <v>42606</v>
       </c>
       <c r="C83" s="22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D83" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E83" s="24" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F83" s="25" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
@@ -2759,16 +2813,16 @@
         <v>42606</v>
       </c>
       <c r="C84" s="22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D84" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E84" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="F84" s="25" t="s">
         <v>136</v>
-      </c>
-      <c r="F84" s="25" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
@@ -2779,23 +2833,23 @@
         <v>42606</v>
       </c>
       <c r="C85" s="22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D85" s="23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E85" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="F85" s="25" t="s">
         <v>163</v>
-      </c>
-      <c r="F85" s="25" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="86" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="11"/>
       <c r="B86" s="11"/>
       <c r="C86" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D86" s="13"/>
       <c r="E86" s="11"/>
@@ -2812,23 +2866,23 @@
         <v>42607</v>
       </c>
       <c r="C87" s="22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D87" s="23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E87" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="F87" s="25" t="s">
         <v>163</v>
-      </c>
-      <c r="F87" s="25" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="11"/>
       <c r="B88" s="28"/>
       <c r="C88" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D88" s="11"/>
       <c r="E88" s="32"/>
@@ -2836,82 +2890,82 @@
     </row>
     <row r="89" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B89" s="26">
         <v>42608</v>
       </c>
       <c r="C89" s="22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D89" s="23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E89" s="24" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F89" s="25" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="90" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B90" s="26">
         <v>42608</v>
       </c>
       <c r="C90" s="22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D90" s="23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E90" s="24" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F90" s="25" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="91" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B91" s="26">
         <v>42608</v>
       </c>
       <c r="C91" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="D91" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="E91" s="24" t="s">
         <v>174</v>
       </c>
-      <c r="D91" s="23" t="s">
-        <v>79</v>
-      </c>
-      <c r="E91" s="24" t="s">
-        <v>175</v>
-      </c>
       <c r="F91" s="25" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B92" s="26">
         <v>42608</v>
       </c>
       <c r="C92" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="D92" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="E92" s="24" t="s">
         <v>174</v>
       </c>
-      <c r="D92" s="23" t="s">
-        <v>79</v>
-      </c>
-      <c r="E92" s="24" t="s">
+      <c r="F92" s="25" t="s">
         <v>175</v>
-      </c>
-      <c r="F92" s="25" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
@@ -2922,23 +2976,23 @@
         <v>42608</v>
       </c>
       <c r="C93" s="22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D93" s="23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E93" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="F93" s="25" t="s">
         <v>163</v>
-      </c>
-      <c r="F93" s="25" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="11"/>
       <c r="B94" s="28"/>
       <c r="C94" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D94" s="11"/>
       <c r="E94" s="32"/>
@@ -2946,69 +3000,69 @@
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B95" s="26">
         <v>42611</v>
       </c>
       <c r="C95" s="22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D95" s="23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E95" s="24" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F95" s="25" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B96" s="26">
         <v>42611</v>
       </c>
       <c r="C96" s="22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D96" s="23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E96" s="24" t="s">
+        <v>178</v>
+      </c>
+      <c r="F96" s="25" t="s">
         <v>179</v>
-      </c>
-      <c r="F96" s="25" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="97" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A97" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B97" s="26">
         <v>42611</v>
       </c>
       <c r="C97" s="22" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D97" s="23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E97" s="24" t="s">
+        <v>180</v>
+      </c>
+      <c r="F97" s="25" t="s">
         <v>181</v>
-      </c>
-      <c r="F97" s="25" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="11"/>
       <c r="B98" s="28"/>
       <c r="C98" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D98" s="11"/>
       <c r="E98" s="32"/>
@@ -3016,22 +3070,22 @@
     </row>
     <row r="99" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A99" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B99" s="26">
         <v>42612</v>
       </c>
       <c r="C99" s="22" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D99" s="23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E99" s="24" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F99" s="19" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
@@ -3042,16 +3096,16 @@
         <v>42612</v>
       </c>
       <c r="C100" s="22" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D100" s="23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E100" s="24" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F100" s="25" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
@@ -3062,83 +3116,83 @@
         <v>42612</v>
       </c>
       <c r="C101" s="22" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D101" s="23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E101" s="24" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F101" s="25" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B102" s="26">
         <v>42612</v>
       </c>
       <c r="C102" s="22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D102" s="23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E102" s="24" t="s">
+        <v>178</v>
+      </c>
+      <c r="F102" s="25" t="s">
         <v>179</v>
-      </c>
-      <c r="F102" s="25" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B103" s="26">
         <v>42612</v>
       </c>
       <c r="C103" s="22" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D103" s="23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E103" s="24" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F103" s="25" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="104" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B104" s="26">
         <v>42612</v>
       </c>
       <c r="C104" s="22" t="s">
+        <v>189</v>
+      </c>
+      <c r="D104" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="E104" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="F104" s="25" t="s">
         <v>190</v>
-      </c>
-      <c r="D104" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="E104" s="24" t="s">
-        <v>189</v>
-      </c>
-      <c r="F104" s="25" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="11"/>
       <c r="B105" s="11"/>
       <c r="C105" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D105" s="13"/>
       <c r="E105" s="11"/>
@@ -3152,16 +3206,16 @@
         <v>42613</v>
       </c>
       <c r="C106" s="22" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D106" s="23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E106" s="24" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F106" s="25" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
@@ -3172,63 +3226,63 @@
         <v>42613</v>
       </c>
       <c r="C107" s="22" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D107" s="23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E107" s="24" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F107" s="25" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="108" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B108" s="16">
         <v>42613</v>
       </c>
       <c r="C108" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="D108" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="E108" s="24" t="s">
         <v>174</v>
       </c>
-      <c r="D108" s="23" t="s">
-        <v>79</v>
-      </c>
-      <c r="E108" s="24" t="s">
-        <v>175</v>
-      </c>
       <c r="F108" s="25" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B109" s="16">
         <v>42613</v>
       </c>
       <c r="C109" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="D109" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="E109" s="24" t="s">
         <v>174</v>
       </c>
-      <c r="D109" s="23" t="s">
-        <v>79</v>
-      </c>
-      <c r="E109" s="24" t="s">
+      <c r="F109" s="25" t="s">
         <v>175</v>
-      </c>
-      <c r="F109" s="25" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="110" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="11"/>
       <c r="B110" s="11"/>
       <c r="C110" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D110" s="13"/>
       <c r="E110" s="11"/>
@@ -3245,23 +3299,23 @@
         <v>42614</v>
       </c>
       <c r="C111" s="22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D111" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E111" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="F111" s="21" t="s">
         <v>129</v>
-      </c>
-      <c r="F111" s="21" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="11"/>
       <c r="B112" s="28"/>
       <c r="C112" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D112" s="11"/>
       <c r="E112" s="32"/>
@@ -3275,16 +3329,16 @@
         <v>42615</v>
       </c>
       <c r="C113" s="22" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D113" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E113" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="F113" s="21" t="s">
         <v>129</v>
-      </c>
-      <c r="F113" s="21" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
@@ -3295,43 +3349,43 @@
         <v>42615</v>
       </c>
       <c r="C114" s="22" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D114" s="23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E114" s="24" t="s">
+        <v>164</v>
+      </c>
+      <c r="F114" s="25" t="s">
         <v>165</v>
-      </c>
-      <c r="F114" s="25" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="115" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A115" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B115" s="26">
         <v>42615</v>
       </c>
       <c r="C115" s="22" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D115" s="23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E115" s="24" t="s">
+        <v>192</v>
+      </c>
+      <c r="F115" s="25" t="s">
         <v>193</v>
-      </c>
-      <c r="F115" s="25" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="11"/>
       <c r="B116" s="28"/>
       <c r="C116" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D116" s="11"/>
       <c r="E116" s="32"/>
@@ -3345,83 +3399,83 @@
         <v>42619</v>
       </c>
       <c r="C117" s="22" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D117" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E117" s="24" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F117" s="25" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="118" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B118" s="26">
         <v>42619</v>
       </c>
       <c r="C118" s="22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D118" s="23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E118" s="24" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F118" s="25" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="119" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B119" s="26">
         <v>42619</v>
       </c>
       <c r="C119" s="22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D119" s="23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E119" s="24" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F119" s="25" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="120" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B120" s="26">
         <v>42619</v>
       </c>
       <c r="C120" s="22" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D120" s="23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E120" s="24" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F120" s="25" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="11"/>
       <c r="B121" s="11"/>
       <c r="C121" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D121" s="13"/>
       <c r="E121" s="11"/>
@@ -3429,185 +3483,185 @@
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B122" s="26">
         <v>42620</v>
       </c>
       <c r="C122" s="22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D122" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E122" s="24" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F122" s="25" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B123" s="26">
         <v>42620</v>
       </c>
       <c r="C123" s="22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D123" s="23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E123" s="24" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F123" s="25" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B124" s="26">
         <v>42620</v>
       </c>
       <c r="C124" s="22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D124" s="23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E124" s="24" t="s">
+        <v>201</v>
+      </c>
+      <c r="F124" s="25" t="s">
         <v>202</v>
-      </c>
-      <c r="F124" s="25" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B125" s="26">
         <v>42620</v>
       </c>
       <c r="C125" s="22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D125" s="23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E125" s="24" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F125" s="25" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="126" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B126" s="26">
         <v>42620</v>
       </c>
       <c r="C126" s="22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D126" s="23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E126" s="24" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F126" s="25" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B127" s="26">
         <v>42620</v>
       </c>
       <c r="C127" s="22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D127" s="23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E127" s="24" t="s">
+        <v>174</v>
+      </c>
+      <c r="F127" s="25" t="s">
         <v>175</v>
-      </c>
-      <c r="F127" s="25" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B128" s="26">
         <v>42620</v>
       </c>
       <c r="C128" s="22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D128" s="23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E128" s="24" t="s">
+        <v>178</v>
+      </c>
+      <c r="F128" s="25" t="s">
         <v>179</v>
       </c>
-      <c r="F128" s="25" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B129" s="26">
         <v>42620</v>
       </c>
       <c r="C129" s="22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D129" s="23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E129" s="24" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F129" s="25" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B130" s="26">
         <v>42620</v>
       </c>
       <c r="C130" s="22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D130" s="23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E130" s="24" t="s">
+        <v>204</v>
+      </c>
+      <c r="F130" s="25" t="s">
         <v>205</v>
       </c>
-      <c r="F130" s="25" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" s="15" t="s">
         <v>19</v>
       </c>
@@ -3615,56 +3669,289 @@
         <v>42620</v>
       </c>
       <c r="C131" s="22" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D131" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E131" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="F131" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="F131" s="21" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="132" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="132" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A132" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B132" s="26">
         <v>42620</v>
       </c>
       <c r="C132" s="22" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D132" s="23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E132" s="24" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F132" s="19" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B133" s="26">
         <v>42620</v>
       </c>
       <c r="C133" s="22" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D133" s="23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E133" s="24" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F133" s="25" t="s">
-        <v>199</v>
+        <v>198</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="11"/>
+      <c r="B134" s="11"/>
+      <c r="C134" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="D134" s="13"/>
+      <c r="E134" s="11"/>
+      <c r="F134" s="13"/>
+      <c r="G134" s="14"/>
+      <c r="H134" s="11"/>
+      <c r="I134" s="11"/>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A135" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B135" s="26">
+        <v>42621</v>
+      </c>
+      <c r="C135" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="D135" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E135" s="24" t="s">
+        <v>212</v>
+      </c>
+      <c r="F135" s="25" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A136" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B136" s="26">
+        <v>42621</v>
+      </c>
+      <c r="C136" s="22" t="s">
+        <v>213</v>
+      </c>
+      <c r="D136" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="E136" s="24" t="s">
+        <v>214</v>
+      </c>
+      <c r="F136" s="25" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A137" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B137" s="26">
+        <v>42621</v>
+      </c>
+      <c r="C137" s="22" t="s">
+        <v>215</v>
+      </c>
+      <c r="D137" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E137" s="24" t="s">
+        <v>216</v>
+      </c>
+      <c r="F137" s="25" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A138" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B138" s="26">
+        <v>42621</v>
+      </c>
+      <c r="C138" s="22" t="s">
+        <v>215</v>
+      </c>
+      <c r="D138" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E138" s="24" t="s">
+        <v>217</v>
+      </c>
+      <c r="F138" s="25" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A139" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B139" s="26">
+        <v>42621</v>
+      </c>
+      <c r="C139" s="22" t="s">
+        <v>215</v>
+      </c>
+      <c r="D139" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="E139" s="24" t="s">
+        <v>218</v>
+      </c>
+      <c r="F139" s="25" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A140" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B140" s="26">
+        <v>42621</v>
+      </c>
+      <c r="C140" s="22" t="s">
+        <v>215</v>
+      </c>
+      <c r="D140" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E140" s="24" t="s">
+        <v>224</v>
+      </c>
+      <c r="F140" s="25" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A141" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B141" s="26">
+        <v>42621</v>
+      </c>
+      <c r="C141" s="22" t="s">
+        <v>226</v>
+      </c>
+      <c r="D141" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E141" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="F141" s="21" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A142" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B142" s="26">
+        <v>42621</v>
+      </c>
+      <c r="C142" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="D142" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E142" s="24" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A143" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B143" s="26">
+        <v>42621</v>
+      </c>
+      <c r="C143" s="22" t="s">
+        <v>227</v>
+      </c>
+      <c r="D143" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E143" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="F143" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="G143" s="15"/>
+      <c r="H143" s="15"/>
+      <c r="I143" s="15"/>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A144" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B144" s="26">
+        <v>42615</v>
+      </c>
+      <c r="C144" s="22" t="s">
+        <v>226</v>
+      </c>
+      <c r="D144" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="E144" s="24" t="s">
+        <v>164</v>
+      </c>
+      <c r="F144" s="25" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A145" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B145" s="26">
+        <v>42615</v>
+      </c>
+      <c r="C145" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="D145" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="E145" s="24" t="s">
+        <v>228</v>
+      </c>
+      <c r="F145" s="25" t="s">
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -3674,13 +3961,13 @@
     <sortCondition ref="D427:D515"/>
   </sortState>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A22:A23 B6 B2 A7:A8 B9 A10:A16 B17 A18:A20 B21 A3:A5 B24 A25:A27 B28 B32 A29:A31 A33:A34 B35 A36:A37 B38 A39:A53 B54 A55:A57 B58 A59:A63 B64 A65:A80 B81 A82:A85 B86 A87:A104 B105 A106:A109 B110 A111:A120 B121 A122:A1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A22:A23 B6 B2 A7:A8 B9 A10:A16 B17 A18:A20 B21 A3:A5 B24 A25:A27 B28 B32 A29:A31 A33:A34 B35 A36:A37 B38 A39:A53 B54 A55:A57 B58 A59:A63 B64 A65:A80 B81 A82:A85 B86 A87:A104 B105 A106:A109 B110 A111:A120 B121 A122:A133 B134 A135:A1048576">
       <formula1>Task_type</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6 E2 D22:D23 D7:D8 E9 D10:D16 E17 D18:D20 E21 D3:D5 E24 D25:D27 E28 E32 D29:D31 D33:D34 E35 D36:D37 E38 D39:D53 E54 D55:D57 E58 D59:D63 E64 D65:D80 E81 D82:D85 E86 D87:D104 E105 D106:D109 E110 D111:D120 E121 D122:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6 E2 D22:D23 D7:D8 E9 D10:D16 E17 D18:D20 E21 D3:D5 E24 D25:D27 E28 E32 D29:D31 D33:D34 E35 D36:D37 E38 D39:D53 E54 D55:D57 E58 D59:D63 E64 D65:D80 E81 D82:D85 E86 D87:D104 E105 D106:D109 E110 D111:D120 E121 D122:D133 E134 D135:D1048576">
       <formula1>Building</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 A2 A9 A17 A21 A24 A28 A32 A35 A38 A54 A58 A64 A81 A86 A105 A110 A121">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 A2 A9 A17 A21 A24 A28 A32 A35 A38 A54 A58 A64 A81 A86 A105 A110 A121 A134">
       <formula1>Staff_Name</formula1>
     </dataValidation>
   </dataValidations>
@@ -3696,8 +3983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C58"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A38" sqref="A2:A38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3720,10 +4007,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>21</v>
@@ -3748,7 +4035,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -3759,23 +4046,23 @@
         <v>16</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>14</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>15</v>
@@ -3786,24 +4073,24 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>19</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>36</v>
+        <v>210</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -3811,7 +4098,7 @@
         <v>32</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>23</v>
@@ -3819,10 +4106,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>28</v>
@@ -3833,7 +4120,7 @@
         <v>3</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>24</v>
@@ -3844,21 +4131,21 @@
         <v>7</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -3866,10 +4153,10 @@
         <v>4</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -3880,37 +4167,37 @@
         <v>13</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>29</v>
@@ -3921,10 +4208,10 @@
         <v>6</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -3932,18 +4219,18 @@
         <v>34</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>26</v>
@@ -3951,72 +4238,72 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
@@ -4024,15 +4311,15 @@
         <v>8</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
@@ -4040,10 +4327,10 @@
         <v>33</v>
       </c>
       <c r="C33" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>9</v>
       </c>
@@ -4051,48 +4338,48 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C35" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C36" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C36" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C37" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C37" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A38" s="1" t="s">
-        <v>102</v>
-      </c>
       <c r="C38" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="C39" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="C40" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
File update, still in local mode
</commit_message>
<xml_diff>
--- a/CLASSOPS/Derek/Derek's Log.xlsx
+++ b/CLASSOPS/Derek/Derek's Log.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="229">
   <si>
     <t>Staff Name</t>
   </si>
@@ -1304,11 +1304,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I145"/>
+  <dimension ref="A1:I151"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B136" sqref="B136:B145"/>
+      <pane ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A152" sqref="A152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3739,7 +3739,7 @@
         <v>12</v>
       </c>
       <c r="B135" s="26">
-        <v>42622</v>
+        <v>42621</v>
       </c>
       <c r="C135" s="22" t="s">
         <v>211</v>
@@ -3759,7 +3759,7 @@
         <v>12</v>
       </c>
       <c r="B136" s="26">
-        <v>42622</v>
+        <v>42621</v>
       </c>
       <c r="C136" s="22" t="s">
         <v>213</v>
@@ -3779,7 +3779,7 @@
         <v>12</v>
       </c>
       <c r="B137" s="26">
-        <v>42622</v>
+        <v>42621</v>
       </c>
       <c r="C137" s="22" t="s">
         <v>215</v>
@@ -3799,7 +3799,7 @@
         <v>12</v>
       </c>
       <c r="B138" s="26">
-        <v>42622</v>
+        <v>42621</v>
       </c>
       <c r="C138" s="22" t="s">
         <v>215</v>
@@ -3819,7 +3819,7 @@
         <v>12</v>
       </c>
       <c r="B139" s="26">
-        <v>42622</v>
+        <v>42621</v>
       </c>
       <c r="C139" s="22" t="s">
         <v>215</v>
@@ -3839,7 +3839,7 @@
         <v>19</v>
       </c>
       <c r="B140" s="26">
-        <v>42622</v>
+        <v>42621</v>
       </c>
       <c r="C140" s="22" t="s">
         <v>215</v>
@@ -3859,7 +3859,7 @@
         <v>19</v>
       </c>
       <c r="B141" s="26">
-        <v>42622</v>
+        <v>42621</v>
       </c>
       <c r="C141" s="22" t="s">
         <v>226</v>
@@ -3879,7 +3879,7 @@
         <v>80</v>
       </c>
       <c r="B142" s="26">
-        <v>42622</v>
+        <v>42621</v>
       </c>
       <c r="C142" s="22" t="s">
         <v>208</v>
@@ -3896,7 +3896,7 @@
         <v>80</v>
       </c>
       <c r="B143" s="26">
-        <v>42622</v>
+        <v>42621</v>
       </c>
       <c r="C143" s="22" t="s">
         <v>227</v>
@@ -3919,7 +3919,7 @@
         <v>19</v>
       </c>
       <c r="B144" s="26">
-        <v>42622</v>
+        <v>42621</v>
       </c>
       <c r="C144" s="22" t="s">
         <v>226</v>
@@ -3934,12 +3934,12 @@
         <v>165</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B145" s="26">
-        <v>42622</v>
+        <v>42621</v>
       </c>
       <c r="C145" s="22" t="s">
         <v>134</v>
@@ -3951,6 +3951,119 @@
         <v>228</v>
       </c>
       <c r="F145" s="25" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A146" s="11"/>
+      <c r="B146" s="11"/>
+      <c r="C146" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="D146" s="13"/>
+      <c r="E146" s="11"/>
+      <c r="F146" s="13"/>
+      <c r="G146" s="14"/>
+      <c r="H146" s="11"/>
+      <c r="I146" s="11"/>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A147" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B147" s="26">
+        <v>42622</v>
+      </c>
+      <c r="C147" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="D147" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E147" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="F147" s="25" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A148" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B148" s="26">
+        <v>42622</v>
+      </c>
+      <c r="C148" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="D148" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E148" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="F148" s="25" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A149" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B149" s="26">
+        <v>42622</v>
+      </c>
+      <c r="C149" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="D149" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E149" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="F149" s="21" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A150" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B150" s="26">
+        <v>42622</v>
+      </c>
+      <c r="C150" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="D150" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="E150" s="24" t="s">
+        <v>164</v>
+      </c>
+      <c r="F150" s="25" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A151" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B151" s="26">
+        <v>42622</v>
+      </c>
+      <c r="C151" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="D151" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="E151" s="24" t="s">
+        <v>228</v>
+      </c>
+      <c r="F151" s="25" t="s">
         <v>165</v>
       </c>
     </row>
@@ -3961,13 +4074,13 @@
     <sortCondition ref="D427:D515"/>
   </sortState>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A22:A23 B6 B2 A7:A8 B9 A10:A16 B17 A18:A20 B21 A3:A5 B24 A25:A27 B28 B32 A29:A31 A33:A34 B35 A36:A37 B38 A39:A53 B54 A55:A57 B58 A59:A63 B64 A65:A80 B81 A82:A85 B86 A87:A104 B105 A106:A109 B110 A111:A120 B121 A122:A133 B134 A135:A1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A22:A23 B6 B2 A7:A8 B9 A10:A16 B17 A18:A20 B21 A3:A5 B24 A25:A27 B28 B32 A29:A31 A33:A34 B35 A36:A37 B38 A39:A53 B54 A55:A57 B58 A59:A63 B64 A65:A80 B81 A82:A85 B86 A87:A104 B105 A106:A109 B110 A111:A120 B121 A122:A133 B134 A135:A145 B146 A147:A1048576">
       <formula1>Task_type</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6 E2 D22:D23 D7:D8 E9 D10:D16 E17 D18:D20 E21 D3:D5 E24 D25:D27 E28 E32 D29:D31 D33:D34 E35 D36:D37 E38 D39:D53 E54 D55:D57 E58 D59:D63 E64 D65:D80 E81 D82:D85 E86 D87:D104 E105 D106:D109 E110 D111:D120 E121 D122:D133 E134 D135:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6 E2 D22:D23 D7:D8 E9 D10:D16 E17 D18:D20 E21 D3:D5 E24 D25:D27 E28 E32 D29:D31 D33:D34 E35 D36:D37 E38 D39:D53 E54 D55:D57 E58 D59:D63 E64 D65:D80 E81 D82:D85 E86 D87:D104 E105 D106:D109 E110 D111:D120 E121 D122:D133 E134 D135:D145 E146 D147:D1048576">
       <formula1>Building</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 A2 A9 A17 A21 A24 A28 A32 A35 A38 A54 A58 A64 A81 A86 A105 A110 A121 A134">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 A2 A9 A17 A21 A24 A28 A32 A35 A38 A54 A58 A64 A81 A86 A105 A110 A121 A134 A146">
       <formula1>Staff_Name</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Minor bug fixes and we are still on locals
</commit_message>
<xml_diff>
--- a/CLASSOPS/Derek/Derek's Log.xlsx
+++ b/CLASSOPS/Derek/Derek's Log.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="245">
   <si>
     <t>Staff Name</t>
   </si>
@@ -772,6 +772,54 @@
   </si>
   <si>
     <t>118</t>
+  </si>
+  <si>
+    <t>004</t>
+  </si>
+  <si>
+    <t>Gary Spraakman</t>
+  </si>
+  <si>
+    <t>303</t>
+  </si>
+  <si>
+    <t>Karl Schmid</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>Alan Marshall</t>
+  </si>
+  <si>
+    <t>107A</t>
+  </si>
+  <si>
+    <t>Marie-Jolie Rwigema</t>
+  </si>
+  <si>
+    <t>Lisa Feldstein</t>
+  </si>
+  <si>
+    <t>N812</t>
+  </si>
+  <si>
+    <t>S801</t>
+  </si>
+  <si>
+    <t>Rick Sin</t>
+  </si>
+  <si>
+    <t>1830</t>
+  </si>
+  <si>
+    <t>1152A</t>
+  </si>
+  <si>
+    <t>Roll-in PC.  Disconnect from laptop input and store in Vari 1155.</t>
+  </si>
+  <si>
+    <t>2150</t>
   </si>
 </sst>
 </file>
@@ -1304,11 +1352,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I151"/>
+  <dimension ref="A1:I166"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A152" sqref="A152"/>
+      <pane ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G166" sqref="G166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4065,6 +4113,284 @@
       </c>
       <c r="F151" s="25" t="s">
         <v>165</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A152" s="11"/>
+      <c r="B152" s="28"/>
+      <c r="C152" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="D152" s="11"/>
+      <c r="E152" s="32"/>
+      <c r="F152" s="34"/>
+    </row>
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A153" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B153" s="26">
+        <v>42625</v>
+      </c>
+      <c r="C153" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="D153" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="E153" s="24" t="s">
+        <v>229</v>
+      </c>
+      <c r="F153" s="25" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A154" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B154" s="26">
+        <v>42625</v>
+      </c>
+      <c r="C154" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="D154" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="E154" s="24" t="s">
+        <v>231</v>
+      </c>
+      <c r="F154" s="25" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A155" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B155" s="26">
+        <v>42625</v>
+      </c>
+      <c r="C155" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="D155" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E155" s="24" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A156" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B156" s="26">
+        <v>42625</v>
+      </c>
+      <c r="C156" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="D156" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="E156" s="24" t="s">
+        <v>233</v>
+      </c>
+      <c r="F156" s="25" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A157" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B157" s="26">
+        <v>42625</v>
+      </c>
+      <c r="C157" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="D157" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="E157" s="24" t="s">
+        <v>235</v>
+      </c>
+      <c r="F157" s="25" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A158" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="B158" s="26">
+        <v>42625</v>
+      </c>
+      <c r="C158" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="D158" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="E158" s="24" t="s">
+        <v>178</v>
+      </c>
+      <c r="F158" s="25" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A159" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B159" s="26">
+        <v>42625</v>
+      </c>
+      <c r="C159" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="D159" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E159" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="F159" s="21" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A160" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B160" s="26">
+        <v>42625</v>
+      </c>
+      <c r="C160" s="22" t="s">
+        <v>241</v>
+      </c>
+      <c r="D160" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E160" s="24" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A161" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B161" s="26">
+        <v>42625</v>
+      </c>
+      <c r="C161" s="22" t="s">
+        <v>215</v>
+      </c>
+      <c r="D161" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="E161" s="24" t="s">
+        <v>192</v>
+      </c>
+      <c r="F161" s="25" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A162" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B162" s="26">
+        <v>42625</v>
+      </c>
+      <c r="C162" s="22" t="s">
+        <v>215</v>
+      </c>
+      <c r="D162" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E162" s="24" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A163" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B163" s="26">
+        <v>42625</v>
+      </c>
+      <c r="C163" s="22" t="s">
+        <v>215</v>
+      </c>
+      <c r="D163" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E163" s="24" t="s">
+        <v>239</v>
+      </c>
+      <c r="F163" s="25" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A164" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B164" s="26">
+        <v>42625</v>
+      </c>
+      <c r="C164" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="D164" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E164" s="24" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A165" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B165" s="26">
+        <v>42625</v>
+      </c>
+      <c r="C165" s="22" t="s">
+        <v>189</v>
+      </c>
+      <c r="D165" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E165" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="F165" s="25" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A166" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="B166" s="26">
+        <v>42625</v>
+      </c>
+      <c r="C166" s="22" t="s">
+        <v>244</v>
+      </c>
+      <c r="D166" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="E166" s="24" t="s">
+        <v>242</v>
+      </c>
+      <c r="F166" s="25" t="s">
+        <v>243</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added "Modified time" to the first message alert. and working on closing all instances of EXCEL correctly.
</commit_message>
<xml_diff>
--- a/CLASSOPS/Derek/Derek's Log.xlsx
+++ b/CLASSOPS/Derek/Derek's Log.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="839" uniqueCount="251">
   <si>
     <t>Staff Name</t>
   </si>
@@ -820,6 +820,24 @@
   </si>
   <si>
     <t>2150</t>
+  </si>
+  <si>
+    <t>Luiz Marcio Cysneiros</t>
+  </si>
+  <si>
+    <t>Stephen Chen</t>
+  </si>
+  <si>
+    <t>107</t>
+  </si>
+  <si>
+    <t>Vitaly Kiryushcenko</t>
+  </si>
+  <si>
+    <t>Younes Benslimane</t>
+  </si>
+  <si>
+    <t>1545</t>
   </si>
 </sst>
 </file>
@@ -1352,11 +1370,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I166"/>
+  <dimension ref="A1:I176"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G166" sqref="G166"/>
+      <pane ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F179" sqref="F179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4391,6 +4409,189 @@
       </c>
       <c r="F166" s="25" t="s">
         <v>243</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A167" s="11"/>
+      <c r="B167" s="28"/>
+      <c r="C167" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="D167" s="11"/>
+      <c r="E167" s="32"/>
+      <c r="F167" s="34"/>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A168" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B168" s="26">
+        <v>42626</v>
+      </c>
+      <c r="C168" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="D168" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="E168" s="24" t="s">
+        <v>218</v>
+      </c>
+      <c r="F168" s="25" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A169" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B169" s="26">
+        <v>42626</v>
+      </c>
+      <c r="C169" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="D169" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E169" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="F169" s="21"/>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A170" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B170" s="26">
+        <v>42626</v>
+      </c>
+      <c r="C170" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="D170" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E170" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="F170" s="21" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A171" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B171" s="26">
+        <v>42626</v>
+      </c>
+      <c r="C171" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="D171" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E171" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="F171" s="21"/>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A172" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B172" s="26">
+        <v>42626</v>
+      </c>
+      <c r="C172" s="22" t="s">
+        <v>241</v>
+      </c>
+      <c r="D172" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E172" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="F172" s="25" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A173" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B173" s="26">
+        <v>42626</v>
+      </c>
+      <c r="C173" s="22" t="s">
+        <v>215</v>
+      </c>
+      <c r="D173" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="E173" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="F173" s="25" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A174" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B174" s="26">
+        <v>42626</v>
+      </c>
+      <c r="C174" s="22" t="s">
+        <v>215</v>
+      </c>
+      <c r="D174" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="E174" s="24" t="s">
+        <v>247</v>
+      </c>
+      <c r="F174" s="25" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A175" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B175" s="26">
+        <v>42626</v>
+      </c>
+      <c r="C175" s="22" t="s">
+        <v>215</v>
+      </c>
+      <c r="D175" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="E175" s="24" t="s">
+        <v>218</v>
+      </c>
+      <c r="F175" s="25" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A176" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B176" s="26">
+        <v>42626</v>
+      </c>
+      <c r="C176" s="22" t="s">
+        <v>250</v>
+      </c>
+      <c r="D176" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="E176" s="24" t="s">
+        <v>214</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update files and test, reset permissions. Need to build and install
</commit_message>
<xml_diff>
--- a/CLASSOPS/Derek/Derek's Log.xlsx
+++ b/CLASSOPS/Derek/Derek's Log.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="959" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="273">
   <si>
     <t>Staff Name</t>
   </si>
@@ -1436,11 +1436,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I203"/>
+  <dimension ref="A1:I206"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A173" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E208" sqref="E208:F208"/>
+      <pane ySplit="1" topLeftCell="A182" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C206" sqref="C206"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5156,7 +5156,7 @@
         <v>42628</v>
       </c>
       <c r="C203" s="22" t="s">
-        <v>227</v>
+        <v>244</v>
       </c>
       <c r="D203" s="23" t="s">
         <v>59</v>
@@ -5166,6 +5166,56 @@
       </c>
       <c r="F203" s="25" t="s">
         <v>272</v>
+      </c>
+    </row>
+    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A204" s="11"/>
+      <c r="B204" s="11"/>
+      <c r="C204" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="D204" s="13"/>
+      <c r="E204" s="11"/>
+      <c r="F204" s="13"/>
+      <c r="G204" s="14"/>
+      <c r="H204" s="11"/>
+      <c r="I204" s="11"/>
+    </row>
+    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A205" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B205" s="26">
+        <v>42629</v>
+      </c>
+      <c r="C205" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="D205" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E205" s="24" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A206" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B206" s="26">
+        <v>42629</v>
+      </c>
+      <c r="C206" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="D206" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E206" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="F206" s="21" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -5175,13 +5225,13 @@
     <sortCondition ref="D427:D515"/>
   </sortState>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A22:A23 B6 B2 A7:A8 B9 A10:A16 B17 A18:A20 B21 A3:A5 B24 A25:A27 B28 B32 A29:A31 A33:A34 B35 A36:A37 B38 A39:A53 B54 A55:A57 B58 A59:A63 B64 A65:A80 B81 A82:A85 B86 A87:A104 B105 A106:A109 B110 A111:A120 B121 A122:A133 B134 A135:A145 B146 A147:A176 B177 A178:A195 B196 A197:A199 A200:A1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A22:A23 B6 B2 A7:A8 B9 A10:A16 B17 A18:A20 B21 A3:A5 B24 A25:A27 B28 B32 A29:A31 A33:A34 B35 A36:A37 B38 A39:A53 B54 A55:A57 B58 A59:A63 B64 A65:A80 B81 A82:A85 B86 A87:A104 B105 A106:A109 B110 A111:A120 B121 A122:A133 B134 A135:A145 B146 A147:A176 B177 A178:A195 B196 A197:A203 B204 A205:A1048576">
       <formula1>Task_type</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6 E2 D22:D23 D7:D8 E9 D10:D16 E17 D18:D20 E21 D3:D5 E24 D25:D27 E28 E32 D29:D31 D33:D34 E35 D36:D37 E38 D39:D53 E54 D55:D57 E58 D59:D63 E64 D65:D80 E81 D82:D85 E86 D87:D104 E105 D106:D109 E110 D111:D120 E121 D122:D133 E134 D135:D145 E146 D147:D176 E177 D178:D195 E196 D197:D199 D200:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6 E2 D22:D23 D7:D8 E9 D10:D16 E17 D18:D20 E21 D3:D5 E24 D25:D27 E28 E32 D29:D31 D33:D34 E35 D36:D37 E38 D39:D53 E54 D55:D57 E58 D59:D63 E64 D65:D80 E81 D82:D85 E86 D87:D104 E105 D106:D109 E110 D111:D120 E121 D122:D133 E134 D135:D145 E146 D147:D176 E177 D178:D195 E196 D197:D203 E204 D205:D1048576">
       <formula1>Building</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 A2 A9 A17 A21 A24 A28 A32 A35 A38 A54 A58 A64 A81 A86 A105 A110 A121 A134 A146 A177 A196">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 A2 A9 A17 A21 A24 A28 A32 A35 A38 A54 A58 A64 A81 A86 A105 A110 A121 A134 A146 A177 A196 A204">
       <formula1>Staff_Name</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Tweak to the ranking algo to better sort and distribute the events in a log.
</commit_message>
<xml_diff>
--- a/CLASSOPS/Derek/Derek's Log.xlsx
+++ b/CLASSOPS/Derek/Derek's Log.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="276">
   <si>
     <t>Staff Name</t>
   </si>
@@ -904,6 +904,15 @@
   </si>
   <si>
     <t>Nat Taylor Cinema. Lock all cinema doors after shutdown.</t>
+  </si>
+  <si>
+    <t>221</t>
+  </si>
+  <si>
+    <t>110</t>
+  </si>
+  <si>
+    <t>Jennifer Hilborn</t>
   </si>
 </sst>
 </file>
@@ -1436,11 +1445,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I206"/>
+  <dimension ref="A1:I219"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A182" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C206" sqref="C206"/>
+      <pane ySplit="1" topLeftCell="A200" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C227" sqref="C227"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5215,6 +5224,238 @@
         <v>128</v>
       </c>
       <c r="F206" s="21" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A207" s="11"/>
+      <c r="B207" s="28"/>
+      <c r="C207" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="D207" s="11"/>
+      <c r="E207" s="32"/>
+      <c r="F207" s="34"/>
+    </row>
+    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A208" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B208" s="26">
+        <v>42632</v>
+      </c>
+      <c r="C208" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="D208" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="E208" s="24" t="s">
+        <v>182</v>
+      </c>
+      <c r="F208" s="25" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A209" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="B209" s="26">
+        <v>42632</v>
+      </c>
+      <c r="C209" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="D209" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="E209" s="24" t="s">
+        <v>273</v>
+      </c>
+      <c r="F209" s="25" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A210" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B210" s="26">
+        <v>42632</v>
+      </c>
+      <c r="C210" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="D210" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E210" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="F210" s="21" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A211" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B211" s="26">
+        <v>42632</v>
+      </c>
+      <c r="C211" s="22" t="s">
+        <v>241</v>
+      </c>
+      <c r="D211" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E211" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="F211" s="21"/>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A212" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B212" s="26">
+        <v>42632</v>
+      </c>
+      <c r="C212" s="22" t="s">
+        <v>215</v>
+      </c>
+      <c r="D212" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="E212" s="24" t="s">
+        <v>274</v>
+      </c>
+      <c r="F212" s="25" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A213" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B213" s="26">
+        <v>42632</v>
+      </c>
+      <c r="C213" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="D213" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E213" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="F213" s="21"/>
+    </row>
+    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A214" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B214" s="26">
+        <v>42632</v>
+      </c>
+      <c r="C214" s="22" t="s">
+        <v>189</v>
+      </c>
+      <c r="D214" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E214" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="F214" s="25" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A215" s="11"/>
+      <c r="B215" s="28"/>
+      <c r="C215" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="D215" s="11"/>
+      <c r="E215" s="32"/>
+      <c r="F215" s="34"/>
+    </row>
+    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A216" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B216" s="26">
+        <v>42633</v>
+      </c>
+      <c r="C216" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="D216" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E216" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="F216" s="21"/>
+    </row>
+    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A217" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B217" s="26">
+        <v>42633</v>
+      </c>
+      <c r="C217" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="D217" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E217" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="F217" s="21"/>
+    </row>
+    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A218" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B218" s="26">
+        <v>42633</v>
+      </c>
+      <c r="C218" s="22" t="s">
+        <v>241</v>
+      </c>
+      <c r="D218" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E218" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="F218" s="25" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A219" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B219" s="26">
+        <v>42633</v>
+      </c>
+      <c r="C219" s="22" t="s">
+        <v>226</v>
+      </c>
+      <c r="D219" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E219" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="F219" s="21" t="s">
         <v>129</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Implementation of the "Save Setting" feature. Allowing users to save setting for future sessions.
</commit_message>
<xml_diff>
--- a/CLASSOPS/Derek/Derek's Log.xlsx
+++ b/CLASSOPS/Derek/Derek's Log.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1056" uniqueCount="280">
   <si>
     <t>Staff Name</t>
   </si>
@@ -913,6 +913,18 @@
   </si>
   <si>
     <t>Jennifer Hilborn</t>
+  </si>
+  <si>
+    <t>1016</t>
+  </si>
+  <si>
+    <t>Return web cam, tripod and extension USB cable to Vari 1019.</t>
+  </si>
+  <si>
+    <t>305</t>
+  </si>
+  <si>
+    <t>Equipment is there 24/7.  Turn on for client.  Key in FC 164.</t>
   </si>
 </sst>
 </file>
@@ -1445,11 +1457,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I219"/>
+  <dimension ref="A1:I227"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A200" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C227" sqref="C227"/>
+      <pane ySplit="1" topLeftCell="A196" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B230" sqref="B230"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4150,7 +4162,7 @@
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" s="15" t="s">
-        <v>80</v>
+        <v>19</v>
       </c>
       <c r="B149" s="26">
         <v>42622</v>
@@ -4337,7 +4349,7 @@
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159" s="15" t="s">
-        <v>80</v>
+        <v>19</v>
       </c>
       <c r="B159" s="26">
         <v>42625</v>
@@ -4536,7 +4548,7 @@
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170" s="15" t="s">
-        <v>80</v>
+        <v>19</v>
       </c>
       <c r="B170" s="26">
         <v>42626</v>
@@ -4821,7 +4833,7 @@
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A185" s="15" t="s">
-        <v>80</v>
+        <v>19</v>
       </c>
       <c r="B185" s="26">
         <v>42627</v>
@@ -5139,7 +5151,7 @@
     </row>
     <row r="202" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A202" s="15" t="s">
-        <v>80</v>
+        <v>19</v>
       </c>
       <c r="B202" s="26">
         <v>42628</v>
@@ -5257,7 +5269,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A209" s="15" t="s">
         <v>87</v>
       </c>
@@ -5277,9 +5289,9 @@
         <v>179</v>
       </c>
     </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A210" s="15" t="s">
-        <v>80</v>
+        <v>19</v>
       </c>
       <c r="B210" s="26">
         <v>42632</v>
@@ -5297,7 +5309,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A211" s="15" t="s">
         <v>80</v>
       </c>
@@ -5315,7 +5327,7 @@
       </c>
       <c r="F211" s="21"/>
     </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A212" s="15" t="s">
         <v>12</v>
       </c>
@@ -5335,7 +5347,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A213" s="15" t="s">
         <v>80</v>
       </c>
@@ -5353,7 +5365,7 @@
       </c>
       <c r="F213" s="21"/>
     </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A214" s="15" t="s">
         <v>80</v>
       </c>
@@ -5373,7 +5385,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A215" s="11"/>
       <c r="B215" s="28"/>
       <c r="C215" s="13" t="s">
@@ -5383,7 +5395,7 @@
       <c r="E215" s="32"/>
       <c r="F215" s="34"/>
     </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A216" s="15" t="s">
         <v>80</v>
       </c>
@@ -5401,7 +5413,7 @@
       </c>
       <c r="F216" s="21"/>
     </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A217" s="15" t="s">
         <v>80</v>
       </c>
@@ -5419,7 +5431,7 @@
       </c>
       <c r="F217" s="21"/>
     </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A218" s="15" t="s">
         <v>80</v>
       </c>
@@ -5439,9 +5451,9 @@
         <v>206</v>
       </c>
     </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A219" s="15" t="s">
-        <v>80</v>
+        <v>19</v>
       </c>
       <c r="B219" s="26">
         <v>42633</v>
@@ -5457,6 +5469,155 @@
       </c>
       <c r="F219" s="21" t="s">
         <v>129</v>
+      </c>
+    </row>
+    <row r="220" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A220" s="11"/>
+      <c r="B220" s="11"/>
+      <c r="C220" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="D220" s="13"/>
+      <c r="E220" s="11"/>
+      <c r="F220" s="13"/>
+      <c r="G220" s="14"/>
+      <c r="H220" s="11"/>
+      <c r="I220" s="11"/>
+    </row>
+    <row r="221" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A221" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="B221" s="26">
+        <v>42634</v>
+      </c>
+      <c r="C221" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="D221" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="E221" s="24" t="s">
+        <v>278</v>
+      </c>
+      <c r="F221" s="25" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="222" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A222" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="B222" s="26">
+        <v>42634</v>
+      </c>
+      <c r="C222" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="D222" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="E222" s="24" t="s">
+        <v>276</v>
+      </c>
+      <c r="F222" s="25" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="223" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A223" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B223" s="26">
+        <v>42634</v>
+      </c>
+      <c r="C223" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="D223" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E223" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="F223" s="21" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="224" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A224" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B224" s="26">
+        <v>42634</v>
+      </c>
+      <c r="C224" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="D224" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E224" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="F224" s="21"/>
+    </row>
+    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A225" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B225" s="26">
+        <v>42634</v>
+      </c>
+      <c r="C225" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="D225" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E225" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="F225" s="25" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A226" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B226" s="26">
+        <v>42634</v>
+      </c>
+      <c r="C226" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="D226" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E226" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="F226" s="21"/>
+    </row>
+    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A227" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B227" s="26">
+        <v>42634</v>
+      </c>
+      <c r="C227" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="D227" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="E227" s="24" t="s">
+        <v>278</v>
+      </c>
+      <c r="F227" s="25" t="s">
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -5466,13 +5627,13 @@
     <sortCondition ref="D427:D515"/>
   </sortState>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A22:A23 B6 B2 A7:A8 B9 A10:A16 B17 A18:A20 B21 A3:A5 B24 A25:A27 B28 B32 A29:A31 A33:A34 B35 A36:A37 B38 A39:A53 B54 A55:A57 B58 A59:A63 B64 A65:A80 B81 A82:A85 B86 A87:A104 B105 A106:A109 B110 A111:A120 B121 A122:A133 B134 A135:A145 B146 A147:A176 B177 A178:A195 B196 A197:A203 B204 A205:A1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A22:A23 B6 B2 A7:A8 B9 A10:A16 B17 A18:A20 B21 A3:A5 B24 A25:A27 B28 B32 A29:A31 A33:A34 B35 A36:A37 B38 A39:A53 B54 A55:A57 B58 A59:A63 B64 A65:A80 B81 A82:A85 B86 A87:A104 B105 A106:A109 B110 A111:A120 B121 A122:A133 B134 A135:A145 B146 A147:A176 B177 A178:A195 B196 A197:A203 B204 A205:A219 B220 A221:A1048576">
       <formula1>Task_type</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6 E2 D22:D23 D7:D8 E9 D10:D16 E17 D18:D20 E21 D3:D5 E24 D25:D27 E28 E32 D29:D31 D33:D34 E35 D36:D37 E38 D39:D53 E54 D55:D57 E58 D59:D63 E64 D65:D80 E81 D82:D85 E86 D87:D104 E105 D106:D109 E110 D111:D120 E121 D122:D133 E134 D135:D145 E146 D147:D176 E177 D178:D195 E196 D197:D203 E204 D205:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6 E2 D22:D23 D7:D8 E9 D10:D16 E17 D18:D20 E21 D3:D5 E24 D25:D27 E28 E32 D29:D31 D33:D34 E35 D36:D37 E38 D39:D53 E54 D55:D57 E58 D59:D63 E64 D65:D80 E81 D82:D85 E86 D87:D104 E105 D106:D109 E110 D111:D120 E121 D122:D133 E134 D135:D145 E146 D147:D176 E177 D178:D195 E196 D197:D203 E204 D205:D219 E220 D221:D1048576">
       <formula1>Building</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 A2 A9 A17 A21 A24 A28 A32 A35 A38 A54 A58 A64 A81 A86 A105 A110 A121 A134 A146 A177 A196 A204">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 A2 A9 A17 A21 A24 A28 A32 A35 A38 A54 A58 A64 A81 A86 A105 A110 A121 A134 A146 A177 A196 A204 A220">
       <formula1>Staff_Name</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Comment modifications, file changes, and other minor bug fixes.
</commit_message>
<xml_diff>
--- a/CLASSOPS/Derek/Derek's Log.xlsx
+++ b/CLASSOPS/Derek/Derek's Log.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1056" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1143" uniqueCount="292">
   <si>
     <t>Staff Name</t>
   </si>
@@ -925,6 +925,42 @@
   </si>
   <si>
     <t>Equipment is there 24/7.  Turn on for client.  Key in FC 164.</t>
+  </si>
+  <si>
+    <t>101A</t>
+  </si>
+  <si>
+    <t>Pickup Adesso wireless keyboard and Samsung remote to FDRS 164.</t>
+  </si>
+  <si>
+    <t>Lec mic, stand, cables etc. to Vanier 040.23</t>
+  </si>
+  <si>
+    <t>Second demo.</t>
+  </si>
+  <si>
+    <t>Door code 7083* Screen there already. From FDRS 156A</t>
+  </si>
+  <si>
+    <t>1715</t>
+  </si>
+  <si>
+    <t>Web cam is in FDRS 164 storeroom. Demo to Roopa.</t>
+  </si>
+  <si>
+    <t>Neck mic, small PA. from FDRS 156A.</t>
+  </si>
+  <si>
+    <t>Return web cam and tripod to FDRS 164.</t>
+  </si>
+  <si>
+    <t>1750</t>
+  </si>
+  <si>
+    <t>111</t>
+  </si>
+  <si>
+    <t>Wendy Brathwaite</t>
   </si>
 </sst>
 </file>
@@ -1457,11 +1493,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I227"/>
+  <dimension ref="A1:I246"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A196" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B230" sqref="B230"/>
+      <pane ySplit="1" topLeftCell="A217" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A246" sqref="A246"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5562,7 +5598,7 @@
       </c>
       <c r="F224" s="21"/>
     </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A225" s="15" t="s">
         <v>80</v>
       </c>
@@ -5582,7 +5618,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A226" s="15" t="s">
         <v>80</v>
       </c>
@@ -5600,7 +5636,7 @@
       </c>
       <c r="F226" s="21"/>
     </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A227" s="15" t="s">
         <v>80</v>
       </c>
@@ -5618,6 +5654,369 @@
       </c>
       <c r="F227" s="25" t="s">
         <v>157</v>
+      </c>
+    </row>
+    <row r="228" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A228" s="11"/>
+      <c r="B228" s="11"/>
+      <c r="C228" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="D228" s="13"/>
+      <c r="E228" s="11"/>
+      <c r="F228" s="13"/>
+      <c r="G228" s="14"/>
+      <c r="H228" s="11"/>
+      <c r="I228" s="11"/>
+    </row>
+    <row r="229" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A229" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B229" s="26">
+        <v>42635</v>
+      </c>
+      <c r="C229" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="D229" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E229" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="F229" s="21"/>
+    </row>
+    <row r="230" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A230" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B230" s="26">
+        <v>42635</v>
+      </c>
+      <c r="C230" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="D230" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="E230" s="24" t="s">
+        <v>278</v>
+      </c>
+      <c r="F230" s="25" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="231" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A231" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B231" s="26">
+        <v>42635</v>
+      </c>
+      <c r="C231" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="D231" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="E231" s="24" t="s">
+        <v>280</v>
+      </c>
+      <c r="F231" s="25" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="232" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A232" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="B232" s="26">
+        <v>42635</v>
+      </c>
+      <c r="C232" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="D232" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="E232" s="24" t="s">
+        <v>174</v>
+      </c>
+      <c r="F232" s="25" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="233" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A233" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="B233" s="26">
+        <v>42635</v>
+      </c>
+      <c r="C233" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="D233" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="E233" s="24" t="s">
+        <v>174</v>
+      </c>
+      <c r="F233" s="25" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="234" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A234" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B234" s="26">
+        <v>42635</v>
+      </c>
+      <c r="C234" s="22" t="s">
+        <v>270</v>
+      </c>
+      <c r="D234" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="E234" s="24" t="s">
+        <v>271</v>
+      </c>
+      <c r="F234" s="25" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="235" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A235" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="B235" s="26">
+        <v>42635</v>
+      </c>
+      <c r="C235" s="22" t="s">
+        <v>187</v>
+      </c>
+      <c r="D235" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="E235" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="F235" s="25" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="236" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A236" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="B236" s="26">
+        <v>42635</v>
+      </c>
+      <c r="C236" s="22" t="s">
+        <v>187</v>
+      </c>
+      <c r="D236" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="E236" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="F236" s="25" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="237" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A237" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B237" s="26">
+        <v>42635</v>
+      </c>
+      <c r="C237" s="22" t="s">
+        <v>187</v>
+      </c>
+      <c r="D237" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="E237" s="24" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="238" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A238" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B238" s="26">
+        <v>42635</v>
+      </c>
+      <c r="C238" s="22" t="s">
+        <v>285</v>
+      </c>
+      <c r="D238" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="E238" s="24" t="s">
+        <v>164</v>
+      </c>
+      <c r="F238" s="25" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="239" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A239" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B239" s="26">
+        <v>42635</v>
+      </c>
+      <c r="C239" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="D239" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E239" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="F239" s="21"/>
+    </row>
+    <row r="240" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A240" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B240" s="26">
+        <v>42635</v>
+      </c>
+      <c r="C240" s="22" t="s">
+        <v>289</v>
+      </c>
+      <c r="D240" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="E240" s="24" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A241" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B241" s="26">
+        <v>42635</v>
+      </c>
+      <c r="C241" s="22" t="s">
+        <v>215</v>
+      </c>
+      <c r="D241" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="E241" s="24" t="s">
+        <v>218</v>
+      </c>
+      <c r="F241" s="25" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A242" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="B242" s="26">
+        <v>42635</v>
+      </c>
+      <c r="C242" s="22" t="s">
+        <v>226</v>
+      </c>
+      <c r="D242" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="E242" s="24" t="s">
+        <v>164</v>
+      </c>
+      <c r="F242" s="25" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A243" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B243" s="26">
+        <v>42635</v>
+      </c>
+      <c r="C243" s="22" t="s">
+        <v>226</v>
+      </c>
+      <c r="D243" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E243" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="F243" s="21" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="244" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A244" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="B244" s="26">
+        <v>42635</v>
+      </c>
+      <c r="C244" s="22" t="s">
+        <v>189</v>
+      </c>
+      <c r="D244" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="E244" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="F244" s="25" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="245" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A245" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="B245" s="26">
+        <v>42635</v>
+      </c>
+      <c r="C245" s="22" t="s">
+        <v>189</v>
+      </c>
+      <c r="D245" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="E245" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="F245" s="25" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A246" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B246" s="26">
+        <v>42635</v>
+      </c>
+      <c r="C246" s="22" t="s">
+        <v>227</v>
+      </c>
+      <c r="D246" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E246" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="F246" s="25" t="s">
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -5627,13 +6026,13 @@
     <sortCondition ref="D427:D515"/>
   </sortState>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A22:A23 B6 B2 A7:A8 B9 A10:A16 B17 A18:A20 B21 A3:A5 B24 A25:A27 B28 B32 A29:A31 A33:A34 B35 A36:A37 B38 A39:A53 B54 A55:A57 B58 A59:A63 B64 A65:A80 B81 A82:A85 B86 A87:A104 B105 A106:A109 B110 A111:A120 B121 A122:A133 B134 A135:A145 B146 A147:A176 B177 A178:A195 B196 A197:A203 B204 A205:A219 B220 A221:A1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A22:A23 B6 B2 A7:A8 B9 A10:A16 B17 A18:A20 B21 A3:A5 B24 A25:A27 B28 B32 A29:A31 A33:A34 B35 A36:A37 B38 A39:A53 B54 A55:A57 B58 A59:A63 B64 A65:A80 B81 A82:A85 B86 A87:A104 B105 A106:A109 B110 A111:A120 B121 A122:A133 B134 A135:A145 B146 A147:A176 B177 A178:A195 B196 A197:A203 B204 A205:A219 B220 A221:A227 B228 A229:A1048576">
       <formula1>Task_type</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6 E2 D22:D23 D7:D8 E9 D10:D16 E17 D18:D20 E21 D3:D5 E24 D25:D27 E28 E32 D29:D31 D33:D34 E35 D36:D37 E38 D39:D53 E54 D55:D57 E58 D59:D63 E64 D65:D80 E81 D82:D85 E86 D87:D104 E105 D106:D109 E110 D111:D120 E121 D122:D133 E134 D135:D145 E146 D147:D176 E177 D178:D195 E196 D197:D203 E204 D205:D219 E220 D221:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6 E2 D22:D23 D7:D8 E9 D10:D16 E17 D18:D20 E21 D3:D5 E24 D25:D27 E28 E32 D29:D31 D33:D34 E35 D36:D37 E38 D39:D53 E54 D55:D57 E58 D59:D63 E64 D65:D80 E81 D82:D85 E86 D87:D104 E105 D106:D109 E110 D111:D120 E121 D122:D133 E134 D135:D145 E146 D147:D176 E177 D178:D195 E196 D197:D203 E204 D205:D219 E220 D221:D227 E228 D229:D1048576">
       <formula1>Building</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 A2 A9 A17 A21 A24 A28 A32 A35 A38 A54 A58 A64 A81 A86 A105 A110 A121 A134 A146 A177 A196 A204 A220">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 A2 A9 A17 A21 A24 A28 A32 A35 A38 A54 A58 A64 A81 A86 A105 A110 A121 A134 A146 A177 A196 A204 A220 A228">
       <formula1>Staff_Name</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Update the files and started working on the detail window
</commit_message>
<xml_diff>
--- a/CLASSOPS/Derek/Derek's Log.xlsx
+++ b/CLASSOPS/Derek/Derek's Log.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1143" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1192" uniqueCount="295">
   <si>
     <t>Staff Name</t>
   </si>
@@ -961,6 +961,15 @@
   </si>
   <si>
     <t>Wendy Brathwaite</t>
+  </si>
+  <si>
+    <t>1018</t>
+  </si>
+  <si>
+    <t>Flat screen TV, wireless ethernet and wireless keyboard. Turn off wireless keyboard before placing in carry-all bag. To Vari 1019 across the hall.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pick up Keyboard and remote for the DLP TV. Return to FC 164. </t>
   </si>
 </sst>
 </file>
@@ -1493,11 +1502,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I246"/>
+  <dimension ref="A1:I258"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A217" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A246" sqref="A246"/>
+      <pane ySplit="1" topLeftCell="A241" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E259" sqref="E259"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5257,7 +5266,7 @@
     </row>
     <row r="206" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A206" s="15" t="s">
-        <v>80</v>
+        <v>19</v>
       </c>
       <c r="B206" s="26">
         <v>42629</v>
@@ -5899,7 +5908,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A241" s="15" t="s">
         <v>12</v>
       </c>
@@ -5919,7 +5928,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A242" s="15" t="s">
         <v>93</v>
       </c>
@@ -5939,7 +5948,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A243" s="15" t="s">
         <v>19</v>
       </c>
@@ -5959,7 +5968,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="244" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A244" s="15" t="s">
         <v>91</v>
       </c>
@@ -5979,7 +5988,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="245" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A245" s="15" t="s">
         <v>87</v>
       </c>
@@ -5999,7 +6008,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A246" s="15" t="s">
         <v>80</v>
       </c>
@@ -6017,6 +6026,222 @@
       </c>
       <c r="F246" s="25" t="s">
         <v>206</v>
+      </c>
+    </row>
+    <row r="247" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A247" s="11"/>
+      <c r="B247" s="11"/>
+      <c r="C247" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="D247" s="13"/>
+      <c r="E247" s="11"/>
+      <c r="F247" s="13"/>
+      <c r="G247" s="14"/>
+      <c r="H247" s="11"/>
+      <c r="I247" s="11"/>
+    </row>
+    <row r="248" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A248" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B248" s="26">
+        <v>42636</v>
+      </c>
+      <c r="C248" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="D248" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E248" s="24" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="249" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A249" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B249" s="26">
+        <v>42636</v>
+      </c>
+      <c r="C249" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="D249" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E249" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="F249" s="21" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="250" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A250" s="11"/>
+      <c r="B250" s="28"/>
+      <c r="C250" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="D250" s="11"/>
+      <c r="E250" s="32"/>
+      <c r="F250" s="34"/>
+    </row>
+    <row r="251" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A251" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B251" s="26">
+        <v>42639</v>
+      </c>
+      <c r="C251" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="D251" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="E251" s="24" t="s">
+        <v>182</v>
+      </c>
+      <c r="F251" s="25" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="252" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A252" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="B252" s="26">
+        <v>42639</v>
+      </c>
+      <c r="C252" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="D252" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="E252" s="24" t="s">
+        <v>180</v>
+      </c>
+      <c r="F252" s="25" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="253" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A253" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B253" s="26">
+        <v>42639</v>
+      </c>
+      <c r="C253" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="D253" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E253" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="F253" s="21" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="254" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A254" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B254" s="26">
+        <v>42639</v>
+      </c>
+      <c r="C254" s="22" t="s">
+        <v>241</v>
+      </c>
+      <c r="D254" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E254" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="F254" s="21"/>
+    </row>
+    <row r="255" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A255" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B255" s="26">
+        <v>42639</v>
+      </c>
+      <c r="C255" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="D255" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E255" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="F255" s="21"/>
+    </row>
+    <row r="256" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A256" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B256" s="26">
+        <v>42639</v>
+      </c>
+      <c r="C256" s="22" t="s">
+        <v>189</v>
+      </c>
+      <c r="D256" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E256" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="F256" s="25" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="257" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A257" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="B257" s="26">
+        <v>42639</v>
+      </c>
+      <c r="C257" s="22" t="s">
+        <v>244</v>
+      </c>
+      <c r="D257" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="E257" s="24" t="s">
+        <v>292</v>
+      </c>
+      <c r="F257" s="25" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="258" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A258" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B258" s="26">
+        <v>42639</v>
+      </c>
+      <c r="C258" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="D258" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="E258" s="24" t="s">
+        <v>280</v>
+      </c>
+      <c r="F258" s="25" t="s">
+        <v>294</v>
       </c>
     </row>
   </sheetData>
@@ -6026,13 +6251,13 @@
     <sortCondition ref="D427:D515"/>
   </sortState>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A22:A23 B6 B2 A7:A8 B9 A10:A16 B17 A18:A20 B21 A3:A5 B24 A25:A27 B28 B32 A29:A31 A33:A34 B35 A36:A37 B38 A39:A53 B54 A55:A57 B58 A59:A63 B64 A65:A80 B81 A82:A85 B86 A87:A104 B105 A106:A109 B110 A111:A120 B121 A122:A133 B134 A135:A145 B146 A147:A176 B177 A178:A195 B196 A197:A203 B204 A205:A219 B220 A221:A227 B228 A229:A1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A22:A23 B6 B2 A7:A8 B9 A10:A16 B17 A18:A20 B21 A3:A5 B24 A25:A27 B28 B32 A29:A31 A33:A34 B35 A36:A37 B38 A39:A53 B54 A55:A57 B58 A59:A63 B64 A65:A80 B81 A82:A85 B86 A87:A104 B105 A106:A109 B110 A111:A120 B121 A122:A133 B134 A135:A145 B146 A147:A176 B177 A178:A195 B196 A197:A203 B204 A205:A219 B220 A221:A227 B228 A229:A246 B247 A248:A1048576">
       <formula1>Task_type</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6 E2 D22:D23 D7:D8 E9 D10:D16 E17 D18:D20 E21 D3:D5 E24 D25:D27 E28 E32 D29:D31 D33:D34 E35 D36:D37 E38 D39:D53 E54 D55:D57 E58 D59:D63 E64 D65:D80 E81 D82:D85 E86 D87:D104 E105 D106:D109 E110 D111:D120 E121 D122:D133 E134 D135:D145 E146 D147:D176 E177 D178:D195 E196 D197:D203 E204 D205:D219 E220 D221:D227 E228 D229:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6 E2 D22:D23 D7:D8 E9 D10:D16 E17 D18:D20 E21 D3:D5 E24 D25:D27 E28 E32 D29:D31 D33:D34 E35 D36:D37 E38 D39:D53 E54 D55:D57 E58 D59:D63 E64 D65:D80 E81 D82:D85 E86 D87:D104 E105 D106:D109 E110 D111:D120 E121 D122:D133 E134 D135:D145 E146 D147:D176 E177 D178:D195 E196 D197:D203 E204 D205:D219 E220 D221:D227 E228 D229:D246 E247 D248:D1048576">
       <formula1>Building</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 A2 A9 A17 A21 A24 A28 A32 A35 A38 A54 A58 A64 A81 A86 A105 A110 A121 A134 A146 A177 A196 A204 A220 A228">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 A2 A9 A17 A21 A24 A28 A32 A35 A38 A54 A58 A64 A81 A86 A105 A110 A121 A134 A146 A177 A196 A204 A220 A228 A247">
       <formula1>Staff_Name</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
update files, finished the tasking distro algo, and working on detail window
</commit_message>
<xml_diff>
--- a/CLASSOPS/Derek/Derek's Log.xlsx
+++ b/CLASSOPS/Derek/Derek's Log.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1192" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1245" uniqueCount="297">
   <si>
     <t>Staff Name</t>
   </si>
@@ -970,6 +970,35 @@
   </si>
   <si>
     <t xml:space="preserve">Pick up Keyboard and remote for the DLP TV. Return to FC 164. </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Flat screen TV, wireless keyboard. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Turn off wireless keyboard before placing in carry-all bag</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. To Vari 1019 across the hall. Also includes an ethernet cable and an orange extension cord. </t>
+    </r>
+  </si>
+  <si>
+    <t>Help connect Windows Laptop for Antonella Valeo.  Bring VGA cable and connect her laptop to Input 2 on the projector. Select input 2 on projector.</t>
   </si>
 </sst>
 </file>
@@ -1502,11 +1531,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I258"/>
+  <dimension ref="A1:I271"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A241" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E259" sqref="E259"/>
+      <pane ySplit="1" topLeftCell="A256" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G278" sqref="G278"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6204,7 +6233,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="257" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A257" s="15" t="s">
         <v>87</v>
       </c>
@@ -6224,7 +6253,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="258" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A258" s="15" t="s">
         <v>19</v>
       </c>
@@ -6242,6 +6271,241 @@
       </c>
       <c r="F258" s="25" t="s">
         <v>294</v>
+      </c>
+    </row>
+    <row r="259" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A259" s="11"/>
+      <c r="B259" s="28"/>
+      <c r="C259" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="D259" s="11"/>
+      <c r="E259" s="32"/>
+      <c r="F259" s="34"/>
+    </row>
+    <row r="260" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A260" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B260" s="26">
+        <v>42640</v>
+      </c>
+      <c r="C260" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="D260" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E260" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="F260" s="21"/>
+    </row>
+    <row r="261" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A261" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B261" s="26">
+        <v>42640</v>
+      </c>
+      <c r="C261" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="D261" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E261" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="F261" s="21"/>
+    </row>
+    <row r="262" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A262" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B262" s="26">
+        <v>42640</v>
+      </c>
+      <c r="C262" s="22" t="s">
+        <v>226</v>
+      </c>
+      <c r="D262" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E262" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="F262" s="21" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="263" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A263" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="B263" s="26">
+        <v>42640</v>
+      </c>
+      <c r="C263" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="D263" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="E263" s="24" t="s">
+        <v>292</v>
+      </c>
+      <c r="F263" s="25" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="264" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A264" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B264" s="26">
+        <v>42640</v>
+      </c>
+      <c r="C264" s="22" t="s">
+        <v>244</v>
+      </c>
+      <c r="D264" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E264" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="F264" s="25" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="265" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A265" s="11"/>
+      <c r="B265" s="11"/>
+      <c r="C265" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="D265" s="13"/>
+      <c r="E265" s="11"/>
+      <c r="F265" s="13"/>
+      <c r="G265" s="14"/>
+      <c r="H265" s="11"/>
+      <c r="I265" s="11"/>
+    </row>
+    <row r="266" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A266" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="B266" s="26">
+        <v>42641</v>
+      </c>
+      <c r="C266" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="D266" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="E266" s="24" t="s">
+        <v>276</v>
+      </c>
+      <c r="F266" s="25" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="267" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A267" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B267" s="26">
+        <v>42634</v>
+      </c>
+      <c r="C267" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="D267" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E267" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="F267" s="21" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="268" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A268" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B268" s="26">
+        <v>42634</v>
+      </c>
+      <c r="C268" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="D268" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E268" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="F268" s="21"/>
+    </row>
+    <row r="269" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A269" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B269" s="26">
+        <v>42634</v>
+      </c>
+      <c r="C269" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="D269" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E269" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="F269" s="25" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="270" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A270" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B270" s="26">
+        <v>42634</v>
+      </c>
+      <c r="C270" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="D270" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E270" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="F270" s="21"/>
+    </row>
+    <row r="271" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A271" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B271" s="26">
+        <v>42641</v>
+      </c>
+      <c r="C271" s="22" t="s">
+        <v>215</v>
+      </c>
+      <c r="D271" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E271" s="24" t="s">
+        <v>260</v>
+      </c>
+      <c r="F271" s="25" t="s">
+        <v>296</v>
       </c>
     </row>
   </sheetData>
@@ -6251,13 +6515,13 @@
     <sortCondition ref="D427:D515"/>
   </sortState>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A22:A23 B6 B2 A7:A8 B9 A10:A16 B17 A18:A20 B21 A3:A5 B24 A25:A27 B28 B32 A29:A31 A33:A34 B35 A36:A37 B38 A39:A53 B54 A55:A57 B58 A59:A63 B64 A65:A80 B81 A82:A85 B86 A87:A104 B105 A106:A109 B110 A111:A120 B121 A122:A133 B134 A135:A145 B146 A147:A176 B177 A178:A195 B196 A197:A203 B204 A205:A219 B220 A221:A227 B228 A229:A246 B247 A248:A1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A22:A23 B6 B2 A7:A8 B9 A10:A16 B17 A18:A20 B21 A3:A5 B24 A25:A27 B28 B32 A29:A31 A33:A34 B35 A36:A37 B38 A39:A53 B54 A55:A57 B58 A59:A63 B64 A65:A80 B81 A82:A85 B86 A87:A104 B105 A106:A109 B110 A111:A120 B121 A122:A133 B134 A135:A145 B146 A147:A176 B177 A178:A195 B196 A197:A203 B204 A205:A219 B220 A221:A227 B228 A229:A246 B247 A248:A264 B265 A266:A1048576">
       <formula1>Task_type</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6 E2 D22:D23 D7:D8 E9 D10:D16 E17 D18:D20 E21 D3:D5 E24 D25:D27 E28 E32 D29:D31 D33:D34 E35 D36:D37 E38 D39:D53 E54 D55:D57 E58 D59:D63 E64 D65:D80 E81 D82:D85 E86 D87:D104 E105 D106:D109 E110 D111:D120 E121 D122:D133 E134 D135:D145 E146 D147:D176 E177 D178:D195 E196 D197:D203 E204 D205:D219 E220 D221:D227 E228 D229:D246 E247 D248:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6 E2 D22:D23 D7:D8 E9 D10:D16 E17 D18:D20 E21 D3:D5 E24 D25:D27 E28 E32 D29:D31 D33:D34 E35 D36:D37 E38 D39:D53 E54 D55:D57 E58 D59:D63 E64 D65:D80 E81 D82:D85 E86 D87:D104 E105 D106:D109 E110 D111:D120 E121 D122:D133 E134 D135:D145 E146 D147:D176 E177 D178:D195 E196 D197:D203 E204 D205:D219 E220 D221:D227 E228 D229:D246 E247 D248:D264 E265 D266:D1048576">
       <formula1>Building</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 A2 A9 A17 A21 A24 A28 A32 A35 A38 A54 A58 A64 A81 A86 A105 A110 A121 A134 A146 A177 A196 A204 A220 A228 A247">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 A2 A9 A17 A21 A24 A28 A32 A35 A38 A54 A58 A64 A81 A86 A105 A110 A121 A134 A146 A177 A196 A204 A220 A228 A247 A265">
       <formula1>Staff_Name</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Bug when removing MC
</commit_message>
<xml_diff>
--- a/CLASSOPS/Derek/Derek's Log.xlsx
+++ b/CLASSOPS/Derek/Derek's Log.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1245" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1323" uniqueCount="303">
   <si>
     <t>Staff Name</t>
   </si>
@@ -999,6 +999,24 @@
   </si>
   <si>
     <t>Help connect Windows Laptop for Antonella Valeo.  Bring VGA cable and connect her laptop to Input 2 on the projector. Select input 2 on projector.</t>
+  </si>
+  <si>
+    <t>202</t>
+  </si>
+  <si>
+    <t>Roll-in PC. Disconnect from laptop input and store in FDRS 156A.  VGA cable belongs in the drawer In the classroom.</t>
+  </si>
+  <si>
+    <t>S803</t>
+  </si>
+  <si>
+    <t>Connect Mac laptop for Poiffet. She has cables.</t>
+  </si>
+  <si>
+    <t>N145</t>
+  </si>
+  <si>
+    <t>Instructor has issues with the computer and projector.</t>
   </si>
 </sst>
 </file>
@@ -1139,7 +1157,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1224,6 +1242,15 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1531,11 +1558,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I271"/>
+  <dimension ref="A1:I290"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A256" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G278" sqref="G278"/>
+      <pane ySplit="1" topLeftCell="A270" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D295" sqref="D295"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6417,7 +6444,7 @@
         <v>19</v>
       </c>
       <c r="B267" s="26">
-        <v>42634</v>
+        <v>42641</v>
       </c>
       <c r="C267" s="22" t="s">
         <v>208</v>
@@ -6437,7 +6464,7 @@
         <v>80</v>
       </c>
       <c r="B268" s="26">
-        <v>42634</v>
+        <v>42641</v>
       </c>
       <c r="C268" s="22" t="s">
         <v>208</v>
@@ -6455,7 +6482,7 @@
         <v>80</v>
       </c>
       <c r="B269" s="26">
-        <v>42634</v>
+        <v>42641</v>
       </c>
       <c r="C269" s="22" t="s">
         <v>111</v>
@@ -6475,7 +6502,7 @@
         <v>80</v>
       </c>
       <c r="B270" s="26">
-        <v>42634</v>
+        <v>42641</v>
       </c>
       <c r="C270" s="22" t="s">
         <v>111</v>
@@ -6506,6 +6533,351 @@
       </c>
       <c r="F271" s="25" t="s">
         <v>296</v>
+      </c>
+    </row>
+    <row r="272" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A272" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="B272" s="26">
+        <v>42641</v>
+      </c>
+      <c r="C272" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="D272" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="E272" s="24" t="s">
+        <v>292</v>
+      </c>
+      <c r="F272" s="25" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="273" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A273" s="11"/>
+      <c r="B273" s="11"/>
+      <c r="C273" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="D273" s="13"/>
+      <c r="E273" s="11"/>
+      <c r="F273" s="13"/>
+      <c r="G273" s="14"/>
+      <c r="H273" s="11"/>
+      <c r="I273" s="11"/>
+    </row>
+    <row r="274" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A274" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B274" s="26">
+        <v>42642</v>
+      </c>
+      <c r="C274" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="D274" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E274" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="F274" s="21"/>
+    </row>
+    <row r="275" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A275" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B275" s="26">
+        <v>42642</v>
+      </c>
+      <c r="C275" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="D275" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="E275" s="24" t="s">
+        <v>278</v>
+      </c>
+      <c r="F275" s="25" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="276" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A276" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B276" s="26">
+        <v>42642</v>
+      </c>
+      <c r="C276" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="D276" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E276" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="F276" s="21"/>
+    </row>
+    <row r="277" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A277" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B277" s="26">
+        <v>42642</v>
+      </c>
+      <c r="C277" s="22" t="s">
+        <v>226</v>
+      </c>
+      <c r="D277" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E277" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="F277" s="21" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="278" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A278" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B278" s="26">
+        <v>42642</v>
+      </c>
+      <c r="C278" s="22" t="s">
+        <v>244</v>
+      </c>
+      <c r="D278" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E278" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="F278" s="25" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="279" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A279" s="11"/>
+      <c r="B279" s="11"/>
+      <c r="C279" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="D279" s="13"/>
+      <c r="E279" s="11"/>
+      <c r="F279" s="13"/>
+      <c r="G279" s="14"/>
+      <c r="H279" s="11"/>
+      <c r="I279" s="11"/>
+    </row>
+    <row r="280" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A280" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B280" s="26">
+        <v>42643</v>
+      </c>
+      <c r="C280" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="D280" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E280" s="24" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="281" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A281" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B281" s="26">
+        <v>42643</v>
+      </c>
+      <c r="C281" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="D281" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E281" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="F281" s="21" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="282" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A282" s="11"/>
+      <c r="B282" s="28"/>
+      <c r="C282" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="D282" s="11"/>
+      <c r="E282" s="32"/>
+      <c r="F282" s="34"/>
+    </row>
+    <row r="283" spans="1:9" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A283" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B283" s="26">
+        <v>42646</v>
+      </c>
+      <c r="C283" s="17" t="s">
+        <v>211</v>
+      </c>
+      <c r="D283" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E283" s="35" t="s">
+        <v>299</v>
+      </c>
+      <c r="F283" s="36" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="284" spans="1:9" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A284" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B284" s="26">
+        <v>42646</v>
+      </c>
+      <c r="C284" s="17" t="s">
+        <v>211</v>
+      </c>
+      <c r="D284" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E284" s="35" t="s">
+        <v>301</v>
+      </c>
+      <c r="F284" s="36" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="285" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A285" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B285" s="26">
+        <v>42646</v>
+      </c>
+      <c r="C285" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="D285" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="E285" s="24" t="s">
+        <v>182</v>
+      </c>
+      <c r="F285" s="25" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="286" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A286" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="B286" s="26">
+        <v>42646</v>
+      </c>
+      <c r="C286" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="D286" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="E286" s="24" t="s">
+        <v>297</v>
+      </c>
+      <c r="F286" s="25" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="287" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A287" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B287" s="26">
+        <v>42639</v>
+      </c>
+      <c r="C287" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="D287" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E287" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="F287" s="21" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="288" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A288" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B288" s="26">
+        <v>42639</v>
+      </c>
+      <c r="C288" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="D288" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E288" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="F288" s="21"/>
+    </row>
+    <row r="289" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A289" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B289" s="26">
+        <v>42639</v>
+      </c>
+      <c r="C289" s="22" t="s">
+        <v>241</v>
+      </c>
+      <c r="D289" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E289" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="F289" s="21"/>
+    </row>
+    <row r="290" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A290" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B290" s="26">
+        <v>42639</v>
+      </c>
+      <c r="C290" s="22" t="s">
+        <v>189</v>
+      </c>
+      <c r="D290" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E290" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="F290" s="25" t="s">
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -6515,13 +6887,13 @@
     <sortCondition ref="D427:D515"/>
   </sortState>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A22:A23 B6 B2 A7:A8 B9 A10:A16 B17 A18:A20 B21 A3:A5 B24 A25:A27 B28 B32 A29:A31 A33:A34 B35 A36:A37 B38 A39:A53 B54 A55:A57 B58 A59:A63 B64 A65:A80 B81 A82:A85 B86 A87:A104 B105 A106:A109 B110 A111:A120 B121 A122:A133 B134 A135:A145 B146 A147:A176 B177 A178:A195 B196 A197:A203 B204 A205:A219 B220 A221:A227 B228 A229:A246 B247 A248:A264 B265 A266:A1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A22:A23 B6 B2 A7:A8 B9 A10:A16 B17 A18:A20 B21 A3:A5 B24 A25:A27 B28 B32 A29:A31 A33:A34 B35 A36:A37 B38 A39:A53 B54 A55:A57 B58 A59:A63 B64 A65:A80 B81 A82:A85 B86 A87:A104 B105 A106:A109 B110 A111:A120 B121 A122:A133 B134 A135:A145 B146 A147:A176 B177 A178:A195 B196 A197:A203 B204 A205:A219 B220 A221:A227 B228 A229:A246 B247 A248:A264 B265 A266:A272 B273 A274:A278 B279 A280:A1048576">
       <formula1>Task_type</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6 E2 D22:D23 D7:D8 E9 D10:D16 E17 D18:D20 E21 D3:D5 E24 D25:D27 E28 E32 D29:D31 D33:D34 E35 D36:D37 E38 D39:D53 E54 D55:D57 E58 D59:D63 E64 D65:D80 E81 D82:D85 E86 D87:D104 E105 D106:D109 E110 D111:D120 E121 D122:D133 E134 D135:D145 E146 D147:D176 E177 D178:D195 E196 D197:D203 E204 D205:D219 E220 D221:D227 E228 D229:D246 E247 D248:D264 E265 D266:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6 E2 D22:D23 D7:D8 E9 D10:D16 E17 D18:D20 E21 D3:D5 E24 D25:D27 E28 E32 D29:D31 D33:D34 E35 D36:D37 E38 D39:D53 E54 D55:D57 E58 D59:D63 E64 D65:D80 E81 D82:D85 E86 D87:D104 E105 D106:D109 E110 D111:D120 E121 D122:D133 E134 D135:D145 E146 D147:D176 E177 D178:D195 E196 D197:D203 E204 D205:D219 E220 D221:D227 E228 D229:D246 E247 D248:D264 E265 D266:D272 E273 D274:D278 E279 D280:D1048576">
       <formula1>Building</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 A2 A9 A17 A21 A24 A28 A32 A35 A38 A54 A58 A64 A81 A86 A105 A110 A121 A134 A146 A177 A196 A204 A220 A228 A247 A265">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 A2 A9 A17 A21 A24 A28 A32 A35 A38 A54 A58 A64 A81 A86 A105 A110 A121 A134 A146 A177 A196 A204 A220 A228 A247 A265 A273 A279">
       <formula1>Staff_Name</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
File updates and tests
</commit_message>
<xml_diff>
--- a/CLASSOPS/Derek/Derek's Log.xlsx
+++ b/CLASSOPS/Derek/Derek's Log.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17127"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jhan\Documents\Visual Studio 2015\Projects\ClassOpsLogCreator\CLASSOPS\Derek\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="90" yWindow="150" windowWidth="14865" windowHeight="10785" tabRatio="440"/>
   </bookViews>
@@ -22,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1480" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1536" uniqueCount="346">
   <si>
     <t>Staff Name</t>
   </si>
@@ -1144,11 +1149,14 @@
   <si>
     <t>SCL</t>
   </si>
+  <si>
+    <t>Pick up roll in PC and Projector carts. Return to Vanier 040 basement storeroom. Key is in Founders 164 storeroom.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
@@ -1385,6 +1393,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1432,7 +1443,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1465,9 +1476,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1500,6 +1528,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1679,22 +1724,22 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I321"/>
+  <dimension ref="A1:I334"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A309" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A320" sqref="A320"/>
+      <pane ySplit="1" topLeftCell="A315" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B324" sqref="B324:B334"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="22.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" style="10" customWidth="1"/>
+    <col min="1" max="1" width="27.75" style="10" customWidth="1"/>
     <col min="2" max="2" width="19" style="21" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.375" style="17" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="18" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" style="19" customWidth="1"/>
-    <col min="6" max="6" width="60.42578125" style="20" customWidth="1"/>
-    <col min="7" max="16384" width="22.140625" style="2"/>
+    <col min="5" max="5" width="11.75" style="19" customWidth="1"/>
+    <col min="6" max="6" width="60.375" style="20" customWidth="1"/>
+    <col min="7" max="16384" width="22.125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -7561,7 +7606,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="321" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A321" s="10" t="s">
         <v>80</v>
       </c>
@@ -7575,6 +7620,241 @@
         <v>49</v>
       </c>
       <c r="E321" s="19" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="322" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A322" s="6"/>
+      <c r="B322" s="23"/>
+      <c r="C322" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="D322" s="6"/>
+      <c r="E322" s="27"/>
+      <c r="F322" s="29"/>
+    </row>
+    <row r="323" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A323" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B323" s="21">
+        <v>42652</v>
+      </c>
+      <c r="C323" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D323" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E323" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="324" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A324" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B324" s="21">
+        <v>42652</v>
+      </c>
+      <c r="C324" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D324" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E324" s="19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="325" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A325" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B325" s="21">
+        <v>42652</v>
+      </c>
+      <c r="C325" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D325" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E325" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="F325" s="16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="326" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A326" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B326" s="21">
+        <v>42652</v>
+      </c>
+      <c r="C326" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="D326" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E326" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="F326" s="20" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="327" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A327" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B327" s="21">
+        <v>42652</v>
+      </c>
+      <c r="C327" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D327" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E327" s="19" t="s">
+        <v>321</v>
+      </c>
+      <c r="F327" s="20" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="328" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A328" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B328" s="21">
+        <v>42652</v>
+      </c>
+      <c r="C328" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="D328" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E328" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="F328" s="20" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="329" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A329" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B329" s="21">
+        <v>42652</v>
+      </c>
+      <c r="C329" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D329" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E329" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F329" s="20" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="330" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A330" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B330" s="21">
+        <v>42652</v>
+      </c>
+      <c r="C330" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="D330" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E330" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="F330" s="16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="331" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A331" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B331" s="21">
+        <v>42652</v>
+      </c>
+      <c r="C331" s="17" t="s">
+        <v>324</v>
+      </c>
+      <c r="D331" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E331" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="F331" s="20" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="332" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A332" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B332" s="21">
+        <v>42652</v>
+      </c>
+      <c r="C332" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="D332" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E332" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="333" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A333" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B333" s="21">
+        <v>42652</v>
+      </c>
+      <c r="C333" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D333" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E333" s="19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="334" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A334" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B334" s="21">
+        <v>42652</v>
+      </c>
+      <c r="C334" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D334" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E334" s="19" t="s">
         <v>321</v>
       </c>
     </row>
@@ -7613,9 +7893,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.140625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="29.7109375" style="5" customWidth="1"/>
-    <col min="3" max="3" width="39.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="29.75" style="5" customWidth="1"/>
+    <col min="3" max="3" width="39.25" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Re worked the school zoning and distribution. File updates
</commit_message>
<xml_diff>
--- a/CLASSOPS/Derek/Derek's Log.xlsx
+++ b/CLASSOPS/Derek/Derek's Log.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1562" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1628" uniqueCount="359">
   <si>
     <t>Staff Name</t>
   </si>
@@ -1155,6 +1155,36 @@
   </si>
   <si>
     <t>Pickup VGA cable that was brought in earlier.</t>
+  </si>
+  <si>
+    <t>001 -JCR</t>
+  </si>
+  <si>
+    <t>Senate Chamber - keys for room in Ross S120 storeroom. Turn off projector with remote on PC cart. Turn off PC. Turn off amplifier in back booth. Lock room.</t>
+  </si>
+  <si>
+    <t>Set up Skype camera with tripod with built in PC in room. Skype camera is in Founders 164 storeroom. Tell prof. to stay with equipment until picked up. Tell Masi when end time is.</t>
+  </si>
+  <si>
+    <t>Pick up Skype camera and tripod. Log off PC and crestron and return skype camera and tripod to Founders 164 storeroom.</t>
+  </si>
+  <si>
+    <t>Open doors to Nat Taylor Cinema. Allen key in S120 Ross storeroom.</t>
+  </si>
+  <si>
+    <t>Pick up 3 desk mics, all cables and clips and NECK MIC ALSO. Return to Van 040 basement storeroom.</t>
+  </si>
+  <si>
+    <t>Pick up 2 small speakers and speaker cables, all matts and AC cords. Return to Van 040 storeroom.</t>
+  </si>
+  <si>
+    <t>Set up 2 desk mics with mixer and neck microphone. Milk carton with mic cables, mics, mixer and desk stands is in Vari 1019 storeroom. Volume control on crestron - press mic icon and then ramp up " Podium" volume control.  Neck mic is in podium drawer.</t>
+  </si>
+  <si>
+    <t>Pick up 2 mics, mic cables, 2 desk stands and mixer. Return to Vari 1019 storeroom. Wireless neck mic goes back to podium drawer.</t>
+  </si>
+  <si>
+    <t>All equipment in milk crate in Vari 1019. Night Tech to meet Suzanne in room.</t>
   </si>
 </sst>
 </file>
@@ -1691,11 +1721,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I341"/>
+  <dimension ref="A1:I355"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A319" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A341" sqref="A341"/>
+      <pane ySplit="1" topLeftCell="A343" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F358" sqref="F358"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7940,6 +7970,276 @@
       </c>
       <c r="F341" s="20" t="s">
         <v>348</v>
+      </c>
+    </row>
+    <row r="342" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A342" s="6"/>
+      <c r="B342" s="23"/>
+      <c r="C342" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="D342" s="6"/>
+      <c r="E342" s="27"/>
+      <c r="F342" s="29"/>
+    </row>
+    <row r="343" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A343" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B343" s="21">
+        <v>42656</v>
+      </c>
+      <c r="C343" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="D343" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E343" s="19" t="s">
+        <v>277</v>
+      </c>
+      <c r="F343" s="20" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="344" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A344" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B344" s="21">
+        <v>42656</v>
+      </c>
+      <c r="C344" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D344" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E344" s="19" t="s">
+        <v>349</v>
+      </c>
+      <c r="F344" s="20" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="345" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A345" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="B345" s="21">
+        <v>42656</v>
+      </c>
+      <c r="C345" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D345" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E345" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="F345" s="20" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="346" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A346" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B346" s="21">
+        <v>42656</v>
+      </c>
+      <c r="C346" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D346" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E346" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="F346" s="20" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="347" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A347" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B347" s="21">
+        <v>42656</v>
+      </c>
+      <c r="C347" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="D347" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E347" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="F347" s="20" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="348" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A348" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B348" s="21">
+        <v>42656</v>
+      </c>
+      <c r="C348" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D348" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E348" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F348" s="20" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="349" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A349" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B349" s="21">
+        <v>42656</v>
+      </c>
+      <c r="C349" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D349" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="E349" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="F349" s="20" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="350" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A350" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B350" s="21">
+        <v>42656</v>
+      </c>
+      <c r="C350" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="D350" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="E350" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="F350" s="20" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="351" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A351" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B351" s="21">
+        <v>42656</v>
+      </c>
+      <c r="C351" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="D351" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E351" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F351" s="20" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="352" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A352" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B352" s="21">
+        <v>42656</v>
+      </c>
+      <c r="C352" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="D352" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E352" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F352" s="20" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="353" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A353" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B353" s="21">
+        <v>42656</v>
+      </c>
+      <c r="C353" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D353" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E353" s="19" t="s">
+        <v>199</v>
+      </c>
+      <c r="F353" s="20" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="354" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A354" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B354" s="21">
+        <v>42656</v>
+      </c>
+      <c r="C354" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D354" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E354" s="19" t="s">
+        <v>199</v>
+      </c>
+      <c r="F354" s="20" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="355" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A355" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B355" s="21">
+        <v>42656</v>
+      </c>
+      <c r="C355" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="D355" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E355" s="19" t="s">
+        <v>199</v>
+      </c>
+      <c r="F355" s="20" t="s">
+        <v>357</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated files and added more detail to the detail view.
</commit_message>
<xml_diff>
--- a/CLASSOPS/Derek/Derek's Log.xlsx
+++ b/CLASSOPS/Derek/Derek's Log.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1628" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1657" uniqueCount="363">
   <si>
     <t>Staff Name</t>
   </si>
@@ -1185,6 +1185,18 @@
   </si>
   <si>
     <t>All equipment in milk crate in Vari 1019. Night Tech to meet Suzanne in room.</t>
+  </si>
+  <si>
+    <t>256</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Return large screen DLP TV to Vanier 132 storeroom. Pick up wireless keyboard and remote control. </t>
+  </si>
+  <si>
+    <t>Founders Assembly Hall - group in room using projector and computer in room. No order - please make sure projector gets turned off (remote in Fdrs 156A storeroom. Log off PC and please LOCK ROOM. Key for room in Fdrs 164 storeroom.</t>
+  </si>
+  <si>
+    <t>2050</t>
   </si>
 </sst>
 </file>
@@ -1721,11 +1733,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I355"/>
+  <dimension ref="A1:I362"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A343" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F358" sqref="F358"/>
+      <pane ySplit="1" topLeftCell="A350" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B358" sqref="B358:B362"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8170,7 +8182,7 @@
         <v>42656</v>
       </c>
       <c r="C352" s="17" t="s">
-        <v>226</v>
+        <v>243</v>
       </c>
       <c r="D352" s="18" t="s">
         <v>59</v>
@@ -8230,7 +8242,7 @@
         <v>42656</v>
       </c>
       <c r="C355" s="17" t="s">
-        <v>226</v>
+        <v>243</v>
       </c>
       <c r="D355" s="18" t="s">
         <v>51</v>
@@ -8240,6 +8252,130 @@
       </c>
       <c r="F355" s="20" t="s">
         <v>357</v>
+      </c>
+    </row>
+    <row r="356" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A356" s="6"/>
+      <c r="B356" s="23"/>
+      <c r="C356" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="D356" s="6"/>
+      <c r="E356" s="27"/>
+      <c r="F356" s="29"/>
+    </row>
+    <row r="357" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A357" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B357" s="21">
+        <v>42659</v>
+      </c>
+      <c r="C357" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D357" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E357" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="358" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A358" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B358" s="21">
+        <v>42659</v>
+      </c>
+      <c r="C358" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D358" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E358" s="19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="359" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A359" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B359" s="21">
+        <v>42659</v>
+      </c>
+      <c r="C359" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D359" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E359" s="19" t="s">
+        <v>359</v>
+      </c>
+      <c r="F359" s="20" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="360" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A360" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B360" s="21">
+        <v>42659</v>
+      </c>
+      <c r="C360" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="D360" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E360" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F360" s="20" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="361" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A361" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B361" s="21">
+        <v>42659</v>
+      </c>
+      <c r="C361" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D361" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E361" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="F361" s="16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="362" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A362" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B362" s="21">
+        <v>42659</v>
+      </c>
+      <c r="C362" s="17" t="s">
+        <v>362</v>
+      </c>
+      <c r="D362" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E362" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="F362" s="20" t="s">
+        <v>361</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Version 0.2.8 Beta Release
</commit_message>
<xml_diff>
--- a/CLASSOPS/Derek/Derek's Log.xlsx
+++ b/CLASSOPS/Derek/Derek's Log.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1657" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1681" uniqueCount="364">
   <si>
     <t>Staff Name</t>
   </si>
@@ -1197,6 +1197,9 @@
   </si>
   <si>
     <t>2050</t>
+  </si>
+  <si>
+    <t>Pick up wireless keyboard and remote control and return to Founders 164 storeroom. Leave DLP flat screen tv in room.</t>
   </si>
 </sst>
 </file>
@@ -1733,11 +1736,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I362"/>
+  <dimension ref="A1:I368"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A350" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B358" sqref="B358:B362"/>
+      <pane ySplit="1" topLeftCell="A349" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F370" sqref="F370"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8269,7 +8272,7 @@
         <v>80</v>
       </c>
       <c r="B357" s="21">
-        <v>42659</v>
+        <v>42657</v>
       </c>
       <c r="C357" s="17" t="s">
         <v>105</v>
@@ -8286,7 +8289,7 @@
         <v>80</v>
       </c>
       <c r="B358" s="21">
-        <v>42659</v>
+        <v>42657</v>
       </c>
       <c r="C358" s="17" t="s">
         <v>105</v>
@@ -8303,7 +8306,7 @@
         <v>87</v>
       </c>
       <c r="B359" s="21">
-        <v>42659</v>
+        <v>42657</v>
       </c>
       <c r="C359" s="17" t="s">
         <v>107</v>
@@ -8323,7 +8326,7 @@
         <v>80</v>
       </c>
       <c r="B360" s="21">
-        <v>42659</v>
+        <v>42657</v>
       </c>
       <c r="C360" s="17" t="s">
         <v>172</v>
@@ -8343,7 +8346,7 @@
         <v>19</v>
       </c>
       <c r="B361" s="21">
-        <v>42659</v>
+        <v>42657</v>
       </c>
       <c r="C361" s="17" t="s">
         <v>207</v>
@@ -8363,7 +8366,7 @@
         <v>80</v>
       </c>
       <c r="B362" s="21">
-        <v>42659</v>
+        <v>42657</v>
       </c>
       <c r="C362" s="17" t="s">
         <v>362</v>
@@ -8376,6 +8379,110 @@
       </c>
       <c r="F362" s="20" t="s">
         <v>361</v>
+      </c>
+    </row>
+    <row r="363" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A363" s="6"/>
+      <c r="B363" s="23"/>
+      <c r="C363" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D363" s="6"/>
+      <c r="E363" s="27"/>
+      <c r="F363" s="29"/>
+    </row>
+    <row r="364" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A364" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B364" s="21">
+        <v>42660</v>
+      </c>
+      <c r="C364" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="D364" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E364" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="365" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A365" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B365" s="21">
+        <v>42660</v>
+      </c>
+      <c r="C365" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D365" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E365" s="19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="366" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A366" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B366" s="21">
+        <v>42660</v>
+      </c>
+      <c r="C366" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D366" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E366" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="F366" s="16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="367" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A367" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B367" s="21">
+        <v>42660</v>
+      </c>
+      <c r="C367" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D367" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E367" s="19" t="s">
+        <v>279</v>
+      </c>
+      <c r="F367" s="20" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="368" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A368" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B368" s="21">
+        <v>42660</v>
+      </c>
+      <c r="C368" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="D368" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E368" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F368" s="20" t="s">
+        <v>205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updatre logviewer to show the correct colors
</commit_message>
<xml_diff>
--- a/CLASSOPS/Derek/Derek's Log.xlsx
+++ b/CLASSOPS/Derek/Derek's Log.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1681" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1774" uniqueCount="374">
   <si>
     <t>Staff Name</t>
   </si>
@@ -1200,6 +1200,36 @@
   </si>
   <si>
     <t>Pick up wireless keyboard and remote control and return to Founders 164 storeroom. Leave DLP flat screen tv in room.</t>
+  </si>
+  <si>
+    <t>Turn off PC and projector. Leave all in and lock room.</t>
+  </si>
+  <si>
+    <t>Lec mic is in place already.  Turn on PC and projector. Show client how to adjust volumes from the back mixing board if required.</t>
+  </si>
+  <si>
+    <t>Return lec mic, stand, projector remote and presentation remote to back booth. Lock booth and both entrance doors before leavning.</t>
+  </si>
+  <si>
+    <t>Includes large portable screen. Client supplied own laptop and audio cable. Return to Vanier 040 storeroom.</t>
+  </si>
+  <si>
+    <t>1720</t>
+  </si>
+  <si>
+    <t>Event begins at 6pm. Setup 3 floor stand stage mics according to client's preference with appropriate number of floor mats or tape. From Vanier 040 storeroom.</t>
+  </si>
+  <si>
+    <t>3 stage mics, stands, cables and floor mats. To Vanier 040 store.</t>
+  </si>
+  <si>
+    <t>Event begins at 6pm. Need large portable screen. Client is supplying Mac laptop with own audio cable. From Vanier 040 store.</t>
+  </si>
+  <si>
+    <t>Lec mic, stand, cables etc. To Vanier 040 storeroom.</t>
+  </si>
+  <si>
+    <t>Includes portable screen and mats. To Vanier 040 storeroom.</t>
   </si>
 </sst>
 </file>
@@ -1736,11 +1766,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I368"/>
+  <dimension ref="A1:I389"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A349" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F370" sqref="F370"/>
+      <pane ySplit="1" topLeftCell="A379" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A396" sqref="A396"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8483,6 +8513,394 @@
       </c>
       <c r="F368" s="20" t="s">
         <v>205</v>
+      </c>
+    </row>
+    <row r="369" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A369" s="6"/>
+      <c r="B369" s="23"/>
+      <c r="C369" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="D369" s="6"/>
+      <c r="E369" s="27"/>
+      <c r="F369" s="29"/>
+    </row>
+    <row r="370" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A370" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B370" s="21">
+        <v>42661</v>
+      </c>
+      <c r="C370" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D370" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E370" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="371" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A371" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B371" s="21">
+        <v>42661</v>
+      </c>
+      <c r="C371" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D371" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E371" s="19" t="s">
+        <v>272</v>
+      </c>
+      <c r="F371" s="20" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="372" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A372" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B372" s="21">
+        <v>42661</v>
+      </c>
+      <c r="C372" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="D372" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E372" s="19" t="s">
+        <v>277</v>
+      </c>
+      <c r="F372" s="20" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="373" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A373" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B373" s="21">
+        <v>42661</v>
+      </c>
+      <c r="C373" s="17" t="s">
+        <v>284</v>
+      </c>
+      <c r="D373" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E373" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="F373" s="20" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="374" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A374" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B374" s="21">
+        <v>42661</v>
+      </c>
+      <c r="C374" s="17" t="s">
+        <v>368</v>
+      </c>
+      <c r="D374" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="E374" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="F374" s="20" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="375" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A375" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B375" s="21">
+        <v>42661</v>
+      </c>
+      <c r="C375" s="17" t="s">
+        <v>368</v>
+      </c>
+      <c r="D375" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="E375" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="F375" s="20" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="376" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A376" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B376" s="21">
+        <v>42661</v>
+      </c>
+      <c r="C376" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D376" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E376" s="19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="377" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A377" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B377" s="21">
+        <v>42661</v>
+      </c>
+      <c r="C377" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="D377" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E377" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F377" s="20" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="378" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A378" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B378" s="21">
+        <v>42661</v>
+      </c>
+      <c r="C378" s="17" t="s">
+        <v>324</v>
+      </c>
+      <c r="D378" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E378" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="F378" s="20" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="379" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A379" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B379" s="21">
+        <v>42661</v>
+      </c>
+      <c r="C379" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="D379" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E379" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="F379" s="16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="380" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A380" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B380" s="21">
+        <v>42661</v>
+      </c>
+      <c r="C380" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="D380" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="E380" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="F380" s="20" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="381" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A381" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B381" s="21">
+        <v>42661</v>
+      </c>
+      <c r="C381" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="D381" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="E381" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="F381" s="20" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="382" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A382" s="6"/>
+      <c r="B382" s="23"/>
+      <c r="C382" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D382" s="6"/>
+      <c r="E382" s="27"/>
+      <c r="F382" s="29"/>
+    </row>
+    <row r="383" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A383" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="B383" s="21">
+        <v>42662</v>
+      </c>
+      <c r="C383" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D383" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E383" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="F383" s="20" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="384" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A384" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B384" s="21">
+        <v>42662</v>
+      </c>
+      <c r="C384" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D384" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E384" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="F384" s="20" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="385" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A385" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B385" s="21">
+        <v>42662</v>
+      </c>
+      <c r="C385" s="17" t="s">
+        <v>284</v>
+      </c>
+      <c r="D385" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E385" s="19" t="s">
+        <v>275</v>
+      </c>
+      <c r="F385" s="20" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="386" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A386" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B386" s="21">
+        <v>42662</v>
+      </c>
+      <c r="C386" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D386" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E386" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="F386" s="16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="387" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A387" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B387" s="21">
+        <v>42662</v>
+      </c>
+      <c r="C387" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D387" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E387" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="388" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A388" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B388" s="21">
+        <v>42662</v>
+      </c>
+      <c r="C388" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D388" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E388" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F388" s="20" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="389" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A389" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B389" s="21">
+        <v>42662</v>
+      </c>
+      <c r="C389" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D389" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E389" s="19" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed a bug that causes the event to point to a null reference.
</commit_message>
<xml_diff>
--- a/CLASSOPS/Derek/Derek's Log.xlsx
+++ b/CLASSOPS/Derek/Derek's Log.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17329"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhan\Documents\Visual Studio 2015\Projects\ClassOpsLogCreator\CLASSOPS\Derek\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="90" yWindow="150" windowWidth="14865" windowHeight="10785" tabRatio="440"/>
   </bookViews>
@@ -22,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1823" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1843" uniqueCount="381">
   <si>
     <t>Staff Name</t>
   </si>
@@ -1302,7 +1307,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
@@ -1539,6 +1544,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1586,7 +1594,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1619,9 +1627,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1654,6 +1679,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1833,22 +1875,22 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I400"/>
+  <dimension ref="A1:I405"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A382" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F402" sqref="F402"/>
+      <pane ySplit="1" topLeftCell="A388" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B402" sqref="B402:B405"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="22.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" style="10" customWidth="1"/>
+    <col min="1" max="1" width="27.75" style="10" customWidth="1"/>
     <col min="2" max="2" width="19" style="21" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.375" style="17" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="18" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" style="19" customWidth="1"/>
-    <col min="6" max="6" width="60.42578125" style="20" customWidth="1"/>
-    <col min="7" max="16384" width="22.140625" style="2"/>
+    <col min="5" max="5" width="11.75" style="19" customWidth="1"/>
+    <col min="6" max="6" width="60.375" style="20" customWidth="1"/>
+    <col min="7" max="16384" width="22.125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -9171,6 +9213,93 @@
         <v>136</v>
       </c>
       <c r="F400" s="20" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="401" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A401" s="6"/>
+      <c r="B401" s="23"/>
+      <c r="C401" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="D401" s="6"/>
+      <c r="E401" s="27"/>
+      <c r="F401" s="29"/>
+    </row>
+    <row r="402" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A402" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B402" s="21">
+        <v>42666</v>
+      </c>
+      <c r="C402" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D402" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E402" s="19" t="s">
+        <v>277</v>
+      </c>
+      <c r="F402" s="20" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="403" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A403" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B403" s="21">
+        <v>42666</v>
+      </c>
+      <c r="C403" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D403" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E403" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="404" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A404" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B404" s="21">
+        <v>42666</v>
+      </c>
+      <c r="C404" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D404" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E404" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="F404" s="16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="405" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A405" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B405" s="21">
+        <v>42666</v>
+      </c>
+      <c r="C405" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="D405" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E405" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F405" s="20" t="s">
         <v>205</v>
       </c>
     </row>
@@ -9209,9 +9338,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.140625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="29.7109375" style="5" customWidth="1"/>
-    <col min="3" max="3" width="39.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="29.75" style="5" customWidth="1"/>
+    <col min="3" max="3" width="39.25" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Re did the headers overall
</commit_message>
<xml_diff>
--- a/CLASSOPS/Derek/Derek's Log.xlsx
+++ b/CLASSOPS/Derek/Derek's Log.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1906" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1975" uniqueCount="393">
   <si>
     <t>Staff Name</t>
   </si>
@@ -1338,6 +1338,21 @@
   </si>
   <si>
     <t>Please pickup a pair of laptop speakers loaned to the professor. Return to Vari 1019 MCR.</t>
+  </si>
+  <si>
+    <t>Includes mats but no portable screen. To Vanier 040 storeroom.</t>
+  </si>
+  <si>
+    <t>Lec mic is in place already. One hour operator asssistance.</t>
+  </si>
+  <si>
+    <t>Return lec mic, stand and cable to Ross S120 storeroom.</t>
+  </si>
+  <si>
+    <t>2115</t>
+  </si>
+  <si>
+    <t>Return lec mic, 2 desk mics, 1 audience mic and stands, projector remote and presentation remote to back booth.</t>
   </si>
 </sst>
 </file>
@@ -1874,11 +1889,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I420"/>
+  <dimension ref="A1:I436"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A400" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B426" sqref="B426"/>
+      <pane ySplit="1" topLeftCell="A411" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G432" sqref="G432"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9570,6 +9585,297 @@
         <v>205</v>
       </c>
     </row>
+    <row r="421" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A421" s="6"/>
+      <c r="B421" s="23"/>
+      <c r="C421" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D421" s="6"/>
+      <c r="E421" s="27"/>
+      <c r="F421" s="29"/>
+    </row>
+    <row r="422" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A422" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B422" s="21">
+        <v>42669</v>
+      </c>
+      <c r="C422" s="17" t="s">
+        <v>284</v>
+      </c>
+      <c r="D422" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E422" s="19" t="s">
+        <v>275</v>
+      </c>
+      <c r="F422" s="20" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="423" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A423" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B423" s="21">
+        <v>42669</v>
+      </c>
+      <c r="C423" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D423" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E423" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="F423" s="16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="424" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A424" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B424" s="21">
+        <v>42669</v>
+      </c>
+      <c r="C424" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D424" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E424" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="425" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A425" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B425" s="21">
+        <v>42669</v>
+      </c>
+      <c r="C425" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="D425" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E425" s="19" t="s">
+        <v>259</v>
+      </c>
+      <c r="F425" s="20" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="426" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A426" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B426" s="21">
+        <v>42669</v>
+      </c>
+      <c r="C426" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D426" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E426" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F426" s="20" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="427" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A427" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B427" s="21">
+        <v>42669</v>
+      </c>
+      <c r="C427" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D427" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E427" s="19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="428" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A428" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B428" s="21">
+        <v>42669</v>
+      </c>
+      <c r="C428" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="D428" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E428" s="19" t="s">
+        <v>259</v>
+      </c>
+      <c r="F428" s="20" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="429" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A429" s="6"/>
+      <c r="B429" s="23"/>
+      <c r="C429" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="D429" s="6"/>
+      <c r="E429" s="27"/>
+      <c r="F429" s="29"/>
+    </row>
+    <row r="430" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A430" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B430" s="21">
+        <v>42670</v>
+      </c>
+      <c r="C430" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D430" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E430" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="F430" s="16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="431" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A431" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B431" s="21">
+        <v>42670</v>
+      </c>
+      <c r="C431" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D431" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E431" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="F431" s="20" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="432" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A432" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B432" s="21">
+        <v>42670</v>
+      </c>
+      <c r="C432" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="D432" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E432" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="F432" s="20" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="433" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A433" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B433" s="21">
+        <v>42670</v>
+      </c>
+      <c r="C433" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="D433" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E433" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="434" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A434" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B434" s="21">
+        <v>42670</v>
+      </c>
+      <c r="C434" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="D434" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E434" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F434" s="20" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="435" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A435" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B435" s="21">
+        <v>42670</v>
+      </c>
+      <c r="C435" s="17" t="s">
+        <v>391</v>
+      </c>
+      <c r="D435" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E435" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F435" s="20" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="436" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A436" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B436" s="21">
+        <v>42670</v>
+      </c>
+      <c r="C436" s="17" t="s">
+        <v>391</v>
+      </c>
+      <c r="D436" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E436" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F436" s="20" t="s">
+        <v>205</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0"/>
   <sortState ref="A427:G515">
@@ -9577,10 +9883,10 @@
     <sortCondition ref="D427:D515"/>
   </sortState>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A22:A23 B6 B2 A7:A8 B9 A10:A16 B17 A18:A20 B21 A3:A5 B24 A25:A27 B28 B32 A29:A31 A33:A34 B35 A36:A37 B38 A39:A53 B54 A55:A57 B58 A59:A63 B64 A65:A80 B81 A82:A85 B86 A87:A104 B105 A106:A109 B110 A111:A120 B121 A122:A133 B134 A135:A145 B146 A147:A176 B177 A178:A195 B196 A197:A203 B204 A205:A219 B220 A221:A227 B228 A229:A246 B247 A248:A264 B265 A266:A272 B273 A274:A278 B279 A280:A418 A419:A1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A22:A23 B6 B2 A7:A8 B9 A10:A16 B17 A18:A20 B21 A3:A5 B24 A25:A27 B28 B32 A29:A31 A33:A34 B35 A36:A37 B38 A39:A53 B54 A55:A57 B58 A59:A63 B64 A65:A80 B81 A82:A85 B86 A87:A104 B105 A106:A109 B110 A111:A120 B121 A122:A133 B134 A135:A145 B146 A147:A176 B177 A178:A195 B196 A197:A203 B204 A205:A219 B220 A221:A227 B228 A229:A246 B247 A248:A264 B265 A266:A272 B273 A274:A278 B279 A280:A1048576">
       <formula1>Task_type</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6 E2 D22:D23 D7:D8 E9 D10:D16 E17 D18:D20 E21 D3:D5 E24 D25:D27 E28 E32 D29:D31 D33:D34 E35 D36:D37 E38 D39:D53 E54 D55:D57 E58 D59:D63 E64 D65:D80 E81 D82:D85 E86 D87:D104 E105 D106:D109 E110 D111:D120 E121 D122:D133 E134 D135:D145 E146 D147:D176 E177 D178:D195 E196 D197:D203 E204 D205:D219 E220 D221:D227 E228 D229:D246 E247 D248:D264 E265 D266:D272 E273 D274:D278 E279 D280:D418 D419:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6 E2 D22:D23 D7:D8 E9 D10:D16 E17 D18:D20 E21 D3:D5 E24 D25:D27 E28 E32 D29:D31 D33:D34 E35 D36:D37 E38 D39:D53 E54 D55:D57 E58 D59:D63 E64 D65:D80 E81 D82:D85 E86 D87:D104 E105 D106:D109 E110 D111:D120 E121 D122:D133 E134 D135:D145 E146 D147:D176 E177 D178:D195 E196 D197:D203 E204 D205:D219 E220 D221:D227 E228 D229:D246 E247 D248:D264 E265 D266:D272 E273 D274:D278 E279 D280:D1048576">
       <formula1>Building</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 A2 A9 A17 A21 A24 A28 A32 A35 A38 A54 A58 A64 A81 A86 A105 A110 A121 A134 A146 A177 A196 A204 A220 A228 A247 A265 A273 A279">

</xml_diff>

<commit_message>
update file and release new version 0.2.10
</commit_message>
<xml_diff>
--- a/CLASSOPS/Derek/Derek's Log.xlsx
+++ b/CLASSOPS/Derek/Derek's Log.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1975" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2030" uniqueCount="395">
   <si>
     <t>Staff Name</t>
   </si>
@@ -1353,6 +1353,12 @@
   </si>
   <si>
     <t>Return lec mic, 2 desk mics, 1 audience mic and stands, projector remote and presentation remote to back booth.</t>
+  </si>
+  <si>
+    <t>1 lec mic, 2 desk mics, 3 wireless Shure mics, stands, cables, audio mixer, receivers etc. on a cart.  Make certain to power off Shure wireless mics. Return all items to Vari 1019 MCR. Raul needs some of this equipment for Saturday in his area.</t>
+  </si>
+  <si>
+    <t>Door code 7083*. Leave portable screen. Return to FDRS 156A.</t>
   </si>
 </sst>
 </file>
@@ -1889,11 +1895,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I436"/>
+  <dimension ref="A1:I449"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A411" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G432" sqref="G432"/>
+      <pane ySplit="1" topLeftCell="A438" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C464" sqref="C464"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9874,6 +9880,240 @@
       </c>
       <c r="F436" s="20" t="s">
         <v>205</v>
+      </c>
+    </row>
+    <row r="437" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A437" s="6"/>
+      <c r="B437" s="23"/>
+      <c r="C437" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="D437" s="6"/>
+      <c r="E437" s="27"/>
+      <c r="F437" s="29"/>
+    </row>
+    <row r="438" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A438" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B438" s="21">
+        <v>42671</v>
+      </c>
+      <c r="C438" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D438" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E438" s="19" t="s">
+        <v>199</v>
+      </c>
+      <c r="F438" s="20" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="439" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A439" s="6"/>
+      <c r="B439" s="23"/>
+      <c r="C439" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D439" s="6"/>
+      <c r="E439" s="27"/>
+      <c r="F439" s="29"/>
+    </row>
+    <row r="440" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A440" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B440" s="21">
+        <v>42674</v>
+      </c>
+      <c r="C440" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D440" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E440" s="19" t="s">
+        <v>381</v>
+      </c>
+      <c r="F440" s="14" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="441" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A441" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B441" s="21">
+        <v>42674</v>
+      </c>
+      <c r="C441" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D441" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E441" s="19" t="s">
+        <v>381</v>
+      </c>
+      <c r="F441" s="20" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="442" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A442" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B442" s="21">
+        <v>42674</v>
+      </c>
+      <c r="C442" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D442" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E442" s="19" t="s">
+        <v>279</v>
+      </c>
+      <c r="F442" s="20" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="443" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A443" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B443" s="21">
+        <v>42674</v>
+      </c>
+      <c r="C443" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="D443" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E443" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="F443" s="20" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="444" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A444" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B444" s="21">
+        <v>42674</v>
+      </c>
+      <c r="C444" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D444" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E444" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="F444" s="16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="445" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A445" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B445" s="21">
+        <v>42674</v>
+      </c>
+      <c r="C445" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D445" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E445" s="19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="446" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A446" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B446" s="21">
+        <v>42674</v>
+      </c>
+      <c r="C446" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="D446" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E446" s="19" t="s">
+        <v>277</v>
+      </c>
+      <c r="F446" s="20" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="447" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A447" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B447" s="21">
+        <v>42674</v>
+      </c>
+      <c r="C447" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="D447" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E447" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="448" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A448" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B448" s="21">
+        <v>42674</v>
+      </c>
+      <c r="C448" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="D448" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E448" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F448" s="20" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="449" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A449" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B449" s="21">
+        <v>42674</v>
+      </c>
+      <c r="C449" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="D449" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E449" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="F449" s="20" t="s">
+        <v>394</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
All praphs are saved
</commit_message>
<xml_diff>
--- a/CLASSOPS/Derek/Derek's Log.xlsx
+++ b/CLASSOPS/Derek/Derek's Log.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2059" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2226" uniqueCount="407">
   <si>
     <t>Staff Name</t>
   </si>
@@ -1359,6 +1359,65 @@
   </si>
   <si>
     <t>Door code 7083*. Leave portable screen. Return to FDRS 156A.</t>
+  </si>
+  <si>
+    <t>Audience mic, lec mic, desk mic, neck mic, stands to back booth.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Lee Wiggins would like to have </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>closed captions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> activated on VLC media player to accommodate student. Demo also.</t>
+    </r>
+  </si>
+  <si>
+    <t>DLP flat screen TV. Leave portable screen and network cable, but get carpets. To  Vanier 132 storeroom.</t>
+  </si>
+  <si>
+    <t>Pickup Skype web cam and tripod.  To Ross S120 store.</t>
+  </si>
+  <si>
+    <t>Get wireless keyboard and projector remote from FDRS 156A.</t>
+  </si>
+  <si>
+    <t>Unlock doors to the Nat Taylor Cinema.</t>
+  </si>
+  <si>
+    <t>Return wireless keyboard &amp; projector remote to FDRS 156A.  Pickup straight floor stand supplied earlier. Lock room.</t>
+  </si>
+  <si>
+    <t>Please supply a straight floor stand to LTS. They will supply the mics for this event.</t>
+  </si>
+  <si>
+    <t>201</t>
+  </si>
+  <si>
+    <t>Web cam and tripod to FDRS 164.</t>
+  </si>
+  <si>
+    <t>Neck mic and small PA to FDRS 156A.</t>
+  </si>
+  <si>
+    <t>No mics, just computer and projector. Remotes to the back booth.</t>
   </si>
 </sst>
 </file>
@@ -1895,11 +1954,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I456"/>
+  <dimension ref="A1:I494"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A432" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C460" sqref="C460"/>
+      <pane ySplit="1" topLeftCell="A471" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G485" sqref="G485"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10240,6 +10299,705 @@
         <v>205</v>
       </c>
     </row>
+    <row r="457" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A457" s="6"/>
+      <c r="B457" s="23"/>
+      <c r="C457" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D457" s="6"/>
+      <c r="E457" s="27"/>
+      <c r="F457" s="29"/>
+    </row>
+    <row r="458" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A458" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B458" s="21">
+        <v>42676</v>
+      </c>
+      <c r="C458" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D458" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E458" s="19" t="s">
+        <v>277</v>
+      </c>
+      <c r="F458" s="20" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="459" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A459" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B459" s="21">
+        <v>42676</v>
+      </c>
+      <c r="C459" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="D459" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E459" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="F459" s="20" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="460" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A460" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B460" s="21">
+        <v>42676</v>
+      </c>
+      <c r="C460" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="D460" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E460" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="F460" s="20" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="461" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A461" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B461" s="21">
+        <v>42676</v>
+      </c>
+      <c r="C461" s="17" t="s">
+        <v>284</v>
+      </c>
+      <c r="D461" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E461" s="19" t="s">
+        <v>275</v>
+      </c>
+      <c r="F461" s="20" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="462" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A462" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B462" s="21">
+        <v>42676</v>
+      </c>
+      <c r="C462" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D462" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E462" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="F462" s="16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="463" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A463" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B463" s="21">
+        <v>42676</v>
+      </c>
+      <c r="C463" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D463" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E463" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="464" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A464" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B464" s="21">
+        <v>42676</v>
+      </c>
+      <c r="C464" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="D464" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E464" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="F464" s="20" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="465" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A465" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B465" s="21">
+        <v>42676</v>
+      </c>
+      <c r="C465" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D465" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E465" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F465" s="20" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="466" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A466" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B466" s="21">
+        <v>42676</v>
+      </c>
+      <c r="C466" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D466" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E466" s="19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="467" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A467" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B467" s="21">
+        <v>42676</v>
+      </c>
+      <c r="C467" s="17" t="s">
+        <v>269</v>
+      </c>
+      <c r="D467" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E467" s="19" t="s">
+        <v>202</v>
+      </c>
+      <c r="F467" s="20" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="468" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A468" s="6"/>
+      <c r="B468" s="23"/>
+      <c r="C468" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="D468" s="6"/>
+      <c r="E468" s="27"/>
+      <c r="F468" s="29"/>
+    </row>
+    <row r="469" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A469" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B469" s="21">
+        <v>42677</v>
+      </c>
+      <c r="C469" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D469" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E469" s="19" t="s">
+        <v>279</v>
+      </c>
+      <c r="F469" s="20" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="470" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A470" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B470" s="21">
+        <v>42677</v>
+      </c>
+      <c r="C470" s="17" t="s">
+        <v>284</v>
+      </c>
+      <c r="D470" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E470" s="19" t="s">
+        <v>381</v>
+      </c>
+      <c r="F470" s="20" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="471" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A471" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B471" s="21">
+        <v>42677</v>
+      </c>
+      <c r="C471" s="17" t="s">
+        <v>284</v>
+      </c>
+      <c r="D471" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E471" s="19" t="s">
+        <v>381</v>
+      </c>
+      <c r="F471" s="20" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="472" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A472" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B472" s="21">
+        <v>42677</v>
+      </c>
+      <c r="C472" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D472" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E472" s="19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="473" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A473" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B473" s="21">
+        <v>42677</v>
+      </c>
+      <c r="C473" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="D473" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E473" s="19" t="s">
+        <v>277</v>
+      </c>
+      <c r="F473" s="20" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="474" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A474" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B474" s="21">
+        <v>42677</v>
+      </c>
+      <c r="C474" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="D474" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E474" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F474" s="20" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="475" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A475" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B475" s="21">
+        <v>42677</v>
+      </c>
+      <c r="C475" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="D475" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E475" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="F475" s="16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="476" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A476" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B476" s="21">
+        <v>42677</v>
+      </c>
+      <c r="C476" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="D476" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E476" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="477" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A477" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B477" s="21">
+        <v>42677</v>
+      </c>
+      <c r="C477" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="D477" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E477" s="19" t="s">
+        <v>381</v>
+      </c>
+      <c r="F477" s="20" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="478" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A478" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B478" s="21">
+        <v>42677</v>
+      </c>
+      <c r="C478" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="D478" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E478" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F478" s="20" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="479" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A479" s="6"/>
+      <c r="B479" s="23"/>
+      <c r="C479" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="D479" s="6"/>
+      <c r="E479" s="27"/>
+      <c r="F479" s="29"/>
+    </row>
+    <row r="480" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A480" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B480" s="21">
+        <v>42678</v>
+      </c>
+      <c r="C480" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D480" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E480" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="481" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A481" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B481" s="21">
+        <v>42678</v>
+      </c>
+      <c r="C481" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D481" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E481" s="19" t="s">
+        <v>403</v>
+      </c>
+      <c r="F481" s="20" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="482" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A482" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B482" s="21">
+        <v>42678</v>
+      </c>
+      <c r="C482" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D482" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E482" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="F482" s="16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="483" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A483" s="6"/>
+      <c r="B483" s="23"/>
+      <c r="C483" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D483" s="6"/>
+      <c r="E483" s="27"/>
+      <c r="F483" s="29"/>
+    </row>
+    <row r="484" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A484" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B484" s="21">
+        <v>42681</v>
+      </c>
+      <c r="C484" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D484" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E484" s="19" t="s">
+        <v>277</v>
+      </c>
+      <c r="F484" s="20" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="485" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A485" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B485" s="21">
+        <v>42681</v>
+      </c>
+      <c r="C485" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D485" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E485" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="F485" s="16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="486" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A486" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B486" s="21">
+        <v>42681</v>
+      </c>
+      <c r="C486" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D486" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E486" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="F486" s="20" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="487" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A487" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B487" s="21">
+        <v>42681</v>
+      </c>
+      <c r="C487" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D487" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E487" s="19" t="s">
+        <v>381</v>
+      </c>
+      <c r="F487" s="14" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="488" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A488" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B488" s="21">
+        <v>42681</v>
+      </c>
+      <c r="C488" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D488" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E488" s="19" t="s">
+        <v>381</v>
+      </c>
+      <c r="F488" s="20" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="489" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A489" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B489" s="21">
+        <v>42681</v>
+      </c>
+      <c r="C489" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D489" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E489" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="F489" s="20" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="490" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A490" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B490" s="21">
+        <v>42681</v>
+      </c>
+      <c r="C490" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D490" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E490" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="F490" s="20" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="491" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A491" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B491" s="21">
+        <v>42681</v>
+      </c>
+      <c r="C491" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D491" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E491" s="19" t="s">
+        <v>279</v>
+      </c>
+      <c r="F491" s="20" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="492" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A492" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B492" s="21">
+        <v>42681</v>
+      </c>
+      <c r="C492" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D492" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E492" s="19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="493" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A493" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B493" s="21">
+        <v>42681</v>
+      </c>
+      <c r="C493" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="D493" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E493" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="494" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A494" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B494" s="21">
+        <v>42681</v>
+      </c>
+      <c r="C494" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="D494" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E494" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F494" s="20" t="s">
+        <v>205</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0"/>
   <sortState ref="A427:G515">
@@ -10247,10 +11005,10 @@
     <sortCondition ref="D427:D515"/>
   </sortState>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A22:A23 B6 B2 A7:A8 B9 A10:A16 B17 A18:A20 B21 A3:A5 B24 A25:A27 B28 B32 A29:A31 A33:A34 B35 A36:A37 B38 A39:A53 B54 A55:A57 B58 A59:A63 B64 A65:A80 B81 A82:A85 B86 A87:A104 B105 A106:A109 B110 A111:A120 B121 A122:A133 B134 A135:A145 B146 A147:A176 B177 A178:A195 B196 A197:A203 B204 A205:A219 B220 A221:A227 B228 A229:A246 B247 A248:A264 B265 A266:A272 B273 A274:A278 B279 A280:A453 A454:A1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A22:A23 B6 B2 A7:A8 B9 A10:A16 B17 A18:A20 B21 A3:A5 B24 A25:A27 B28 B32 A29:A31 A33:A34 B35 A36:A37 B38 A39:A53 B54 A55:A57 B58 A59:A63 B64 A65:A80 B81 A82:A85 B86 A87:A104 B105 A106:A109 B110 A111:A120 B121 A122:A133 B134 A135:A145 B146 A147:A176 B177 A178:A195 B196 A197:A203 B204 A205:A219 B220 A221:A227 B228 A229:A246 B247 A248:A264 B265 A266:A272 B273 A274:A278 B279 A280:A491 A492:A1048576">
       <formula1>Task_type</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6 E2 D22:D23 D7:D8 E9 D10:D16 E17 D18:D20 E21 D3:D5 E24 D25:D27 E28 E32 D29:D31 D33:D34 E35 D36:D37 E38 D39:D53 E54 D55:D57 E58 D59:D63 E64 D65:D80 E81 D82:D85 E86 D87:D104 E105 D106:D109 E110 D111:D120 E121 D122:D133 E134 D135:D145 E146 D147:D176 E177 D178:D195 E196 D197:D203 E204 D205:D219 E220 D221:D227 E228 D229:D246 E247 D248:D264 E265 D266:D272 E273 D274:D278 E279 D280:D453 D454:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6 E2 D22:D23 D7:D8 E9 D10:D16 E17 D18:D20 E21 D3:D5 E24 D25:D27 E28 E32 D29:D31 D33:D34 E35 D36:D37 E38 D39:D53 E54 D55:D57 E58 D59:D63 E64 D65:D80 E81 D82:D85 E86 D87:D104 E105 D106:D109 E110 D111:D120 E121 D122:D133 E134 D135:D145 E146 D147:D176 E177 D178:D195 E196 D197:D203 E204 D205:D219 E220 D221:D227 E228 D229:D246 E247 D248:D264 E265 D266:D272 E273 D274:D278 E279 D280:D491 D492:D1048576">
       <formula1>Building</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 A2 A9 A17 A21 A24 A28 A32 A35 A38 A54 A58 A64 A81 A86 A105 A110 A121 A134 A146 A177 A196 A204 A220 A228 A247 A265 A273 A279">

</xml_diff>

<commit_message>
Update the files, made it so the pdf file open when the "Generate" Button is clicked. Released a new version to 0.2.11. Added a whole number percent to the legend. Started working on the admin settings for building adding and deleting
</commit_message>
<xml_diff>
--- a/CLASSOPS/Derek/Derek's Log.xlsx
+++ b/CLASSOPS/Derek/Derek's Log.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2398" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2412" uniqueCount="422">
   <si>
     <t>Staff Name</t>
   </si>
@@ -1999,11 +1999,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I532"/>
+  <dimension ref="A1:I536"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A513" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C533" sqref="C533"/>
+      <pane ySplit="1" topLeftCell="A528" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E537" sqref="E537"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11755,6 +11755,70 @@
         <v>205</v>
       </c>
     </row>
+    <row r="533" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A533" s="6"/>
+      <c r="B533" s="23"/>
+      <c r="C533" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="D533" s="6"/>
+      <c r="E533" s="27"/>
+      <c r="F533" s="29"/>
+    </row>
+    <row r="534" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A534" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B534" s="21">
+        <v>42685</v>
+      </c>
+      <c r="C534" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D534" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E534" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="535" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A535" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B535" s="21">
+        <v>42685</v>
+      </c>
+      <c r="C535" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D535" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E535" s="19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="536" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A536" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B536" s="21">
+        <v>42685</v>
+      </c>
+      <c r="C536" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D536" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E536" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="F536" s="16" t="s">
+        <v>128</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0"/>
   <sortState ref="A427:G515">
@@ -11762,10 +11826,10 @@
     <sortCondition ref="D427:D515"/>
   </sortState>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A22:A23 B6 B2 A7:A8 B9 A10:A16 B17 A18:A20 B21 A3:A5 B24 A25:A27 B28 B32 A29:A31 A33:A34 B35 A36:A37 B38 A39:A53 B54 A55:A57 B58 A59:A63 B64 A65:A80 B81 A82:A85 B86 A87:A104 B105 A106:A109 B110 A111:A120 B121 A122:A133 B134 A135:A145 B146 A147:A176 B177 A178:A195 B196 A197:A203 B204 A205:A219 B220 A221:A227 B228 A229:A246 B247 A248:A264 B265 A266:A272 B273 A274:A278 B279 A280:A532 A533:A1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A22:A23 B6 B2 A7:A8 B9 A10:A16 B17 A18:A20 B21 A3:A5 B24 A25:A27 B28 B32 A29:A31 A33:A34 B35 A36:A37 B38 A39:A53 B54 A55:A57 B58 A59:A63 B64 A65:A80 B81 A82:A85 B86 A87:A104 B105 A106:A109 B110 A111:A120 B121 A122:A133 B134 A135:A145 B146 A147:A176 B177 A178:A195 B196 A197:A203 B204 A205:A219 B220 A221:A227 B228 A229:A246 B247 A248:A264 B265 A266:A272 B273 A274:A278 B279 A280:A1048576">
       <formula1>Task_type</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6 E2 D22:D23 D7:D8 E9 D10:D16 E17 D18:D20 E21 D3:D5 E24 D25:D27 E28 E32 D29:D31 D33:D34 E35 D36:D37 E38 D39:D53 E54 D55:D57 E58 D59:D63 E64 D65:D80 E81 D82:D85 E86 D87:D104 E105 D106:D109 E110 D111:D120 E121 D122:D133 E134 D135:D145 E146 D147:D176 E177 D178:D195 E196 D197:D203 E204 D205:D219 E220 D221:D227 E228 D229:D246 E247 D248:D264 E265 D266:D272 E273 D274:D278 E279 D280:D532 D533:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6 E2 D22:D23 D7:D8 E9 D10:D16 E17 D18:D20 E21 D3:D5 E24 D25:D27 E28 E32 D29:D31 D33:D34 E35 D36:D37 E38 D39:D53 E54 D55:D57 E58 D59:D63 E64 D65:D80 E81 D82:D85 E86 D87:D104 E105 D106:D109 E110 D111:D120 E121 D122:D133 E134 D135:D145 E146 D147:D176 E177 D178:D195 E196 D197:D203 E204 D205:D219 E220 D221:D227 E228 D229:D246 E247 D248:D264 E265 D266:D272 E273 D274:D278 E279 D280:D1048576">
       <formula1>Building</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 A2 A9 A17 A21 A24 A28 A32 A35 A38 A54 A58 A64 A81 A86 A105 A110 A121 A134 A146 A177 A196 A204 A220 A228 A247 A265 A273 A279">

</xml_diff>

<commit_message>
More work on gmail login.
</commit_message>
<xml_diff>
--- a/CLASSOPS/Derek/Derek's Log.xlsx
+++ b/CLASSOPS/Derek/Derek's Log.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2726" uniqueCount="443">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2819" uniqueCount="444">
   <si>
     <t>Staff Name</t>
   </si>
@@ -1743,6 +1743,9 @@
       </rPr>
       <t>. Leave portable screen. Return to FDRS 156A.</t>
     </r>
+  </si>
+  <si>
+    <t>Pick up Skype camera with tripod and USB extension cable. Return to Vari 1019 MCR storeroom. BE ON TIME - CRUCIAL.</t>
   </si>
 </sst>
 </file>
@@ -2279,11 +2282,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I607"/>
+  <dimension ref="A1:I628"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A582" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H600" sqref="H600"/>
+      <pane ySplit="1" topLeftCell="A614" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B635" sqref="B635"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13410,6 +13413,394 @@
         <v>442</v>
       </c>
     </row>
+    <row r="608" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A608" s="6"/>
+      <c r="B608" s="23"/>
+      <c r="C608" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D608" s="6"/>
+      <c r="E608" s="27"/>
+      <c r="F608" s="29"/>
+    </row>
+    <row r="609" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A609" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B609" s="21">
+        <v>42697</v>
+      </c>
+      <c r="C609" s="17" t="s">
+        <v>284</v>
+      </c>
+      <c r="D609" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E609" s="19" t="s">
+        <v>275</v>
+      </c>
+      <c r="F609" s="20" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="610" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A610" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B610" s="21">
+        <v>42697</v>
+      </c>
+      <c r="C610" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D610" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E610" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="611" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A611" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B611" s="21">
+        <v>42697</v>
+      </c>
+      <c r="C611" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="D611" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E611" s="19" t="s">
+        <v>259</v>
+      </c>
+      <c r="F611" s="20" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="612" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A612" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B612" s="21">
+        <v>42697</v>
+      </c>
+      <c r="C612" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D612" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E612" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F612" s="20" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="613" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A613" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B613" s="21">
+        <v>42697</v>
+      </c>
+      <c r="C613" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D613" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E613" s="19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="614" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A614" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B614" s="21">
+        <v>42697</v>
+      </c>
+      <c r="C614" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="D614" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E614" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="F614" s="16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="615" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A615" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B615" s="21">
+        <v>42697</v>
+      </c>
+      <c r="C615" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="D615" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E615" s="19" t="s">
+        <v>259</v>
+      </c>
+      <c r="F615" s="20" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="616" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A616" s="6"/>
+      <c r="B616" s="23"/>
+      <c r="C616" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="D616" s="6"/>
+      <c r="E616" s="27"/>
+      <c r="F616" s="29"/>
+    </row>
+    <row r="617" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A617" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B617" s="21">
+        <v>42698</v>
+      </c>
+      <c r="C617" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D617" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E617" s="19" t="s">
+        <v>279</v>
+      </c>
+      <c r="F617" s="20" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="618" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A618" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B618" s="21">
+        <v>42698</v>
+      </c>
+      <c r="C618" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="D618" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E618" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="F618" s="20" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="619" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A619" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B619" s="21">
+        <v>42698</v>
+      </c>
+      <c r="C619" s="17" t="s">
+        <v>284</v>
+      </c>
+      <c r="D619" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="E619" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="F619" s="20" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="620" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A620" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B620" s="21">
+        <v>42696</v>
+      </c>
+      <c r="C620" s="17" t="s">
+        <v>284</v>
+      </c>
+      <c r="D620" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E620" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="F620" s="20" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="621" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A621" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B621" s="21">
+        <v>42696</v>
+      </c>
+      <c r="C621" s="17" t="s">
+        <v>284</v>
+      </c>
+      <c r="D621" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E621" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="F621" s="20" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="622" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A622" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B622" s="21">
+        <v>42698</v>
+      </c>
+      <c r="C622" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D622" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E622" s="19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="623" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A623" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B623" s="21">
+        <v>42698</v>
+      </c>
+      <c r="C623" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="D623" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E623" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F623" s="20" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="624" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A624" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B624" s="21">
+        <v>42698</v>
+      </c>
+      <c r="C624" s="17" t="s">
+        <v>253</v>
+      </c>
+      <c r="D624" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E624" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="F624" s="20" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="625" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A625" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B625" s="21">
+        <v>42698</v>
+      </c>
+      <c r="C625" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="D625" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="E625" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="F625" s="20" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="626" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A626" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B626" s="21">
+        <v>42698</v>
+      </c>
+      <c r="C626" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="D626" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E626" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="F626" s="16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="627" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A627" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B627" s="21">
+        <v>42698</v>
+      </c>
+      <c r="C627" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="D627" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E627" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="628" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A628" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B628" s="21">
+        <v>42698</v>
+      </c>
+      <c r="C628" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="D628" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E628" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F628" s="20" t="s">
+        <v>205</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0"/>
   <sortState ref="A427:G515">
@@ -13417,10 +13808,10 @@
     <sortCondition ref="D427:D515"/>
   </sortState>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A22:A23 B6 B2 A7:A8 B9 A10:A16 B17 A18:A20 B21 A3:A5 B24 A25:A27 B28 B32 A29:A31 A33:A34 B35 A36:A37 B38 A39:A53 B54 A55:A57 B58 A59:A63 B64 A65:A80 B81 A82:A85 B86 A87:A104 B105 A106:A109 B110 A111:A120 B121 A122:A133 B134 A135:A145 B146 A147:A176 B177 A178:A195 B196 A197:A203 B204 A205:A219 B220 A221:A227 B228 A229:A246 B247 A248:A264 B265 A266:A272 B273 A274:A278 B279 A280:A1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A22:A23 B6 B2 A7:A8 B9 A10:A16 B17 A18:A20 B21 A3:A5 B24 A25:A27 B28 B32 A29:A31 A33:A34 B35 A36:A37 B38 A39:A53 B54 A55:A57 B58 A59:A63 B64 A65:A80 B81 A82:A85 B86 A87:A104 B105 A106:A109 B110 A111:A120 B121 A122:A133 B134 A135:A145 B146 A147:A176 B177 A178:A195 B196 A197:A203 B204 A205:A219 B220 A221:A227 B228 A229:A246 B247 A248:A264 B265 A266:A272 B273 A274:A278 B279 A280:A628 A629:A1048576">
       <formula1>Task_type</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6 E2 D22:D23 D7:D8 E9 D10:D16 E17 D18:D20 E21 D3:D5 E24 D25:D27 E28 E32 D29:D31 D33:D34 E35 D36:D37 E38 D39:D53 E54 D55:D57 E58 D59:D63 E64 D65:D80 E81 D82:D85 E86 D87:D104 E105 D106:D109 E110 D111:D120 E121 D122:D133 E134 D135:D145 E146 D147:D176 E177 D178:D195 E196 D197:D203 E204 D205:D219 E220 D221:D227 E228 D229:D246 E247 D248:D264 E265 D266:D272 E273 D274:D278 E279 D280:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6 E2 D22:D23 D7:D8 E9 D10:D16 E17 D18:D20 E21 D3:D5 E24 D25:D27 E28 E32 D29:D31 D33:D34 E35 D36:D37 E38 D39:D53 E54 D55:D57 E58 D59:D63 E64 D65:D80 E81 D82:D85 E86 D87:D104 E105 D106:D109 E110 D111:D120 E121 D122:D133 E134 D135:D145 E146 D147:D176 E177 D178:D195 E196 D197:D203 E204 D205:D219 E220 D221:D227 E228 D229:D246 E247 D248:D264 E265 D266:D272 E273 D274:D278 E279 D280:D628 D629:D1048576">
       <formula1>Building</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 A2 A9 A17 A21 A24 A28 A32 A35 A38 A54 A58 A64 A81 A86 A105 A110 A121 A134 A146 A177 A196 A204 A220 A228 A247 A265 A273 A279">

</xml_diff>

<commit_message>
TODO: Finish work on the email login system
</commit_message>
<xml_diff>
--- a/CLASSOPS/Derek/Derek's Log.xlsx
+++ b/CLASSOPS/Derek/Derek's Log.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17426"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhan\Documents\Visual Studio 2015\Projects\ClassOpsLogCreator\CLASSOPS\Derek\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="90" yWindow="150" windowWidth="14865" windowHeight="10785" tabRatio="440"/>
   </bookViews>
@@ -22,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2819" uniqueCount="444">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2853" uniqueCount="445">
   <si>
     <t>Staff Name</t>
   </si>
@@ -1747,11 +1752,14 @@
   <si>
     <t>Pick up Skype camera with tripod and USB extension cable. Return to Vari 1019 MCR storeroom. BE ON TIME - CRUCIAL.</t>
   </si>
+  <si>
+    <t>Friday</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
@@ -1988,6 +1996,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -2035,7 +2046,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2068,9 +2079,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2103,6 +2131,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2282,11 +2327,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I628"/>
+  <dimension ref="A1:I636"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A614" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B635" sqref="B635"/>
+      <selection pane="bottomLeft" activeCell="B631" sqref="B631:B636"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13801,6 +13846,150 @@
         <v>205</v>
       </c>
     </row>
+    <row r="629" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A629" s="6"/>
+      <c r="B629" s="23"/>
+      <c r="C629" s="8" t="s">
+        <v>444</v>
+      </c>
+      <c r="D629" s="6"/>
+      <c r="E629" s="27"/>
+      <c r="F629" s="29"/>
+    </row>
+    <row r="630" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A630" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B630" s="21">
+        <v>42699</v>
+      </c>
+      <c r="C630" s="17" t="s">
+        <v>284</v>
+      </c>
+      <c r="D630" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E630" s="19" t="s">
+        <v>275</v>
+      </c>
+      <c r="F630" s="20" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="631" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A631" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B631" s="21">
+        <v>42699</v>
+      </c>
+      <c r="C631" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D631" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E631" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="632" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A632" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B632" s="21">
+        <v>42699</v>
+      </c>
+      <c r="C632" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="D632" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E632" s="19" t="s">
+        <v>259</v>
+      </c>
+      <c r="F632" s="20" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="633" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A633" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B633" s="21">
+        <v>42699</v>
+      </c>
+      <c r="C633" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D633" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E633" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F633" s="20" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="634" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A634" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B634" s="21">
+        <v>42699</v>
+      </c>
+      <c r="C634" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D634" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E634" s="19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="635" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A635" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B635" s="21">
+        <v>42699</v>
+      </c>
+      <c r="C635" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="D635" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E635" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="F635" s="16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="636" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A636" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B636" s="21">
+        <v>42699</v>
+      </c>
+      <c r="C636" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="D636" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E636" s="19" t="s">
+        <v>259</v>
+      </c>
+      <c r="F636" s="20" t="s">
+        <v>348</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0"/>
   <sortState ref="A427:G515">
@@ -13808,10 +13997,10 @@
     <sortCondition ref="D427:D515"/>
   </sortState>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A22:A23 B6 B2 A7:A8 B9 A10:A16 B17 A18:A20 B21 A3:A5 B24 A25:A27 B28 B32 A29:A31 A33:A34 B35 A36:A37 B38 A39:A53 B54 A55:A57 B58 A59:A63 B64 A65:A80 B81 A82:A85 B86 A87:A104 B105 A106:A109 B110 A111:A120 B121 A122:A133 B134 A135:A145 B146 A147:A176 B177 A178:A195 B196 A197:A203 B204 A205:A219 B220 A221:A227 B228 A229:A246 B247 A248:A264 B265 A266:A272 B273 A274:A278 B279 A280:A628 A629:A1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A22:A23 B6 B2 A7:A8 B9 A10:A16 B17 A18:A20 B21 A3:A5 B24 A25:A27 B28 B32 A29:A31 A33:A34 B35 A36:A37 B38 A39:A53 B54 A55:A57 B58 A59:A63 B64 A65:A80 B81 A82:A85 B86 A87:A104 B105 A106:A109 B110 A111:A120 B121 A122:A133 B134 A135:A145 B146 A147:A176 B177 A178:A195 B196 A197:A203 B204 A205:A219 B220 A221:A227 B228 A229:A246 B247 A248:A264 B265 A266:A272 B273 A274:A278 B279 A280:A1048576">
       <formula1>Task_type</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6 E2 D22:D23 D7:D8 E9 D10:D16 E17 D18:D20 E21 D3:D5 E24 D25:D27 E28 E32 D29:D31 D33:D34 E35 D36:D37 E38 D39:D53 E54 D55:D57 E58 D59:D63 E64 D65:D80 E81 D82:D85 E86 D87:D104 E105 D106:D109 E110 D111:D120 E121 D122:D133 E134 D135:D145 E146 D147:D176 E177 D178:D195 E196 D197:D203 E204 D205:D219 E220 D221:D227 E228 D229:D246 E247 D248:D264 E265 D266:D272 E273 D274:D278 E279 D280:D628 D629:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6 E2 D22:D23 D7:D8 E9 D10:D16 E17 D18:D20 E21 D3:D5 E24 D25:D27 E28 E32 D29:D31 D33:D34 E35 D36:D37 E38 D39:D53 E54 D55:D57 E58 D59:D63 E64 D65:D80 E81 D82:D85 E86 D87:D104 E105 D106:D109 E110 D111:D120 E121 D122:D133 E134 D135:D145 E146 D147:D176 E177 D178:D195 E196 D197:D203 E204 D205:D219 E220 D221:D227 E228 D229:D246 E247 D248:D264 E265 D266:D272 E273 D274:D278 E279 D280:D1048576">
       <formula1>Building</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 A2 A9 A17 A21 A24 A28 A32 A35 A38 A54 A58 A64 A81 A86 A105 A110 A121 A134 A146 A177 A196 A204 A220 A228 A247 A265 A273 A279">

</xml_diff>

<commit_message>
FIle update and testing
</commit_message>
<xml_diff>
--- a/CLASSOPS/Derek/Derek's Log.xlsx
+++ b/CLASSOPS/Derek/Derek's Log.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17426"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhan\Documents\Visual Studio 2015\Projects\ClassOpsLogCreator\CLASSOPS\Derek\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="90" yWindow="150" windowWidth="14865" windowHeight="10785" tabRatio="440"/>
   </bookViews>
@@ -27,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2853" uniqueCount="445">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2829" uniqueCount="444">
   <si>
     <t>Staff Name</t>
   </si>
@@ -1752,14 +1747,11 @@
   <si>
     <t>Pick up Skype camera with tripod and USB extension cable. Return to Vari 1019 MCR storeroom. BE ON TIME - CRUCIAL.</t>
   </si>
-  <si>
-    <t>Friday</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
@@ -1996,9 +1988,6 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -2046,7 +2035,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2079,26 +2068,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2131,23 +2103,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2327,11 +2282,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I636"/>
+  <dimension ref="A1:I631"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A614" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B631" sqref="B631:B636"/>
+      <selection pane="bottomLeft" activeCell="C635" sqref="C635"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13850,35 +13805,32 @@
       <c r="A629" s="6"/>
       <c r="B629" s="23"/>
       <c r="C629" s="8" t="s">
-        <v>444</v>
+        <v>139</v>
       </c>
       <c r="D629" s="6"/>
       <c r="E629" s="27"/>
       <c r="F629" s="29"/>
     </row>
-    <row r="630" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="630" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A630" s="10" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="B630" s="21">
         <v>42699</v>
       </c>
       <c r="C630" s="17" t="s">
-        <v>284</v>
+        <v>105</v>
       </c>
       <c r="D630" s="18" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="E630" s="19" t="s">
-        <v>275</v>
-      </c>
-      <c r="F630" s="20" t="s">
-        <v>443</v>
+        <v>108</v>
       </c>
     </row>
     <row r="631" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A631" s="10" t="s">
-        <v>80</v>
+        <v>19</v>
       </c>
       <c r="B631" s="21">
         <v>42699</v>
@@ -13886,108 +13838,14 @@
       <c r="C631" s="17" t="s">
         <v>207</v>
       </c>
-      <c r="D631" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="E631" s="19" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="632" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A632" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B632" s="21">
-        <v>42699</v>
-      </c>
-      <c r="C632" s="17" t="s">
-        <v>214</v>
-      </c>
-      <c r="D632" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="E632" s="19" t="s">
-        <v>259</v>
-      </c>
-      <c r="F632" s="20" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="633" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A633" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="B633" s="21">
-        <v>42699</v>
-      </c>
-      <c r="C633" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="D633" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="E633" s="19" t="s">
-        <v>136</v>
-      </c>
-      <c r="F633" s="20" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="634" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A634" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="B634" s="21">
-        <v>42699</v>
-      </c>
-      <c r="C634" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="D634" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="E634" s="19" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="635" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A635" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B635" s="21">
-        <v>42699</v>
-      </c>
-      <c r="C635" s="17" t="s">
-        <v>225</v>
-      </c>
-      <c r="D635" s="10" t="s">
+      <c r="D631" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="E635" s="15" t="s">
+      <c r="E631" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="F635" s="16" t="s">
+      <c r="F631" s="16" t="s">
         <v>128</v>
-      </c>
-    </row>
-    <row r="636" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A636" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B636" s="21">
-        <v>42699</v>
-      </c>
-      <c r="C636" s="17" t="s">
-        <v>243</v>
-      </c>
-      <c r="D636" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="E636" s="19" t="s">
-        <v>259</v>
-      </c>
-      <c r="F636" s="20" t="s">
-        <v>348</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Published onto version 1.1.0.0
</commit_message>
<xml_diff>
--- a/CLASSOPS/Derek/Derek's Log.xlsx
+++ b/CLASSOPS/Derek/Derek's Log.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2829" uniqueCount="444">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2923" uniqueCount="447">
   <si>
     <t>Staff Name</t>
   </si>
@@ -1746,6 +1746,15 @@
   </si>
   <si>
     <t>Pick up Skype camera with tripod and USB extension cable. Return to Vari 1019 MCR storeroom. BE ON TIME - CRUCIAL.</t>
+  </si>
+  <si>
+    <t>S102</t>
+  </si>
+  <si>
+    <t>Tutorial leader is Onyinechukwu Udeqbe.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -2282,11 +2291,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I631"/>
+  <dimension ref="A1:I656"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A614" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C635" sqref="C635"/>
+      <pane ySplit="1" topLeftCell="A630" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B645" sqref="B645:B652"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13848,6 +13857,402 @@
         <v>128</v>
       </c>
     </row>
+    <row r="632" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A632" s="6"/>
+      <c r="B632" s="23"/>
+      <c r="C632" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D632" s="6"/>
+      <c r="E632" s="27"/>
+      <c r="F632" s="29"/>
+    </row>
+    <row r="633" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A633" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B633" s="21">
+        <v>42702</v>
+      </c>
+      <c r="C633" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D633" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E633" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="F633" s="16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="634" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A634" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B634" s="21">
+        <v>42702</v>
+      </c>
+      <c r="C634" s="17" t="s">
+        <v>269</v>
+      </c>
+      <c r="D634" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E634" s="19" t="s">
+        <v>444</v>
+      </c>
+      <c r="F634" s="20" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="635" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A635" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B635" s="21">
+        <v>42702</v>
+      </c>
+      <c r="C635" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D635" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E635" s="19" t="s">
+        <v>279</v>
+      </c>
+      <c r="F635" s="20" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="636" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A636" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B636" s="21">
+        <v>42702</v>
+      </c>
+      <c r="C636" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="D636" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E636" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="637" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A637" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B637" s="21">
+        <v>42702</v>
+      </c>
+      <c r="C637" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="D637" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E637" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F637" s="20" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="638" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A638" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B638" s="21">
+        <v>42702</v>
+      </c>
+      <c r="C638" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="D638" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E638" s="19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="639" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A639" s="6"/>
+      <c r="B639" s="23"/>
+      <c r="C639" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D639" s="6"/>
+      <c r="E639" s="27"/>
+      <c r="F639" s="29"/>
+    </row>
+    <row r="640" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A640" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B640" s="21">
+        <v>42702</v>
+      </c>
+      <c r="C640" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D640" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E640" s="19" t="s">
+        <v>279</v>
+      </c>
+      <c r="F640" s="20" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="641" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A641" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B641" s="21">
+        <v>42702</v>
+      </c>
+      <c r="C641" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="D641" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E641" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="F641" s="20" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="642" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A642" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B642" s="21">
+        <v>42702</v>
+      </c>
+      <c r="C642" s="17" t="s">
+        <v>284</v>
+      </c>
+      <c r="D642" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="E642" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="F642" s="20" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="643" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A643" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B643" s="21">
+        <v>42696</v>
+      </c>
+      <c r="C643" s="17" t="s">
+        <v>284</v>
+      </c>
+      <c r="D643" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E643" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="F643" s="20" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="644" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A644" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B644" s="21">
+        <v>42696</v>
+      </c>
+      <c r="C644" s="17" t="s">
+        <v>284</v>
+      </c>
+      <c r="D644" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E644" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="F644" s="20" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="645" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A645" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B645" s="21">
+        <v>42702</v>
+      </c>
+      <c r="C645" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D645" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E645" s="19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="646" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A646" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B646" s="21">
+        <v>42702</v>
+      </c>
+      <c r="C646" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="D646" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E646" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F646" s="20" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="647" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A647" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B647" s="21">
+        <v>42702</v>
+      </c>
+      <c r="C647" s="17" t="s">
+        <v>253</v>
+      </c>
+      <c r="D647" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E647" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="F647" s="20" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="648" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A648" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B648" s="21">
+        <v>42702</v>
+      </c>
+      <c r="C648" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="D648" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="E648" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="F648" s="20" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="649" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A649" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B649" s="21">
+        <v>42702</v>
+      </c>
+      <c r="C649" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="D649" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E649" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="F649" s="16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="650" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A650" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B650" s="21">
+        <v>42702</v>
+      </c>
+      <c r="C650" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="D650" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E650" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="651" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A651" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B651" s="21">
+        <v>42702</v>
+      </c>
+      <c r="C651" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="D651" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E651" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F651" s="20" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="652" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A652" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B652" s="21">
+        <v>42702</v>
+      </c>
+      <c r="C652" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="D652" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E652" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F652" s="20" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="653" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A653" s="10" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="654" spans="1:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="655" spans="1:6" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="656" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0"/>
   <sortState ref="A427:G515">

</xml_diff>

<commit_message>
fixed a string bug
</commit_message>
<xml_diff>
--- a/CLASSOPS/Derek/Derek's Log.xlsx
+++ b/CLASSOPS/Derek/Derek's Log.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2923" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3079" uniqueCount="455">
   <si>
     <t>Staff Name</t>
   </si>
@@ -1754,7 +1754,123 @@
     <t>Tutorial leader is Onyinechukwu Udeqbe.</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <r>
+      <t xml:space="preserve">Use the PC cart from VC 040 storeroom that has the small PA underneath. Portable screen is there. Door code </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>7083*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Connect a neck mic and lectern mic to small PA under PC cart.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Leave portable screen and network cable. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Lock room and set the alarm if you know how</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. To Vanier 040 storeroom.</t>
+    </r>
+  </si>
+  <si>
+    <t>Unlock both hallway doors to the Nat Taylor Cinema.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">James Laxer wants to be shown how to play a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>streamed</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> video.</t>
+    </r>
+  </si>
+  <si>
+    <t>Return lectern mic, audience mic and stands, projector remote and presentation remote to back booth.</t>
+  </si>
+  <si>
+    <t>Neck mic, lectern mic and small PA under PC cart, cables, stand and carpets. To Vanier 040 storeroom.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Return web cam and tripod to Vari 1019, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>not Ross S120</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Return lectern mic, desk mic, neck mic and stands, projector remote and presentation remote to back booth.</t>
   </si>
 </sst>
 </file>
@@ -2291,11 +2407,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I656"/>
+  <dimension ref="A1:I690"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A630" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B645" sqref="B645:B652"/>
+      <pane ySplit="1" topLeftCell="A673" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B691" sqref="B691"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13581,7 +13697,7 @@
         <v>80</v>
       </c>
       <c r="B617" s="21">
-        <v>42698</v>
+        <v>42696</v>
       </c>
       <c r="C617" s="17" t="s">
         <v>105</v>
@@ -13972,7 +14088,7 @@
         <v>42702</v>
       </c>
       <c r="C638" s="17" t="s">
-        <v>226</v>
+        <v>243</v>
       </c>
       <c r="D638" s="18" t="s">
         <v>59</v>
@@ -13985,7 +14101,7 @@
       <c r="A639" s="6"/>
       <c r="B639" s="23"/>
       <c r="C639" s="8" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="D639" s="6"/>
       <c r="E639" s="27"/>
@@ -13996,127 +14112,124 @@
         <v>80</v>
       </c>
       <c r="B640" s="21">
-        <v>42702</v>
+        <v>42703</v>
       </c>
       <c r="C640" s="17" t="s">
         <v>105</v>
       </c>
       <c r="D640" s="18" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E640" s="19" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F640" s="20" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="641" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="641" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A641" s="10" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="B641" s="21">
-        <v>42702</v>
+        <v>42703</v>
       </c>
       <c r="C641" s="17" t="s">
-        <v>129</v>
+        <v>210</v>
       </c>
       <c r="D641" s="18" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="E641" s="19" t="s">
-        <v>149</v>
+        <v>411</v>
       </c>
       <c r="F641" s="20" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="642" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="642" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A642" s="10" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="B642" s="21">
-        <v>42702</v>
+        <v>42703</v>
       </c>
       <c r="C642" s="17" t="s">
-        <v>284</v>
+        <v>207</v>
       </c>
       <c r="D642" s="18" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="E642" s="19" t="s">
-        <v>163</v>
-      </c>
-      <c r="F642" s="20" t="s">
-        <v>432</v>
+        <v>106</v>
       </c>
     </row>
     <row r="643" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A643" s="10" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="B643" s="21">
-        <v>42696</v>
+        <v>42703</v>
       </c>
       <c r="C643" s="17" t="s">
-        <v>284</v>
+        <v>110</v>
       </c>
       <c r="D643" s="18" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E643" s="19" t="s">
-        <v>187</v>
+        <v>411</v>
       </c>
       <c r="F643" s="20" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
     </row>
     <row r="644" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A644" s="10" t="s">
-        <v>12</v>
+        <v>80</v>
       </c>
       <c r="B644" s="21">
-        <v>42696</v>
+        <v>42703</v>
       </c>
       <c r="C644" s="17" t="s">
-        <v>284</v>
+        <v>324</v>
       </c>
       <c r="D644" s="18" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="E644" s="19" t="s">
-        <v>187</v>
-      </c>
-      <c r="F644" s="20" t="s">
-        <v>439</v>
+        <v>108</v>
       </c>
     </row>
     <row r="645" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A645" s="10" t="s">
-        <v>80</v>
+        <v>19</v>
       </c>
       <c r="B645" s="21">
-        <v>42702</v>
+        <v>42703</v>
       </c>
       <c r="C645" s="17" t="s">
-        <v>207</v>
-      </c>
-      <c r="D645" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="E645" s="19" t="s">
-        <v>106</v>
+        <v>225</v>
+      </c>
+      <c r="D645" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E645" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="F645" s="16" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="646" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A646" s="10" t="s">
-        <v>19</v>
+        <v>80</v>
       </c>
       <c r="B646" s="21">
-        <v>42702</v>
+        <v>42703</v>
       </c>
       <c r="C646" s="17" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="D646" s="18" t="s">
         <v>59</v>
@@ -14125,67 +14238,54 @@
         <v>136</v>
       </c>
       <c r="F646" s="20" t="s">
-        <v>400</v>
+        <v>205</v>
       </c>
     </row>
     <row r="647" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A647" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="B647" s="21">
-        <v>42702</v>
-      </c>
-      <c r="C647" s="17" t="s">
-        <v>253</v>
-      </c>
-      <c r="D647" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="E647" s="19" t="s">
-        <v>187</v>
-      </c>
-      <c r="F647" s="20" t="s">
-        <v>442</v>
-      </c>
+      <c r="A647" s="6"/>
+      <c r="B647" s="23"/>
+      <c r="C647" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D647" s="6"/>
+      <c r="E647" s="27"/>
+      <c r="F647" s="29"/>
     </row>
     <row r="648" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A648" s="10" t="s">
         <v>93</v>
       </c>
       <c r="B648" s="21">
-        <v>42702</v>
+        <v>42704</v>
       </c>
       <c r="C648" s="17" t="s">
-        <v>225</v>
+        <v>284</v>
       </c>
       <c r="D648" s="18" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E648" s="19" t="s">
-        <v>163</v>
+        <v>275</v>
       </c>
       <c r="F648" s="20" t="s">
-        <v>380</v>
+        <v>443</v>
       </c>
     </row>
     <row r="649" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A649" s="10" t="s">
-        <v>19</v>
+        <v>80</v>
       </c>
       <c r="B649" s="21">
-        <v>42702</v>
+        <v>42704</v>
       </c>
       <c r="C649" s="17" t="s">
-        <v>225</v>
-      </c>
-      <c r="D649" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="E649" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="F649" s="16" t="s">
-        <v>128</v>
+        <v>207</v>
+      </c>
+      <c r="D649" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E649" s="19" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="650" spans="1:6" x14ac:dyDescent="0.25">
@@ -14193,16 +14293,19 @@
         <v>80</v>
       </c>
       <c r="B650" s="21">
-        <v>42702</v>
+        <v>42704</v>
       </c>
       <c r="C650" s="17" t="s">
-        <v>225</v>
+        <v>110</v>
       </c>
       <c r="D650" s="18" t="s">
         <v>59</v>
       </c>
       <c r="E650" s="19" t="s">
-        <v>108</v>
+        <v>136</v>
+      </c>
+      <c r="F650" s="20" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="651" spans="1:6" x14ac:dyDescent="0.25">
@@ -14210,49 +14313,727 @@
         <v>80</v>
       </c>
       <c r="B651" s="21">
-        <v>42702</v>
+        <v>42704</v>
       </c>
       <c r="C651" s="17" t="s">
-        <v>243</v>
+        <v>110</v>
       </c>
       <c r="D651" s="18" t="s">
         <v>59</v>
       </c>
       <c r="E651" s="19" t="s">
-        <v>136</v>
-      </c>
-      <c r="F651" s="20" t="s">
-        <v>205</v>
+        <v>106</v>
       </c>
     </row>
     <row r="652" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A652" s="10" t="s">
-        <v>80</v>
+        <v>19</v>
       </c>
       <c r="B652" s="21">
-        <v>42702</v>
+        <v>42704</v>
       </c>
       <c r="C652" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="D652" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E652" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="F652" s="16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="653" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A653" s="6"/>
+      <c r="B653" s="23"/>
+      <c r="C653" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="D653" s="6"/>
+      <c r="E653" s="27"/>
+      <c r="F653" s="29"/>
+    </row>
+    <row r="654" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A654" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B654" s="21">
+        <v>42705</v>
+      </c>
+      <c r="C654" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D654" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E654" s="19" t="s">
+        <v>279</v>
+      </c>
+      <c r="F654" s="20" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="655" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A655" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B655" s="21">
+        <v>42705</v>
+      </c>
+      <c r="C655" s="17" t="s">
+        <v>284</v>
+      </c>
+      <c r="D655" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="E655" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="F655" s="20" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="656" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A656" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B656" s="21">
+        <v>42705</v>
+      </c>
+      <c r="C656" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D656" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E656" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="F656" s="20" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="657" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A657" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B657" s="21">
+        <v>42705</v>
+      </c>
+      <c r="C657" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D657" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E657" s="19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="658" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A658" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B658" s="21">
+        <v>42705</v>
+      </c>
+      <c r="C658" s="17" t="s">
+        <v>384</v>
+      </c>
+      <c r="D658" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E658" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="F658" s="20" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="659" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A659" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B659" s="21">
+        <v>42705</v>
+      </c>
+      <c r="C659" s="17" t="s">
+        <v>384</v>
+      </c>
+      <c r="D659" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E659" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="F659" s="20" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="660" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A660" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B660" s="21">
+        <v>42705</v>
+      </c>
+      <c r="C660" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="D660" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E660" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F660" s="20" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="661" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A661" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B661" s="21">
+        <v>42705</v>
+      </c>
+      <c r="C661" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="D661" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E661" s="19" t="s">
+        <v>291</v>
+      </c>
+      <c r="F661" s="20" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="662" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A662" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B662" s="21">
+        <v>42705</v>
+      </c>
+      <c r="C662" s="17" t="s">
+        <v>253</v>
+      </c>
+      <c r="D662" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E662" s="19" t="s">
+        <v>277</v>
+      </c>
+      <c r="F662" s="20" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="663" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A663" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B663" s="21">
+        <v>42705</v>
+      </c>
+      <c r="C663" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="D663" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="E663" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="F663" s="20" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="664" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A664" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B664" s="21">
+        <v>42705</v>
+      </c>
+      <c r="C664" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="D664" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E664" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="F664" s="16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="665" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A665" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B665" s="21">
+        <v>42705</v>
+      </c>
+      <c r="C665" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="D665" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E665" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="666" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A666" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B666" s="21">
+        <v>42705</v>
+      </c>
+      <c r="C666" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="D666" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E666" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="F666" s="20" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="667" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A667" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B667" s="21">
+        <v>42705</v>
+      </c>
+      <c r="C667" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="D667" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E667" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="F667" s="20" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="668" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A668" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B668" s="21">
+        <v>42705</v>
+      </c>
+      <c r="C668" s="17" t="s">
         <v>243</v>
       </c>
-      <c r="D652" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="E652" s="19" t="s">
+      <c r="D668" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E668" s="19" t="s">
         <v>136</v>
       </c>
-      <c r="F652" s="20" t="s">
+      <c r="F668" s="20" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="653" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A653" s="10" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="654" spans="1:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="655" spans="1:6" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="656" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="669" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A669" s="6"/>
+      <c r="B669" s="23"/>
+      <c r="C669" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="D669" s="6"/>
+      <c r="E669" s="27"/>
+      <c r="F669" s="29"/>
+    </row>
+    <row r="670" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A670" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B670" s="21">
+        <v>42706</v>
+      </c>
+      <c r="C670" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D670" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E670" s="19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="671" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A671" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B671" s="21">
+        <v>42706</v>
+      </c>
+      <c r="C671" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D671" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E671" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="672" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A672" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B672" s="21">
+        <v>42706</v>
+      </c>
+      <c r="C672" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D672" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E672" s="19" t="s">
+        <v>381</v>
+      </c>
+      <c r="F672" s="14" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="673" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A673" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B673" s="21">
+        <v>42706</v>
+      </c>
+      <c r="C673" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D673" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E673" s="19" t="s">
+        <v>381</v>
+      </c>
+      <c r="F673" s="20" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="674" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A674" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B674" s="21">
+        <v>42706</v>
+      </c>
+      <c r="C674" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D674" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E674" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="F674" s="16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="675" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A675" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B675" s="21">
+        <v>42706</v>
+      </c>
+      <c r="C675" s="17" t="s">
+        <v>253</v>
+      </c>
+      <c r="D675" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E675" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F675" s="20" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="676" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A676" s="6"/>
+      <c r="B676" s="23"/>
+      <c r="C676" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D676" s="6"/>
+      <c r="E676" s="27"/>
+      <c r="F676" s="29"/>
+    </row>
+    <row r="677" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A677" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B677" s="21">
+        <v>42709</v>
+      </c>
+      <c r="C677" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D677" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E677" s="19" t="s">
+        <v>277</v>
+      </c>
+      <c r="F677" s="20" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="678" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A678" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B678" s="21">
+        <v>42709</v>
+      </c>
+      <c r="C678" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D678" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E678" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="F678" s="16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="679" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A679" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B679" s="21">
+        <v>42709</v>
+      </c>
+      <c r="C679" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D679" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E679" s="19" t="s">
+        <v>381</v>
+      </c>
+      <c r="F679" s="14" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="680" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A680" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B680" s="21">
+        <v>42709</v>
+      </c>
+      <c r="C680" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D680" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E680" s="19" t="s">
+        <v>381</v>
+      </c>
+      <c r="F680" s="20" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="681" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A681" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B681" s="21">
+        <v>42709</v>
+      </c>
+      <c r="C681" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D681" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E681" s="19" t="s">
+        <v>279</v>
+      </c>
+      <c r="F681" s="20" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="682" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A682" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B682" s="21">
+        <v>42709</v>
+      </c>
+      <c r="C682" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D682" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E682" s="19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="683" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A683" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B683" s="21">
+        <v>42709</v>
+      </c>
+      <c r="C683" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="D683" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E683" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="684" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A684" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B684" s="21">
+        <v>42709</v>
+      </c>
+      <c r="C684" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="D684" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E684" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F684" s="20" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="685" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A685" s="6"/>
+      <c r="B685" s="23"/>
+      <c r="C685" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="D685" s="6"/>
+      <c r="E685" s="27"/>
+      <c r="F685" s="29"/>
+    </row>
+    <row r="686" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A686" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B686" s="21">
+        <v>42710</v>
+      </c>
+      <c r="C686" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D686" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E686" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="687" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A687" s="6"/>
+      <c r="B687" s="23"/>
+      <c r="C687" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D687" s="6"/>
+      <c r="E687" s="27"/>
+      <c r="F687" s="29"/>
+    </row>
+    <row r="688" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A688" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B688" s="21">
+        <v>42711</v>
+      </c>
+      <c r="C688" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="D688" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E688" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="F688" s="20" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="689" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A689" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B689" s="21">
+        <v>42711</v>
+      </c>
+      <c r="C689" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="D689" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E689" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="F689" s="20" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="690" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A690" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B690" s="21">
+        <v>42711</v>
+      </c>
+      <c r="C690" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D690" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E690" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="F690" s="16" t="s">
+        <v>128</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0"/>
   <sortState ref="A427:G515">

</xml_diff>

<commit_message>
Files updates fixed a bug that would cause the system to crash if the time was incorrectly formated. Used a trim on the string to ensure no white space.
</commit_message>
<xml_diff>
--- a/CLASSOPS/Derek/Derek's Log.xlsx
+++ b/CLASSOPS/Derek/Derek's Log.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3079" uniqueCount="455">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3105" uniqueCount="456">
   <si>
     <t>Staff Name</t>
   </si>
@@ -1871,6 +1871,9 @@
   </si>
   <si>
     <t>Return lectern mic, desk mic, neck mic and stands, projector remote and presentation remote to back booth.</t>
+  </si>
+  <si>
+    <t>Return lectern mic, desk mic, neck and stands, projector remote and presentation remote to back booth.</t>
   </si>
 </sst>
 </file>
@@ -2407,11 +2410,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I690"/>
+  <dimension ref="A1:I696"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A673" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B691" sqref="B691"/>
+      <pane ySplit="1" topLeftCell="A674" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D699" sqref="D699"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15032,6 +15035,116 @@
       </c>
       <c r="F690" s="16" t="s">
         <v>128</v>
+      </c>
+    </row>
+    <row r="691" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A691" s="6"/>
+      <c r="B691" s="23"/>
+      <c r="C691" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="D691" s="6"/>
+      <c r="E691" s="27"/>
+      <c r="F691" s="29"/>
+    </row>
+    <row r="692" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A692" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B692" s="21">
+        <v>42712</v>
+      </c>
+      <c r="C692" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D692" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E692" s="19" t="s">
+        <v>277</v>
+      </c>
+      <c r="F692" s="20" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="693" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A693" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B693" s="21">
+        <v>42712</v>
+      </c>
+      <c r="C693" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D693" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E693" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="F693" s="16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="694" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A694" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B694" s="21">
+        <v>42712</v>
+      </c>
+      <c r="C694" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="D694" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E694" s="19" t="s">
+        <v>381</v>
+      </c>
+      <c r="F694" s="14" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="695" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A695" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B695" s="21">
+        <v>42712</v>
+      </c>
+      <c r="C695" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="D695" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E695" s="19" t="s">
+        <v>381</v>
+      </c>
+      <c r="F695" s="20" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="696" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A696" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B696" s="21">
+        <v>42712</v>
+      </c>
+      <c r="C696" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="D696" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E696" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="F696" s="20" t="s">
+        <v>455</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed a bug that would cause the CLO to not be updates if the feed is off by one day. Clear clipboard before pasting it into excel. Updates files.
</commit_message>
<xml_diff>
--- a/CLASSOPS/Derek/Derek's Log.xlsx
+++ b/CLASSOPS/Derek/Derek's Log.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3105" uniqueCount="456">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3214" uniqueCount="471">
   <si>
     <t>Staff Name</t>
   </si>
@@ -1874,6 +1874,51 @@
   </si>
   <si>
     <t>Return lectern mic, desk mic, neck and stands, projector remote and presentation remote to back booth.</t>
+  </si>
+  <si>
+    <t>Large screen TV in room already with PC. Just demo how to use equipment - client playing DVD disc thru PC with VLC.</t>
+  </si>
+  <si>
+    <t>Pick up large screen TV (DLP unit) with wireless keyboard and return to Vanier 132 storeroom (behind elevator). Go early so doesn't get locked in.</t>
+  </si>
+  <si>
+    <t>Log off crestron and return wireless keyboard to rack drawer.</t>
+  </si>
+  <si>
+    <t>1020</t>
+  </si>
+  <si>
+    <t>Make sure neck mic goes back to drawer - log off.</t>
+  </si>
+  <si>
+    <t>204</t>
+  </si>
+  <si>
+    <t>1158</t>
+  </si>
+  <si>
+    <t>Log off crestron.</t>
+  </si>
+  <si>
+    <t>Log off crestron and return neck mic to drawer.</t>
+  </si>
+  <si>
+    <t>050A</t>
+  </si>
+  <si>
+    <t>050B</t>
+  </si>
+  <si>
+    <t>050C</t>
+  </si>
+  <si>
+    <t>114</t>
+  </si>
+  <si>
+    <t>115</t>
+  </si>
+  <si>
+    <t>116</t>
   </si>
 </sst>
 </file>
@@ -2410,11 +2455,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I696"/>
+  <dimension ref="A1:I721"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A674" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D699" sqref="D699"/>
+      <pane ySplit="1" topLeftCell="A692" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F717" sqref="F717"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15145,6 +15190,460 @@
       </c>
       <c r="F696" s="20" t="s">
         <v>455</v>
+      </c>
+    </row>
+    <row r="697" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A697" s="6"/>
+      <c r="B697" s="23"/>
+      <c r="C697" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="D697" s="6"/>
+      <c r="E697" s="27"/>
+      <c r="F697" s="29"/>
+    </row>
+    <row r="698" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A698" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B698" s="21">
+        <v>42713</v>
+      </c>
+      <c r="C698" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="D698" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E698" s="19" t="s">
+        <v>310</v>
+      </c>
+      <c r="F698" s="20" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="699" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A699" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B699" s="21">
+        <v>42713</v>
+      </c>
+      <c r="C699" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="D699" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E699" s="19" t="s">
+        <v>310</v>
+      </c>
+      <c r="F699" s="20" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="700" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A700" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B700" s="21">
+        <v>42713</v>
+      </c>
+      <c r="C700" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D700" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E700" s="19" t="s">
+        <v>275</v>
+      </c>
+      <c r="F700" s="20" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="701" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A701" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B701" s="21">
+        <v>42713</v>
+      </c>
+      <c r="C701" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D701" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E701" s="19" t="s">
+        <v>291</v>
+      </c>
+      <c r="F701" s="20" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="702" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A702" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B702" s="21">
+        <v>42713</v>
+      </c>
+      <c r="C702" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D702" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E702" s="19" t="s">
+        <v>459</v>
+      </c>
+      <c r="F702" s="20" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="703" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A703" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B703" s="21">
+        <v>42713</v>
+      </c>
+      <c r="C703" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D703" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E703" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="F703" s="20" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="704" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A704" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B704" s="21">
+        <v>42713</v>
+      </c>
+      <c r="C704" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D704" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="E704" s="19" t="s">
+        <v>200</v>
+      </c>
+      <c r="F704" s="20" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="705" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A705" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B705" s="21">
+        <v>42713</v>
+      </c>
+      <c r="C705" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D705" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E705" s="19" t="s">
+        <v>461</v>
+      </c>
+      <c r="F705" s="20" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="706" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A706" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B706" s="21">
+        <v>42713</v>
+      </c>
+      <c r="C706" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D706" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E706" s="19" t="s">
+        <v>462</v>
+      </c>
+      <c r="F706" s="20" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="707" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A707" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B707" s="21">
+        <v>42713</v>
+      </c>
+      <c r="C707" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D707" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E707" s="19" t="s">
+        <v>411</v>
+      </c>
+      <c r="F707" s="20" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="708" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A708" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B708" s="21">
+        <v>42713</v>
+      </c>
+      <c r="C708" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D708" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E708" s="19" t="s">
+        <v>191</v>
+      </c>
+      <c r="F708" s="20" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="709" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A709" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B709" s="21">
+        <v>42713</v>
+      </c>
+      <c r="C709" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D709" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E709" s="19" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="710" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A710" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B710" s="21">
+        <v>42713</v>
+      </c>
+      <c r="C710" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D710" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E710" s="19" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="711" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A711" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B711" s="21">
+        <v>42713</v>
+      </c>
+      <c r="C711" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D711" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E711" s="19" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="712" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A712" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B712" s="21">
+        <v>42713</v>
+      </c>
+      <c r="C712" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="D712" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E712" s="19" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="713" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A713" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B713" s="21">
+        <v>42713</v>
+      </c>
+      <c r="C713" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="D713" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E713" s="19" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="714" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A714" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B714" s="21">
+        <v>42713</v>
+      </c>
+      <c r="C714" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D714" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E714" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="F714" s="16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="715" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A715" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B715" s="21">
+        <v>42713</v>
+      </c>
+      <c r="C715" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D715" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="E715" s="19" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="716" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A716" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B716" s="21">
+        <v>42713</v>
+      </c>
+      <c r="C716" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="D716" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E716" s="19" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="717" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A717" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B717" s="21">
+        <v>42713</v>
+      </c>
+      <c r="C717" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="D717" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E717" s="19" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="718" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A718" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B718" s="21">
+        <v>42713</v>
+      </c>
+      <c r="C718" s="17" t="s">
+        <v>253</v>
+      </c>
+      <c r="D718" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E718" s="19" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="719" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A719" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B719" s="21">
+        <v>42713</v>
+      </c>
+      <c r="C719" s="17" t="s">
+        <v>253</v>
+      </c>
+      <c r="D719" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E719" s="19" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="720" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A720" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B720" s="21">
+        <v>42713</v>
+      </c>
+      <c r="C720" s="17" t="s">
+        <v>253</v>
+      </c>
+      <c r="D720" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E720" s="19" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="721" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A721" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B721" s="21">
+        <v>42713</v>
+      </c>
+      <c r="C721" s="17" t="s">
+        <v>253</v>
+      </c>
+      <c r="D721" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E721" s="19" t="s">
+        <v>273</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a Excel Kill method that fires off at the start of the application execution. Created a work around when the zone super logs have blank rows at the end of the file. Cleared the clipboard once completed.
</commit_message>
<xml_diff>
--- a/CLASSOPS/Derek/Derek's Log.xlsx
+++ b/CLASSOPS/Derek/Derek's Log.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3214" uniqueCount="471">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3275" uniqueCount="475">
   <si>
     <t>Staff Name</t>
   </si>
@@ -1919,6 +1919,18 @@
   </si>
   <si>
     <t>116</t>
+  </si>
+  <si>
+    <t>Meet Professor Lawrence Lam.</t>
+  </si>
+  <si>
+    <t>Meet Professor Xiaofeng Zhou</t>
+  </si>
+  <si>
+    <t>Log in and route the DVD player so it's ready to play for T. Conlin.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Return lectern mic, audience mic, stands, projector remote and presentation remote to back booth. There is an additional neck microphone that needs to be picked up as well. </t>
   </si>
 </sst>
 </file>
@@ -2455,11 +2467,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I721"/>
+  <dimension ref="A1:I736"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A692" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F717" sqref="F717"/>
+      <pane ySplit="1" topLeftCell="A713" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F736" sqref="F736"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15629,7 +15641,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="721" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="721" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A721" s="10" t="s">
         <v>80</v>
       </c>
@@ -15644,6 +15656,270 @@
       </c>
       <c r="E721" s="19" t="s">
         <v>273</v>
+      </c>
+    </row>
+    <row r="722" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A722" s="6"/>
+      <c r="B722" s="23"/>
+      <c r="C722" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="D722" s="6"/>
+      <c r="E722" s="27"/>
+      <c r="F722" s="29"/>
+    </row>
+    <row r="723" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A723" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B723" s="21">
+        <v>42738</v>
+      </c>
+      <c r="C723" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D723" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E723" s="19" t="s">
+        <v>277</v>
+      </c>
+      <c r="F723" s="20" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="724" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A724" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B724" s="21">
+        <v>42738</v>
+      </c>
+      <c r="C724" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D724" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E724" s="19" t="s">
+        <v>381</v>
+      </c>
+      <c r="F724" s="14" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="725" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A725" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B725" s="21">
+        <v>42738</v>
+      </c>
+      <c r="C725" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D725" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E725" s="19" t="s">
+        <v>381</v>
+      </c>
+      <c r="F725" s="20" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="726" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A726" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B726" s="21">
+        <v>42738</v>
+      </c>
+      <c r="C726" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D726" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E726" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="F726" s="16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="727" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A727" s="6"/>
+      <c r="B727" s="23"/>
+      <c r="C727" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D727" s="6"/>
+      <c r="E727" s="27"/>
+      <c r="F727" s="29"/>
+    </row>
+    <row r="728" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A728" s="6"/>
+      <c r="B728" s="23"/>
+      <c r="C728" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="D728" s="6"/>
+      <c r="E728" s="27"/>
+      <c r="F728" s="29"/>
+    </row>
+    <row r="729" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A729" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B729" s="21">
+        <v>42740</v>
+      </c>
+      <c r="C729" s="17" t="s">
+        <v>210</v>
+      </c>
+      <c r="D729" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E729" s="19" t="s">
+        <v>425</v>
+      </c>
+      <c r="F729" s="20" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="730" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A730" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B730" s="21">
+        <v>42740</v>
+      </c>
+      <c r="C730" s="17" t="s">
+        <v>269</v>
+      </c>
+      <c r="D730" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E730" s="19" t="s">
+        <v>202</v>
+      </c>
+      <c r="F730" s="20" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="731" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A731" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B731" s="21">
+        <v>42740</v>
+      </c>
+      <c r="C731" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D731" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E731" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="F731" s="16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="732" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A732" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B732" s="21">
+        <v>42740</v>
+      </c>
+      <c r="C732" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D732" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E732" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="F732" s="20" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="733" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A733" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B733" s="21">
+        <v>42740</v>
+      </c>
+      <c r="C733" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D733" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E733" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F733" s="20" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="734" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A734" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B734" s="21">
+        <v>42740</v>
+      </c>
+      <c r="C734" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D734" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E734" s="19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="735" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A735" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B735" s="21">
+        <v>42740</v>
+      </c>
+      <c r="C735" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D735" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E735" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="736" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A736" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B736" s="21">
+        <v>42740</v>
+      </c>
+      <c r="C736" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="D736" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E736" s="19" t="s">
+        <v>217</v>
+      </c>
+      <c r="F736" s="20" t="s">
+        <v>472</v>
       </c>
     </row>
   </sheetData>
@@ -15653,10 +15929,10 @@
     <sortCondition ref="D427:D515"/>
   </sortState>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A22:A23 B6 B2 A7:A8 B9 A10:A16 B17 A18:A20 B21 A3:A5 B24 A25:A27 B28 B32 A29:A31 A33:A34 B35 A36:A37 B38 A39:A53 B54 A55:A57 B58 A59:A63 B64 A65:A80 B81 A82:A85 B86 A87:A104 B105 A106:A109 B110 A111:A120 B121 A122:A133 B134 A135:A145 B146 A147:A176 B177 A178:A195 B196 A197:A203 B204 A205:A219 B220 A221:A227 B228 A229:A246 B247 A248:A264 B265 A266:A272 B273 A274:A278 B279 A280:A1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A22:A23 B6 B2 A7:A8 B9 A10:A16 B17 A18:A20 B21 A3:A5 B24 A25:A27 B28 B32 A29:A31 A33:A34 B35 A36:A37 B38 A39:A53 B54 A55:A57 B58 A59:A63 B64 A65:A80 B81 A82:A85 B86 A87:A104 B105 A106:A109 B110 A111:A120 B121 A122:A133 B134 A135:A145 B146 A147:A176 B177 A178:A195 B196 A197:A203 B204 A205:A219 B220 A221:A227 B228 A229:A246 B247 A248:A264 B265 A266:A272 B273 A274:A278 B279 A280:A736 A737:A1048576">
       <formula1>Task_type</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6 E2 D22:D23 D7:D8 E9 D10:D16 E17 D18:D20 E21 D3:D5 E24 D25:D27 E28 E32 D29:D31 D33:D34 E35 D36:D37 E38 D39:D53 E54 D55:D57 E58 D59:D63 E64 D65:D80 E81 D82:D85 E86 D87:D104 E105 D106:D109 E110 D111:D120 E121 D122:D133 E134 D135:D145 E146 D147:D176 E177 D178:D195 E196 D197:D203 E204 D205:D219 E220 D221:D227 E228 D229:D246 E247 D248:D264 E265 D266:D272 E273 D274:D278 E279 D280:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6 E2 D22:D23 D7:D8 E9 D10:D16 E17 D18:D20 E21 D3:D5 E24 D25:D27 E28 E32 D29:D31 D33:D34 E35 D36:D37 E38 D39:D53 E54 D55:D57 E58 D59:D63 E64 D65:D80 E81 D82:D85 E86 D87:D104 E105 D106:D109 E110 D111:D120 E121 D122:D133 E134 D135:D145 E146 D147:D176 E177 D178:D195 E196 D197:D203 E204 D205:D219 E220 D221:D227 E228 D229:D246 E247 D248:D264 E265 D266:D272 E273 D274:D278 E279 D280:D736 D737:D1048576">
       <formula1>Building</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 A2 A9 A17 A21 A24 A28 A32 A35 A38 A54 A58 A64 A81 A86 A105 A110 A121 A134 A146 A177 A196 A204 A220 A228 A247 A265 A273 A279">

</xml_diff>

<commit_message>
Update files, more test runs.
</commit_message>
<xml_diff>
--- a/CLASSOPS/Derek/Derek's Log.xlsx
+++ b/CLASSOPS/Derek/Derek's Log.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3275" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3281" uniqueCount="475">
   <si>
     <t>Staff Name</t>
   </si>
@@ -2467,11 +2467,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I736"/>
+  <dimension ref="A1:I738"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A713" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F736" sqref="F736"/>
+      <pane ySplit="1" topLeftCell="A716" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B739" sqref="B739"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15922,6 +15922,36 @@
         <v>472</v>
       </c>
     </row>
+    <row r="737" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A737" s="6"/>
+      <c r="B737" s="23"/>
+      <c r="C737" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="D737" s="6"/>
+      <c r="E737" s="27"/>
+      <c r="F737" s="29"/>
+    </row>
+    <row r="738" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A738" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B738" s="21">
+        <v>42741</v>
+      </c>
+      <c r="C738" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D738" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E738" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="F738" s="16" t="s">
+        <v>128</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0"/>
   <sortState ref="A427:G515">
@@ -15929,10 +15959,10 @@
     <sortCondition ref="D427:D515"/>
   </sortState>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A22:A23 B6 B2 A7:A8 B9 A10:A16 B17 A18:A20 B21 A3:A5 B24 A25:A27 B28 B32 A29:A31 A33:A34 B35 A36:A37 B38 A39:A53 B54 A55:A57 B58 A59:A63 B64 A65:A80 B81 A82:A85 B86 A87:A104 B105 A106:A109 B110 A111:A120 B121 A122:A133 B134 A135:A145 B146 A147:A176 B177 A178:A195 B196 A197:A203 B204 A205:A219 B220 A221:A227 B228 A229:A246 B247 A248:A264 B265 A266:A272 B273 A274:A278 B279 A280:A736 A737:A1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A22:A23 B6 B2 A7:A8 B9 A10:A16 B17 A18:A20 B21 A3:A5 B24 A25:A27 B28 B32 A29:A31 A33:A34 B35 A36:A37 B38 A39:A53 B54 A55:A57 B58 A59:A63 B64 A65:A80 B81 A82:A85 B86 A87:A104 B105 A106:A109 B110 A111:A120 B121 A122:A133 B134 A135:A145 B146 A147:A176 B177 A178:A195 B196 A197:A203 B204 A205:A219 B220 A221:A227 B228 A229:A246 B247 A248:A264 B265 A266:A272 B273 A274:A278 B279 A280:A1048576">
       <formula1>Task_type</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6 E2 D22:D23 D7:D8 E9 D10:D16 E17 D18:D20 E21 D3:D5 E24 D25:D27 E28 E32 D29:D31 D33:D34 E35 D36:D37 E38 D39:D53 E54 D55:D57 E58 D59:D63 E64 D65:D80 E81 D82:D85 E86 D87:D104 E105 D106:D109 E110 D111:D120 E121 D122:D133 E134 D135:D145 E146 D147:D176 E177 D178:D195 E196 D197:D203 E204 D205:D219 E220 D221:D227 E228 D229:D246 E247 D248:D264 E265 D266:D272 E273 D274:D278 E279 D280:D736 D737:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6 E2 D22:D23 D7:D8 E9 D10:D16 E17 D18:D20 E21 D3:D5 E24 D25:D27 E28 E32 D29:D31 D33:D34 E35 D36:D37 E38 D39:D53 E54 D55:D57 E58 D59:D63 E64 D65:D80 E81 D82:D85 E86 D87:D104 E105 D106:D109 E110 D111:D120 E121 D122:D133 E134 D135:D145 E146 D147:D176 E177 D178:D195 E196 D197:D203 E204 D205:D219 E220 D221:D227 E228 D229:D246 E247 D248:D264 E265 D266:D272 E273 D274:D278 E279 D280:D1048576">
       <formula1>Building</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 A2 A9 A17 A21 A24 A28 A32 A35 A38 A54 A58 A64 A81 A86 A105 A110 A121 A134 A146 A177 A196 A204 A220 A228 A247 A265 A273 A279">

</xml_diff>

<commit_message>
File updated, permissions reset, fixed an email bug sending to the wrong account.
</commit_message>
<xml_diff>
--- a/CLASSOPS/Derek/Derek's Log.xlsx
+++ b/CLASSOPS/Derek/Derek's Log.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3281" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3345" uniqueCount="484">
   <si>
     <t>Staff Name</t>
   </si>
@@ -1931,6 +1931,33 @@
   </si>
   <si>
     <t xml:space="preserve">Return lectern mic, audience mic, stands, projector remote and presentation remote to back booth. There is an additional neck microphone that needs to be picked up as well. </t>
+  </si>
+  <si>
+    <t>Meet instructor Sanjeev Dhuga</t>
+  </si>
+  <si>
+    <t>Meet instructor Douglas McCready</t>
+  </si>
+  <si>
+    <t>1650</t>
+  </si>
+  <si>
+    <t>140</t>
+  </si>
+  <si>
+    <t>PC and neck mic is there.  Demo for Khan Le. Door code 7083*</t>
+  </si>
+  <si>
+    <t>Meet instructor Susan Ehrlich</t>
+  </si>
+  <si>
+    <t>Meet instructor Karen Murray</t>
+  </si>
+  <si>
+    <t>Meet instructor Jill Prindiville</t>
+  </si>
+  <si>
+    <t>Leave portable screen. Door code 7083* return to FDRS 156A.</t>
   </si>
 </sst>
 </file>
@@ -2467,11 +2494,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I738"/>
+  <dimension ref="A1:I752"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A716" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B739" sqref="B739"/>
+      <pane ySplit="1" topLeftCell="A728" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A752" sqref="A752"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15950,6 +15977,270 @@
       </c>
       <c r="F738" s="16" t="s">
         <v>128</v>
+      </c>
+    </row>
+    <row r="739" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A739" s="6"/>
+      <c r="B739" s="23"/>
+      <c r="C739" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D739" s="6"/>
+      <c r="E739" s="27"/>
+      <c r="F739" s="29"/>
+    </row>
+    <row r="740" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A740" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B740" s="21">
+        <v>42744</v>
+      </c>
+      <c r="C740" s="17" t="s">
+        <v>210</v>
+      </c>
+      <c r="D740" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E740" s="19" t="s">
+        <v>462</v>
+      </c>
+      <c r="F740" s="20" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="741" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A741" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B741" s="21">
+        <v>42744</v>
+      </c>
+      <c r="C741" s="17" t="s">
+        <v>210</v>
+      </c>
+      <c r="D741" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E741" s="19" t="s">
+        <v>191</v>
+      </c>
+      <c r="F741" s="20" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="742" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A742" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B742" s="21">
+        <v>42744</v>
+      </c>
+      <c r="C742" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D742" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E742" s="19" t="s">
+        <v>279</v>
+      </c>
+      <c r="F742" s="20" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="743" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A743" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B743" s="21">
+        <v>42744</v>
+      </c>
+      <c r="C743" s="17" t="s">
+        <v>477</v>
+      </c>
+      <c r="D743" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E743" s="19" t="s">
+        <v>478</v>
+      </c>
+      <c r="F743" s="20" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="744" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A744" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B744" s="21">
+        <v>42744</v>
+      </c>
+      <c r="C744" s="17" t="s">
+        <v>368</v>
+      </c>
+      <c r="D744" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E744" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="F744" s="20" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="745" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A745" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B745" s="21">
+        <v>42744</v>
+      </c>
+      <c r="C745" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D745" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E745" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="F745" s="16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="746" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A746" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B746" s="21">
+        <v>42744</v>
+      </c>
+      <c r="C746" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D746" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E746" s="19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="747" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A747" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B747" s="21">
+        <v>42744</v>
+      </c>
+      <c r="C747" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="D747" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E747" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="748" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A748" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B748" s="21">
+        <v>42744</v>
+      </c>
+      <c r="C748" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="D748" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E748" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F748" s="20" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="749" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A749" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B749" s="21">
+        <v>42744</v>
+      </c>
+      <c r="C749" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="D749" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E749" s="19" t="s">
+        <v>257</v>
+      </c>
+      <c r="F749" s="20" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="750" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A750" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B750" s="21">
+        <v>42744</v>
+      </c>
+      <c r="C750" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="D750" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="E750" s="19" t="s">
+        <v>199</v>
+      </c>
+      <c r="F750" s="20" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="751" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A751" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B751" s="21">
+        <v>42744</v>
+      </c>
+      <c r="C751" s="17" t="s">
+        <v>324</v>
+      </c>
+      <c r="D751" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E751" s="19" t="s">
+        <v>478</v>
+      </c>
+      <c r="F751" s="20" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="752" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A752" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B752" s="21">
+        <v>42744</v>
+      </c>
+      <c r="C752" s="17" t="s">
+        <v>324</v>
+      </c>
+      <c r="D752" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E752" s="19" t="s">
+        <v>478</v>
+      </c>
+      <c r="F752" s="20" t="s">
+        <v>405</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Testing more methods for the copy paste erros
</commit_message>
<xml_diff>
--- a/CLASSOPS/Derek/Derek's Log.xlsx
+++ b/CLASSOPS/Derek/Derek's Log.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3345" uniqueCount="484">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3539" uniqueCount="499">
   <si>
     <t>Staff Name</t>
   </si>
@@ -1958,6 +1958,51 @@
   </si>
   <si>
     <t>Leave portable screen. Door code 7083* return to FDRS 156A.</t>
+  </si>
+  <si>
+    <t>East Bear Pit</t>
+  </si>
+  <si>
+    <t>3 wired mics, neck mic, stands, projector remote and presentation remote to back booth.</t>
+  </si>
+  <si>
+    <t>Web cam and tripod to Ross S120.</t>
+  </si>
+  <si>
+    <t>Meet instructor who shall remain nameless for the moment.</t>
+  </si>
+  <si>
+    <t>3009</t>
+  </si>
+  <si>
+    <t>3 flat screen TVs, wireless keyboards (turn off), 2 TV remotes and extension cords. Two of the PC's have wireless network receivers attached, the other is hard wired to the wall jack.  Return all to Vari 1155 and connect all 3 PC's to wired internet router there.</t>
+  </si>
+  <si>
+    <t>Return lectern mic, 2 desk mics, stands, projector remote and presentation remote to back booth.</t>
+  </si>
+  <si>
+    <t>Meet instructor Asma Sidddiqi</t>
+  </si>
+  <si>
+    <t>Meet instructor Carole Bigwood.  Monitor cutting out?</t>
+  </si>
+  <si>
+    <t>No mics were used. Pc and projector only.</t>
+  </si>
+  <si>
+    <t>Pick up amplifier, 2 speaker cables and 2 large speakers. Return to Van 040 basement storeroom.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pick up all matts and ac cords and return to Van 040 basement. Key for room in Fdrs 164 storeroom keyrack. </t>
+  </si>
+  <si>
+    <t>Built in PC not working - roll in PC cart in room going thru document camera input. Press "Doc cam" to "Projector to get image on screen. Demo to prof.</t>
+  </si>
+  <si>
+    <t>Pick up roll in PC and return to Vari 1019 storeroom.</t>
+  </si>
+  <si>
+    <t>Open up Nat Taylor cinema.</t>
   </si>
 </sst>
 </file>
@@ -2494,11 +2539,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I752"/>
+  <dimension ref="A1:I797"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A728" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A752" sqref="A752"/>
+      <pane ySplit="1" topLeftCell="A778" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F800" sqref="F800"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16241,6 +16286,825 @@
       </c>
       <c r="F752" s="20" t="s">
         <v>405</v>
+      </c>
+    </row>
+    <row r="753" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A753" s="6"/>
+      <c r="B753" s="23"/>
+      <c r="C753" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="D753" s="6"/>
+      <c r="E753" s="27"/>
+      <c r="F753" s="29"/>
+    </row>
+    <row r="754" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A754" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B754" s="21">
+        <v>42745</v>
+      </c>
+      <c r="C754" s="17" t="s">
+        <v>210</v>
+      </c>
+      <c r="D754" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E754" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="F754" s="20" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="755" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A755" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B755" s="21">
+        <v>42745</v>
+      </c>
+      <c r="C755" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D755" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E755" s="19" t="s">
+        <v>177</v>
+      </c>
+      <c r="F755" s="20" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="756" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A756" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B756" s="21">
+        <v>42745</v>
+      </c>
+      <c r="C756" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D756" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E756" s="19" t="s">
+        <v>279</v>
+      </c>
+      <c r="F756" s="20" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="757" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A757" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B757" s="21">
+        <v>42745</v>
+      </c>
+      <c r="C757" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D757" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E757" s="19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="758" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A758" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B758" s="21">
+        <v>42745</v>
+      </c>
+      <c r="C758" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="D758" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E758" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="F758" s="16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="759" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A759" s="6"/>
+      <c r="B759" s="23"/>
+      <c r="C759" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D759" s="6"/>
+      <c r="E759" s="27"/>
+      <c r="F759" s="29"/>
+    </row>
+    <row r="760" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A760" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B760" s="21">
+        <v>42746</v>
+      </c>
+      <c r="C760" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D760" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="E760" s="19" t="s">
+        <v>484</v>
+      </c>
+      <c r="F760" s="20" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="761" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A761" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B761" s="21">
+        <v>42746</v>
+      </c>
+      <c r="C761" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="D761" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E761" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="F761" s="20" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="762" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A762" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B762" s="21">
+        <v>42746</v>
+      </c>
+      <c r="C762" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="D762" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E762" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="F762" s="20" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="763" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A763" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B763" s="21">
+        <v>42746</v>
+      </c>
+      <c r="C763" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="D763" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E763" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="F763" s="20" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="764" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A764" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B764" s="21">
+        <v>42746</v>
+      </c>
+      <c r="C764" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="D764" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E764" s="19" t="s">
+        <v>488</v>
+      </c>
+      <c r="F764" s="20" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="765" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A765" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B765" s="21">
+        <v>42746</v>
+      </c>
+      <c r="C765" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D765" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E765" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F765" s="20" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="766" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A766" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B766" s="21">
+        <v>42746</v>
+      </c>
+      <c r="C766" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="D766" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E766" s="19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="767" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A767" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B767" s="21">
+        <v>42746</v>
+      </c>
+      <c r="C767" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="D767" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E767" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="F767" s="16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="768" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A768" s="6"/>
+      <c r="B768" s="23"/>
+      <c r="C768" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="D768" s="6"/>
+      <c r="E768" s="27"/>
+      <c r="F768" s="29"/>
+    </row>
+    <row r="769" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A769" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B769" s="21">
+        <v>42747</v>
+      </c>
+      <c r="C769" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D769" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E769" s="19" t="s">
+        <v>177</v>
+      </c>
+      <c r="F769" s="20" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="770" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A770" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B770" s="21">
+        <v>42747</v>
+      </c>
+      <c r="C770" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D770" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E770" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="F770" s="16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="771" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A771" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B771" s="21">
+        <v>42747</v>
+      </c>
+      <c r="C771" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D771" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E771" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F771" s="20" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="772" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A772" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B772" s="21">
+        <v>42747</v>
+      </c>
+      <c r="C772" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="D772" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E772" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="F772" s="20" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="773" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A773" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B773" s="21">
+        <v>42747</v>
+      </c>
+      <c r="C773" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D773" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E773" s="19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="774" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A774" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B774" s="21">
+        <v>42747</v>
+      </c>
+      <c r="C774" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D774" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E774" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="775" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A775" s="6"/>
+      <c r="B775" s="23"/>
+      <c r="C775" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="D775" s="6"/>
+      <c r="E775" s="27"/>
+      <c r="F775" s="29"/>
+    </row>
+    <row r="776" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A776" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B776" s="21">
+        <v>42748</v>
+      </c>
+      <c r="C776" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D776" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E776" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="F776" s="16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="777" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A777" s="6"/>
+      <c r="B777" s="23"/>
+      <c r="C777" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D777" s="6"/>
+      <c r="E777" s="27"/>
+      <c r="F777" s="29"/>
+    </row>
+    <row r="778" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A778" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B778" s="21">
+        <v>42751</v>
+      </c>
+      <c r="C778" s="17" t="s">
+        <v>269</v>
+      </c>
+      <c r="D778" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E778" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="F778" s="20" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="779" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A779" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B779" s="21">
+        <v>42751</v>
+      </c>
+      <c r="C779" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D779" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E779" s="19" t="s">
+        <v>279</v>
+      </c>
+      <c r="F779" s="20" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="780" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A780" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B780" s="21">
+        <v>42751</v>
+      </c>
+      <c r="C780" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D780" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E780" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="F780" s="20" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="781" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A781" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B781" s="21">
+        <v>42751</v>
+      </c>
+      <c r="C781" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D781" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E781" s="19" t="s">
+        <v>272</v>
+      </c>
+      <c r="F781" s="20" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="782" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A782" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B782" s="21">
+        <v>42751</v>
+      </c>
+      <c r="C782" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D782" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E782" s="19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="783" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A783" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B783" s="21">
+        <v>42751</v>
+      </c>
+      <c r="C783" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="D783" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E783" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="784" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A784" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B784" s="21">
+        <v>42751</v>
+      </c>
+      <c r="C784" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="D784" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E784" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F784" s="20" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="785" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A785" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B785" s="21">
+        <v>42751</v>
+      </c>
+      <c r="C785" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="D785" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E785" s="19" t="s">
+        <v>191</v>
+      </c>
+      <c r="F785" s="20" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="786" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A786" s="6"/>
+      <c r="B786" s="23"/>
+      <c r="C786" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="D786" s="6"/>
+      <c r="E786" s="27"/>
+      <c r="F786" s="29"/>
+    </row>
+    <row r="787" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A787" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B787" s="21">
+        <v>42752</v>
+      </c>
+      <c r="C787" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D787" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E787" s="19" t="s">
+        <v>279</v>
+      </c>
+      <c r="F787" s="20" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="788" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A788" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B788" s="21">
+        <v>42752</v>
+      </c>
+      <c r="C788" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D788" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E788" s="19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="789" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A789" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B789" s="21">
+        <v>42752</v>
+      </c>
+      <c r="C789" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="D789" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E789" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="F789" s="16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="790" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A790" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B790" s="21">
+        <v>42752</v>
+      </c>
+      <c r="C790" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D790" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E790" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="F790" s="20" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="791" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A791" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B791" s="21">
+        <v>42752</v>
+      </c>
+      <c r="C791" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D791" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E791" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="F791" s="20" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="792" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A792" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B792" s="21">
+        <v>42752</v>
+      </c>
+      <c r="C792" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D792" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E792" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="F792" s="20" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="793" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A793" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B793" s="21">
+        <v>42752</v>
+      </c>
+      <c r="C793" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D793" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E793" s="19" t="s">
+        <v>199</v>
+      </c>
+      <c r="F793" s="20" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="794" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A794" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B794" s="21">
+        <v>42752</v>
+      </c>
+      <c r="C794" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D794" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E794" s="19" t="s">
+        <v>199</v>
+      </c>
+      <c r="F794" s="20" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="795" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A795" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B795" s="21">
+        <v>42752</v>
+      </c>
+      <c r="C795" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="D795" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E795" s="19" t="s">
+        <v>199</v>
+      </c>
+      <c r="F795" s="20" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="796" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A796" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B796" s="21">
+        <v>42752</v>
+      </c>
+      <c r="C796" s="17" t="s">
+        <v>185</v>
+      </c>
+      <c r="D796" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E796" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F796" s="20" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="797" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A797" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B797" s="21">
+        <v>42752</v>
+      </c>
+      <c r="C797" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="D797" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E797" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F797" s="20" t="s">
+        <v>205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ready for a build. all new features tested and ready.
</commit_message>
<xml_diff>
--- a/CLASSOPS/Derek/Derek's Log.xlsx
+++ b/CLASSOPS/Derek/Derek's Log.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17571"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhan\Documents\Visual Studio 2015\Projects\ClassOpsLogCreator\CLASSOPS\Derek\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="90" yWindow="150" windowWidth="14865" windowHeight="10785" tabRatio="440"/>
   </bookViews>
@@ -22,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3539" uniqueCount="499">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3613" uniqueCount="507">
   <si>
     <t>Staff Name</t>
   </si>
@@ -2004,11 +2009,35 @@
   <si>
     <t>Open up Nat Taylor cinema.</t>
   </si>
+  <si>
+    <t>Projector remote and presentation remote to back booth. No mics.</t>
+  </si>
+  <si>
+    <t>Rotunda</t>
+  </si>
+  <si>
+    <t>Flat screen TV, with PC,wireless keyboard and extension cord. Turn off wireless keyboard and place in the bag before transporting to Vari 1155. Connect ethernet cable to PC in 1155.</t>
+  </si>
+  <si>
+    <t>001-D.H.</t>
+  </si>
+  <si>
+    <t>Event starts at 6pm. No mics needed. Client is playing music from another source. They have their own auxilliary cable. Get from Vanier 040 storeroom.</t>
+  </si>
+  <si>
+    <t>Carpets, cables, tripods etc. Return to Vanier 040 storeroom.</t>
+  </si>
+  <si>
+    <t>Meet instructor Chima Osakwe. No one showed up last week.</t>
+  </si>
+  <si>
+    <t>Cart PC is connected to laptop input. Disconnect and bring to Vari 1155 with orange ext. cord. Put VGA cable and internet cable back in the drawer of Vari A.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
@@ -2245,6 +2274,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -2292,7 +2324,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2325,9 +2357,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2360,6 +2409,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2539,11 +2605,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I797"/>
+  <dimension ref="A1:I815"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A778" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F800" sqref="F800"/>
+      <pane ySplit="1" topLeftCell="A807" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A815" sqref="A815"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16927,29 +16993,29 @@
         <v>106</v>
       </c>
     </row>
-    <row r="789" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="789" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A789" s="10" t="s">
-        <v>19</v>
+        <v>91</v>
       </c>
       <c r="B789" s="21">
         <v>42752</v>
       </c>
       <c r="C789" s="17" t="s">
-        <v>225</v>
-      </c>
-      <c r="D789" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D789" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="E789" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="F789" s="16" t="s">
-        <v>128</v>
+      <c r="E789" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="F789" s="20" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="790" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A790" s="10" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="B790" s="21">
         <v>42752</v>
@@ -16964,12 +17030,12 @@
         <v>158</v>
       </c>
       <c r="F790" s="20" t="s">
-        <v>354</v>
+        <v>494</v>
       </c>
     </row>
     <row r="791" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A791" s="10" t="s">
-        <v>82</v>
+        <v>19</v>
       </c>
       <c r="B791" s="21">
         <v>42752</v>
@@ -16984,27 +17050,27 @@
         <v>158</v>
       </c>
       <c r="F791" s="20" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="792" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="792" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A792" s="10" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B792" s="21">
         <v>42752</v>
       </c>
       <c r="C792" s="17" t="s">
-        <v>105</v>
+        <v>133</v>
       </c>
       <c r="D792" s="18" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E792" s="19" t="s">
-        <v>158</v>
+        <v>199</v>
       </c>
       <c r="F792" s="20" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
     </row>
     <row r="793" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -17015,7 +17081,7 @@
         <v>42752</v>
       </c>
       <c r="C793" s="17" t="s">
-        <v>133</v>
+        <v>110</v>
       </c>
       <c r="D793" s="18" t="s">
         <v>51</v>
@@ -17027,15 +17093,15 @@
         <v>496</v>
       </c>
     </row>
-    <row r="794" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="794" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A794" s="10" t="s">
-        <v>12</v>
+        <v>87</v>
       </c>
       <c r="B794" s="21">
         <v>42752</v>
       </c>
       <c r="C794" s="17" t="s">
-        <v>110</v>
+        <v>226</v>
       </c>
       <c r="D794" s="18" t="s">
         <v>51</v>
@@ -17044,38 +17110,38 @@
         <v>199</v>
       </c>
       <c r="F794" s="20" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
     </row>
     <row r="795" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A795" s="10" t="s">
-        <v>87</v>
+        <v>19</v>
       </c>
       <c r="B795" s="21">
         <v>42752</v>
       </c>
       <c r="C795" s="17" t="s">
-        <v>226</v>
+        <v>185</v>
       </c>
       <c r="D795" s="18" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="E795" s="19" t="s">
-        <v>199</v>
+        <v>136</v>
       </c>
       <c r="F795" s="20" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
     </row>
     <row r="796" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A796" s="10" t="s">
-        <v>19</v>
+        <v>80</v>
       </c>
       <c r="B796" s="21">
         <v>42752</v>
       </c>
       <c r="C796" s="17" t="s">
-        <v>185</v>
+        <v>226</v>
       </c>
       <c r="D796" s="18" t="s">
         <v>59</v>
@@ -17084,27 +17150,345 @@
         <v>136</v>
       </c>
       <c r="F796" s="20" t="s">
-        <v>498</v>
+        <v>205</v>
       </c>
     </row>
     <row r="797" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A797" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="B797" s="21">
-        <v>42752</v>
-      </c>
-      <c r="C797" s="17" t="s">
-        <v>226</v>
-      </c>
-      <c r="D797" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="E797" s="19" t="s">
+      <c r="A797" s="6"/>
+      <c r="B797" s="23"/>
+      <c r="C797" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D797" s="6"/>
+      <c r="E797" s="27"/>
+      <c r="F797" s="29"/>
+    </row>
+    <row r="798" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A798" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B798" s="21">
+        <v>42753</v>
+      </c>
+      <c r="C798" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D798" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E798" s="19" t="s">
+        <v>500</v>
+      </c>
+      <c r="F798" s="20" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="799" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A799" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B799" s="21">
+        <v>42753</v>
+      </c>
+      <c r="C799" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D799" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="E799" s="19" t="s">
+        <v>502</v>
+      </c>
+      <c r="F799" s="20" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="800" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A800" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B800" s="21">
+        <v>42753</v>
+      </c>
+      <c r="C800" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D800" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E800" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="F800" s="20" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="801" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A801" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B801" s="21">
+        <v>42753</v>
+      </c>
+      <c r="C801" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="D801" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E801" s="19" t="s">
+        <v>199</v>
+      </c>
+      <c r="F801" s="20" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="802" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A802" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B802" s="21">
+        <v>42753</v>
+      </c>
+      <c r="C802" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="D802" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E802" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="F802" s="20" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="803" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A803" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B803" s="21">
+        <v>42753</v>
+      </c>
+      <c r="C803" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D803" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E803" s="19" t="s">
         <v>136</v>
       </c>
-      <c r="F797" s="20" t="s">
+      <c r="F803" s="20" t="s">
         <v>205</v>
+      </c>
+    </row>
+    <row r="804" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A804" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B804" s="21">
+        <v>42753</v>
+      </c>
+      <c r="C804" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D804" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E804" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="805" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A805" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B805" s="21">
+        <v>42753</v>
+      </c>
+      <c r="C805" s="17" t="s">
+        <v>253</v>
+      </c>
+      <c r="D805" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="E805" s="19" t="s">
+        <v>502</v>
+      </c>
+      <c r="F805" s="20" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="806" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A806" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B806" s="21">
+        <v>42753</v>
+      </c>
+      <c r="C806" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="D806" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E806" s="19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="807" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A807" s="6"/>
+      <c r="B807" s="23"/>
+      <c r="C807" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="D807" s="6"/>
+      <c r="E807" s="27"/>
+      <c r="F807" s="29"/>
+    </row>
+    <row r="808" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A808" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B808" s="21">
+        <v>42754</v>
+      </c>
+      <c r="C808" s="17" t="s">
+        <v>284</v>
+      </c>
+      <c r="D808" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="E808" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="F808" s="20" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="809" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A809" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B809" s="21">
+        <v>42754</v>
+      </c>
+      <c r="C809" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D809" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E809" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F809" s="20" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="810" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A810" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B810" s="21">
+        <v>42754</v>
+      </c>
+      <c r="C810" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="D810" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E810" s="19" t="s">
+        <v>277</v>
+      </c>
+      <c r="F810" s="20" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="811" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A811" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B811" s="21">
+        <v>42754</v>
+      </c>
+      <c r="C811" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D811" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E811" s="19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="812" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A812" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B812" s="21">
+        <v>42754</v>
+      </c>
+      <c r="C812" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D812" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E812" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="813" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A813" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B813" s="21">
+        <v>42754</v>
+      </c>
+      <c r="C813" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="D813" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="E813" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="F813" s="20" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="814" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A814" s="6"/>
+      <c r="B814" s="23"/>
+      <c r="C814" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="D814" s="6"/>
+      <c r="E814" s="27"/>
+      <c r="F814" s="29"/>
+    </row>
+    <row r="815" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A815" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B815" s="21">
+        <v>42755</v>
+      </c>
+      <c r="C815" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D815" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E815" s="19" t="s">
+        <v>289</v>
+      </c>
+      <c r="F815" s="20" t="s">
+        <v>380</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update files and put into test mode
</commit_message>
<xml_diff>
--- a/CLASSOPS/Derek/Derek's Log.xlsx
+++ b/CLASSOPS/Derek/Derek's Log.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17571"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhan\Documents\Visual Studio 2015\Projects\ClassOpsLogCreator\CLASSOPS\Derek\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="90" yWindow="150" windowWidth="14865" windowHeight="10785" tabRatio="440"/>
   </bookViews>
@@ -27,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3613" uniqueCount="507">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3890" uniqueCount="533">
   <si>
     <t>Staff Name</t>
   </si>
@@ -2033,15 +2028,162 @@
   <si>
     <t>Cart PC is connected to laptop input. Disconnect and bring to Vari 1155 with orange ext. cord. Put VGA cable and internet cable back in the drawer of Vari A.</t>
   </si>
+  <si>
+    <t>Meet Jill Prindiville. No one showed for her demo on Jan. 9th.</t>
+  </si>
+  <si>
+    <t>S757</t>
+  </si>
+  <si>
+    <t>Includes portable screen. To Vanier 040 storeroom.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Pick up webcam with tripod and USB extension cable </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>if supplied</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Return to FDRS 164. BE ON TIME - CRUCIAL.</t>
+    </r>
+  </si>
+  <si>
+    <t>Amplifier, speakers, cables and carpets. To Vanier 040 storeroom.</t>
+  </si>
+  <si>
+    <t>Neck mic. To Vanier 040 storeroom with large PA.</t>
+  </si>
+  <si>
+    <t>Turn off PA system. Computer not used.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">3 desk mics, 1 neck mic, audio mixer, carpets, stands, cables, but </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>not</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the cable to the lectern area. To FDRS 156A</t>
+    </r>
+  </si>
+  <si>
+    <t>Log in and demo the DVD player so it's ready to play for Terry Conlin. Note: This is a repeating request for assistance. Make sure the DVD operation is fully understood by the professor.</t>
+  </si>
+  <si>
+    <t>Meet Bahar Nasirzadeh.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Includes portable screen. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Lock room and set the alarm if you know how</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. To Vanier 040 store.</t>
+    </r>
+  </si>
+  <si>
+    <t>Event starts at 6pm. Need portable screen also from Vanier 040.</t>
+  </si>
+  <si>
+    <t>Return lectern mic, 2 desk mics, stands, projector remote and presentation remote to back booth. Lock room-both entrances.</t>
+  </si>
+  <si>
+    <t>SET UP FROM VC 040</t>
+  </si>
+  <si>
+    <t>Return to VC 040</t>
+  </si>
+  <si>
+    <t>Pick up the small PA + wireless mic on a cart, return to FC 156A</t>
+  </si>
+  <si>
+    <t>Return lectern mic, 2 desk mics, 2 audience mics, stands, projector remote and presentation remote to back audio booth. Lock booth and both exits when leaving.</t>
+  </si>
+  <si>
+    <t>Flat screen TV and extension cord goes back to Vari 1155. Use care when going through doorways to avoid scratching the TV screen. Check that the wireless keyboard is turned off before transporting in the bag. Check that the TV remote is in the bag also.</t>
+  </si>
+  <si>
+    <t>Lectern mic and small PA under PC cart, cables, stand and carpets. To Vanier 040 storeroom.</t>
+  </si>
+  <si>
+    <t>N783</t>
+  </si>
+  <si>
+    <t>Meet Marie-Christine Pioffet. Needs assistance playing a DVD.</t>
+  </si>
+  <si>
+    <t>Flat screen TV and extension cord goes back to Vari 1155. Reconnect the ethernet cable from the router to the PC in 1155.Use care when going through doorways to avoid scratching the TV screen. Check that the wireless keyboard is turned off before transporting in the bag. Check that the TV remote is in the bag also.  Be on time. Room may be locked if you are late.</t>
+  </si>
+  <si>
+    <t>2230</t>
+  </si>
+  <si>
+    <t>Meet Steve Chan. Wants to hook his laptop up to use Skype.</t>
+  </si>
+  <si>
+    <t>Flat screen TV, wireless keyboard, TV remote, ethernet cable and extension cord. Turn off wireless keyboard and place in the bag before transporting to Vari 1155. Reconnect ethernet cable to the PC from the router and plug into power once inside 1155.</t>
+  </si>
+  <si>
+    <t>Pickup web cam and triod. Return kit to SLH 114L MCR.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2083,6 +2225,13 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2172,7 +2321,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2262,6 +2411,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
@@ -2273,9 +2443,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -2324,7 +2491,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2357,26 +2524,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2409,23 +2559,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2605,11 +2738,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I815"/>
+  <dimension ref="A1:I879"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A807" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A815" sqref="A815"/>
+      <pane ySplit="1" topLeftCell="A857" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B873" sqref="B873"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17489,6 +17622,1173 @@
       </c>
       <c r="F815" s="20" t="s">
         <v>380</v>
+      </c>
+    </row>
+    <row r="816" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A816" s="6"/>
+      <c r="B816" s="23"/>
+      <c r="C816" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D816" s="6"/>
+      <c r="E816" s="27"/>
+      <c r="F816" s="29"/>
+    </row>
+    <row r="817" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A817" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B817" s="21">
+        <v>42758</v>
+      </c>
+      <c r="C817" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D817" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E817" s="19" t="s">
+        <v>279</v>
+      </c>
+      <c r="F817" s="20" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="818" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A818" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B818" s="21">
+        <v>42758</v>
+      </c>
+      <c r="C818" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="D818" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E818" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="F818" s="20" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="819" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A819" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B819" s="21">
+        <v>42758</v>
+      </c>
+      <c r="C819" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D819" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E819" s="19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="820" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A820" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B820" s="21">
+        <v>42758</v>
+      </c>
+      <c r="C820" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="D820" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E820" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="821" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A821" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B821" s="21">
+        <v>42758</v>
+      </c>
+      <c r="C821" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="D821" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E821" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F821" s="20" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="822" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A822" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B822" s="21">
+        <v>42758</v>
+      </c>
+      <c r="C822" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="D822" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="E822" s="19" t="s">
+        <v>199</v>
+      </c>
+      <c r="F822" s="20" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="823" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A823" s="6"/>
+      <c r="B823" s="23"/>
+      <c r="C823" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="D823" s="6"/>
+      <c r="E823" s="27"/>
+      <c r="F823" s="29"/>
+    </row>
+    <row r="824" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A824" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B824" s="21">
+        <v>42759</v>
+      </c>
+      <c r="C824" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D824" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E824" s="19" t="s">
+        <v>277</v>
+      </c>
+      <c r="F824" s="20" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="825" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A825" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B825" s="21">
+        <v>42759</v>
+      </c>
+      <c r="C825" s="17" t="s">
+        <v>368</v>
+      </c>
+      <c r="D825" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E825" s="19" t="s">
+        <v>508</v>
+      </c>
+      <c r="F825" s="20" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="826" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A826" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B826" s="21">
+        <v>42759</v>
+      </c>
+      <c r="C826" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D826" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E826" s="19" t="s">
+        <v>279</v>
+      </c>
+      <c r="F826" s="20" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="827" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A827" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B827" s="21">
+        <v>42759</v>
+      </c>
+      <c r="C827" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D827" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E827" s="19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="828" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A828" s="6"/>
+      <c r="B828" s="23"/>
+      <c r="C828" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D828" s="6"/>
+      <c r="E828" s="27"/>
+      <c r="F828" s="29"/>
+    </row>
+    <row r="829" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A829" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B829" s="21">
+        <v>42760</v>
+      </c>
+      <c r="C829" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D829" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E829" s="19" t="s">
+        <v>263</v>
+      </c>
+      <c r="F829" s="20" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="830" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A830" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B830" s="21">
+        <v>42760</v>
+      </c>
+      <c r="C830" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D830" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E830" s="19" t="s">
+        <v>263</v>
+      </c>
+      <c r="F830" s="20" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="831" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A831" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B831" s="21">
+        <v>42760</v>
+      </c>
+      <c r="C831" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D831" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E831" s="19" t="s">
+        <v>263</v>
+      </c>
+      <c r="F831" s="20" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="832" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A832" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B832" s="21">
+        <v>42705</v>
+      </c>
+      <c r="C832" s="17" t="s">
+        <v>284</v>
+      </c>
+      <c r="D832" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E832" s="19" t="s">
+        <v>466</v>
+      </c>
+      <c r="F832" s="20" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="833" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A833" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B833" s="21">
+        <v>42760</v>
+      </c>
+      <c r="C833" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D833" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E833" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F833" s="20" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="834" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A834" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B834" s="21">
+        <v>42760</v>
+      </c>
+      <c r="C834" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D834" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E834" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="835" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A835" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B835" s="21">
+        <v>42760</v>
+      </c>
+      <c r="C835" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="D835" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E835" s="19" t="s">
+        <v>466</v>
+      </c>
+      <c r="F835" s="20" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="836" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A836" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B836" s="21">
+        <v>42760</v>
+      </c>
+      <c r="C836" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="D836" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E836" s="19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="837" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A837" s="6"/>
+      <c r="B837" s="23"/>
+      <c r="C837" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="D837" s="6"/>
+      <c r="E837" s="27"/>
+      <c r="F837" s="29"/>
+    </row>
+    <row r="838" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A838" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B838" s="21">
+        <v>42761</v>
+      </c>
+      <c r="C838" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D838" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E838" s="19" t="s">
+        <v>381</v>
+      </c>
+      <c r="F838" s="20" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="839" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A839" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B839" s="21">
+        <v>42761</v>
+      </c>
+      <c r="C839" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D839" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E839" s="19" t="s">
+        <v>381</v>
+      </c>
+      <c r="F839" s="20" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="840" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A840" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B840" s="21">
+        <v>42761</v>
+      </c>
+      <c r="C840" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D840" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E840" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="841" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A841" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B841" s="21">
+        <v>42761</v>
+      </c>
+      <c r="C841" s="17" t="s">
+        <v>269</v>
+      </c>
+      <c r="D841" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E841" s="19" t="s">
+        <v>202</v>
+      </c>
+      <c r="F841" s="20" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="842" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A842" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B842" s="21">
+        <v>42761</v>
+      </c>
+      <c r="C842" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="D842" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E842" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="F842" s="20" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="843" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A843" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B843" s="21">
+        <v>42761</v>
+      </c>
+      <c r="C843" s="17" t="s">
+        <v>368</v>
+      </c>
+      <c r="D843" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E843" s="19" t="s">
+        <v>275</v>
+      </c>
+      <c r="F843" s="20" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="844" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A844" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B844" s="21">
+        <v>42761</v>
+      </c>
+      <c r="C844" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D844" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E844" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F844" s="20" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="845" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A845" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B845" s="21">
+        <v>42761</v>
+      </c>
+      <c r="C845" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D845" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E845" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="F845" s="20" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="846" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A846" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B846" s="21">
+        <v>42761</v>
+      </c>
+      <c r="C846" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D846" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E846" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="F846" s="20" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="847" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A847" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B847" s="21">
+        <v>42761</v>
+      </c>
+      <c r="C847" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D847" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E847" s="19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="848" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A848" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B848" s="21">
+        <v>42761</v>
+      </c>
+      <c r="C848" s="17" t="s">
+        <v>362</v>
+      </c>
+      <c r="D848" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E848" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="F848" s="20" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="849" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A849" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B849" s="21">
+        <v>42761</v>
+      </c>
+      <c r="C849" s="17" t="s">
+        <v>362</v>
+      </c>
+      <c r="D849" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E849" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="F849" s="20" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="850" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A850" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="B850" s="21">
+        <v>42761</v>
+      </c>
+      <c r="C850" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D850" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E850" s="19" t="s">
+        <v>296</v>
+      </c>
+      <c r="F850" s="20" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="851" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A851" s="6"/>
+      <c r="B851" s="23"/>
+      <c r="C851" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="D851" s="6"/>
+      <c r="E851" s="27"/>
+      <c r="F851" s="29"/>
+    </row>
+    <row r="852" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A852" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B852" s="21">
+        <v>42762</v>
+      </c>
+      <c r="C852" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D852" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E852" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="F852" s="20" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="853" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A853" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B853" s="21">
+        <v>42762</v>
+      </c>
+      <c r="C853" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D853" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E853" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="F853" s="20" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="854" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A854" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B854" s="21">
+        <v>42762</v>
+      </c>
+      <c r="C854" s="17" t="s">
+        <v>253</v>
+      </c>
+      <c r="D854" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E854" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="F854" s="20" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="855" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A855" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B855" s="21">
+        <v>42762</v>
+      </c>
+      <c r="C855" s="17" t="s">
+        <v>253</v>
+      </c>
+      <c r="D855" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E855" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="F855" s="20" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="856" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A856" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B856" s="21">
+        <v>42762</v>
+      </c>
+      <c r="C856" s="17" t="s">
+        <v>253</v>
+      </c>
+      <c r="D856" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E856" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="F856" s="20" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="857" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A857" s="6"/>
+      <c r="B857" s="23"/>
+      <c r="C857" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D857" s="6"/>
+      <c r="E857" s="27"/>
+      <c r="F857" s="29"/>
+    </row>
+    <row r="858" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A858" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B858" s="21">
+        <v>42765</v>
+      </c>
+      <c r="C858" s="17" t="s">
+        <v>210</v>
+      </c>
+      <c r="D858" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E858" s="19" t="s">
+        <v>298</v>
+      </c>
+      <c r="F858" s="20" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="859" spans="1:6" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A859" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B859" s="21">
+        <v>42765</v>
+      </c>
+      <c r="C859" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D859" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E859" s="19" t="s">
+        <v>526</v>
+      </c>
+      <c r="F859" s="20" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="860" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A860" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B860" s="21">
+        <v>42765</v>
+      </c>
+      <c r="C860" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D860" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E860" s="19" t="s">
+        <v>279</v>
+      </c>
+      <c r="F860" s="20" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="861" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A861" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B861" s="21">
+        <v>42765</v>
+      </c>
+      <c r="C861" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D861" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E861" s="19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="862" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A862" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B862" s="21">
+        <v>42765</v>
+      </c>
+      <c r="C862" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="D862" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E862" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="863" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A863" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B863" s="21">
+        <v>42765</v>
+      </c>
+      <c r="C863" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="D863" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E863" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F863" s="20" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="864" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A864" s="6"/>
+      <c r="B864" s="23"/>
+      <c r="C864" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="D864" s="6"/>
+      <c r="E864" s="27"/>
+      <c r="F864" s="29"/>
+    </row>
+    <row r="865" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A865" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B865" s="21">
+        <v>42766</v>
+      </c>
+      <c r="C865" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D865" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E865" s="19" t="s">
+        <v>277</v>
+      </c>
+      <c r="F865" s="20" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="866" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A866" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B866" s="21">
+        <v>42766</v>
+      </c>
+      <c r="C866" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D866" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="E866" s="19" t="s">
+        <v>191</v>
+      </c>
+      <c r="F866" s="20" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="867" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A867" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B867" s="21">
+        <v>42766</v>
+      </c>
+      <c r="C867" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D867" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E867" s="19" t="s">
+        <v>279</v>
+      </c>
+      <c r="F867" s="20" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="868" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A868" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B868" s="21">
+        <v>42766</v>
+      </c>
+      <c r="C868" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="D868" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="E868" s="19" t="s">
+        <v>246</v>
+      </c>
+      <c r="F868" s="20" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="869" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A869" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B869" s="21">
+        <v>42766</v>
+      </c>
+      <c r="C869" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D869" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E869" s="19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="870" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A870" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B870" s="21">
+        <v>42766</v>
+      </c>
+      <c r="C870" s="17" t="s">
+        <v>253</v>
+      </c>
+      <c r="D870" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E870" s="19" t="s">
+        <v>275</v>
+      </c>
+      <c r="F870" s="20" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="871" spans="1:6" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A871" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="B871" s="34">
+        <v>42766</v>
+      </c>
+      <c r="C871" s="35" t="s">
+        <v>529</v>
+      </c>
+      <c r="D871" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="E871" s="37" t="s">
+        <v>136</v>
+      </c>
+      <c r="F871" s="38" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="872" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A872" s="6"/>
+      <c r="B872" s="23"/>
+      <c r="C872" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="D872" s="6"/>
+      <c r="E872" s="27"/>
+      <c r="F872" s="29"/>
+    </row>
+    <row r="873" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A873" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B873" s="21">
+        <v>42766</v>
+      </c>
+      <c r="C873" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D873" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E873" s="19" t="s">
+        <v>277</v>
+      </c>
+      <c r="F873" s="20" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="874" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A874" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B874" s="21">
+        <v>42766</v>
+      </c>
+      <c r="C874" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D874" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="E874" s="19" t="s">
+        <v>191</v>
+      </c>
+      <c r="F874" s="20" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="875" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A875" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B875" s="21">
+        <v>42766</v>
+      </c>
+      <c r="C875" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D875" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E875" s="19" t="s">
+        <v>279</v>
+      </c>
+      <c r="F875" s="20" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="876" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A876" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B876" s="21">
+        <v>42766</v>
+      </c>
+      <c r="C876" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="D876" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="E876" s="19" t="s">
+        <v>246</v>
+      </c>
+      <c r="F876" s="20" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="877" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A877" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B877" s="21">
+        <v>42766</v>
+      </c>
+      <c r="C877" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D877" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E877" s="19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="878" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A878" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B878" s="21">
+        <v>42766</v>
+      </c>
+      <c r="C878" s="17" t="s">
+        <v>253</v>
+      </c>
+      <c r="D878" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E878" s="19" t="s">
+        <v>275</v>
+      </c>
+      <c r="F878" s="20" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="879" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A879" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B879" s="34">
+        <v>42766</v>
+      </c>
+      <c r="C879" s="35" t="s">
+        <v>529</v>
+      </c>
+      <c r="D879" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="E879" s="37" t="s">
+        <v>136</v>
+      </c>
+      <c r="F879" s="38" t="s">
+        <v>271</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update to version 1.1.5 and updated files.
</commit_message>
<xml_diff>
--- a/CLASSOPS/Derek/Derek's Log.xlsx
+++ b/CLASSOPS/Derek/Derek's Log.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3890" uniqueCount="533">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4536" uniqueCount="572">
   <si>
     <t>Staff Name</t>
   </si>
@@ -2170,10 +2170,283 @@
     <t>Meet Steve Chan. Wants to hook his laptop up to use Skype.</t>
   </si>
   <si>
-    <t>Flat screen TV, wireless keyboard, TV remote, ethernet cable and extension cord. Turn off wireless keyboard and place in the bag before transporting to Vari 1155. Reconnect ethernet cable to the PC from the router and plug into power once inside 1155.</t>
-  </si>
-  <si>
     <t>Pickup web cam and triod. Return kit to SLH 114L MCR.</t>
+  </si>
+  <si>
+    <t>Return lectern mic, audience mic, stands, projector remote and presentation remote to back booth. Lock room-both entrances.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Pick up webcam with tripod and USB extension cable </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>if supplied</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Return kit to FDRS 164. BE ON TIME - CRUCIAL.</t>
+    </r>
+  </si>
+  <si>
+    <t>DLP flat screen TV. To  Vanier 132 storeroom.</t>
+  </si>
+  <si>
+    <t>Flat screen TV, wireless keyboard, TV remote, ethernet cable and extension cord. Turn off wireless keyboard and place in the bag before transporting to Vari 1155. Reconnect ethernet cable to the PC from the router and plug into power, once inside 1155.</t>
+  </si>
+  <si>
+    <t>DLP flat screen TV. Lock room after leaving. To Vanier 132 store.</t>
+  </si>
+  <si>
+    <t>Student group here. Please return the wireless keyboard and remote for the projector to FC 156A</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1 lectern mic, stand, but </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>not</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the cable to the lectern area. Turn off PA system. To FDRS 156A.</t>
+    </r>
+  </si>
+  <si>
+    <t>Return wireless keyboard and projector remote to FDRS 156A.</t>
+  </si>
+  <si>
+    <t>Return lectern mic, 2 audience mics, stands, projector remote and presentation remote to back booth. Lock room-both entrances.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meet Steve Chan. Wants to hook up his laptop to use Skype. This is his second request...was shown this last week. </t>
+  </si>
+  <si>
+    <r>
+      <t>DLP flat screen TV ,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>wireless keyboard and TV remote control</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. To  Vanier 132 storeroom.</t>
+    </r>
+  </si>
+  <si>
+    <t>Meet Susan Ehrlich and show how to use the VHS player.</t>
+  </si>
+  <si>
+    <t>Disconnect the VHS player from the auxilliary inputs and take to Ross S120 storeroom. RCA cables stay with the player.</t>
+  </si>
+  <si>
+    <t>Roll in a VHS player and connect RCA cables to auxilliary inputs.</t>
+  </si>
+  <si>
+    <t>Return lectern mic, 2 desk mic, stands, projector remote and presentation remote to back booth. Lock room-both entrances.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Flat screen TV, wireless keyboard, TV remote, ethernet cable and extension cord. Turn off wireless keyboard and place in the bag before transporting to Vari 1155. Reconnect ethernet cable to the PC from the router and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PLUG INTO POWER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, once inside 1155.</t>
+    </r>
+  </si>
+  <si>
+    <t>Leave portable screen. Door code 7083* Return to FDRS 156A.</t>
+  </si>
+  <si>
+    <t>Lectern mic and small PA under projector cart, cables, stand and carpets. To Vanier 040 storeroom.</t>
+  </si>
+  <si>
+    <t>Return lectern mic, audience mic, 2 desk mics, stands, projector remote and presentation remote to back booth. Lock room-both entrances.</t>
+  </si>
+  <si>
+    <t>Subsequent demo for Terry Conlin at this location.</t>
+  </si>
+  <si>
+    <t>Wireless keyboard and projector remote should be there already from earlier today. Please check.</t>
+  </si>
+  <si>
+    <t>1 audience mic, 2 desk mics, wireless neck mic.  Lectern mic is already in place from earlier today. Turn on large PA if it is not on already. Mics, stands and cables are in FDRS 156A. Event begins at 5pm.</t>
+  </si>
+  <si>
+    <t>Leave all in room, just shut off PC, projector and amplifier. Lock room overnight for continuation of this event on Saturday morning.</t>
+  </si>
+  <si>
+    <t>Meet Karen Murray.</t>
+  </si>
+  <si>
+    <t>Leave all in room, just turn off PC and projector. Lock room.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>READ CAREFULLY</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Pickup 4 mics only. Unclip them and leave all stands, clips, cables etc. Turn off PA system. To FDRS 156A.</t>
+    </r>
+  </si>
+  <si>
+    <t>Lectern mic, stand, cables and small PA to FDRS 156A.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Return webcam, tripod and USB extension if supplied to FDRS 164. </t>
+  </si>
+  <si>
+    <r>
+      <t>3 floor mics, 1 lectern mic, stands, carpets and cables, but</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> not the carpet and cable to the lectern area</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. (This particular instruction has not been adhered to recently). Turn off PA system. To FDRS 156A.</t>
+    </r>
+  </si>
+  <si>
+    <t>Neck mic and small PA under projector cart. To Vanier 040 store.</t>
+  </si>
+  <si>
+    <t>Includes portable screen. Lock room. To Vanier 040 store.</t>
+  </si>
+  <si>
+    <t>DLP flat screen TV. Leave their network cable and portable screen. Lock room. To Vanier 132 store.</t>
+  </si>
+  <si>
+    <t>2 neck mics, mixer, small PA to FDRS 156A.</t>
+  </si>
+  <si>
+    <r>
+      <t>1 lectern mic and stand. Leave</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> carpet and cable to the lectern area</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Turn off PA system. To FDRS 156A.</t>
+    </r>
+  </si>
+  <si>
+    <t>Turn off PC and projector. Leave in and lock room.</t>
+  </si>
+  <si>
+    <t>TOA neck mic and receiver with small PA at the back of the room. Neck mic is most likely at the front of the room. To Ross S120 store.</t>
+  </si>
+  <si>
+    <t>TOA neck mic and receiver with small PA to FDRS 156A.</t>
+  </si>
+  <si>
+    <t>Includes projector. Leave their network cable and portable screen. Lock room. To Vanier 132 store.</t>
+  </si>
+  <si>
+    <t>Lectern mic and stand. Leave cable in positon. Turn off PA system and lock the assembly hall. To FDRS 156A.</t>
+  </si>
+  <si>
+    <t>Lectern mic and stand. Cable is in positon already. Turn on PA system. From FDRS 156A.</t>
   </si>
 </sst>
 </file>
@@ -2183,7 +2456,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2232,6 +2505,19 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2321,7 +2607,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2426,11 +2712,26 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2738,11 +3039,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I879"/>
+  <dimension ref="A1:I1028"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A857" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B873" sqref="B873"/>
+      <pane ySplit="1" topLeftCell="A1011" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F1020" sqref="F1020"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18544,7 +18845,7 @@
         <v>191</v>
       </c>
       <c r="F866" s="20" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="867" spans="1:6" x14ac:dyDescent="0.25">
@@ -18621,10 +18922,10 @@
         <v>275</v>
       </c>
       <c r="F870" s="20" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="871" spans="1:6" s="39" customFormat="1" x14ac:dyDescent="0.25">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="871" spans="1:6" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A871" s="33" t="s">
         <v>80</v>
       </c>
@@ -18640,7 +18941,7 @@
       <c r="E871" s="37" t="s">
         <v>136</v>
       </c>
-      <c r="F871" s="38" t="s">
+      <c r="F871" s="39" t="s">
         <v>271</v>
       </c>
     </row>
@@ -18648,101 +18949,98 @@
       <c r="A872" s="6"/>
       <c r="B872" s="23"/>
       <c r="C872" s="8" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D872" s="6"/>
       <c r="E872" s="27"/>
       <c r="F872" s="29"/>
     </row>
-    <row r="873" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="873" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A873" s="10" t="s">
-        <v>13</v>
+        <v>92</v>
       </c>
       <c r="B873" s="21">
-        <v>42766</v>
+        <v>42767</v>
       </c>
       <c r="C873" s="17" t="s">
-        <v>105</v>
-      </c>
-      <c r="D873" s="18" t="s">
-        <v>49</v>
+        <v>284</v>
+      </c>
+      <c r="D873" s="10" t="s">
+        <v>55</v>
       </c>
       <c r="E873" s="19" t="s">
-        <v>277</v>
+        <v>466</v>
       </c>
       <c r="F873" s="20" t="s">
-        <v>364</v>
+        <v>432</v>
       </c>
     </row>
     <row r="874" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A874" s="10" t="s">
-        <v>13</v>
+        <v>80</v>
       </c>
       <c r="B874" s="21">
-        <v>42766</v>
+        <v>42767</v>
       </c>
       <c r="C874" s="17" t="s">
-        <v>207</v>
+        <v>110</v>
       </c>
       <c r="D874" s="18" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E874" s="19" t="s">
-        <v>191</v>
+        <v>136</v>
       </c>
       <c r="F874" s="20" t="s">
-        <v>532</v>
+        <v>205</v>
       </c>
     </row>
     <row r="875" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A875" s="10" t="s">
-        <v>13</v>
+        <v>80</v>
       </c>
       <c r="B875" s="21">
-        <v>42766</v>
+        <v>42767</v>
       </c>
       <c r="C875" s="17" t="s">
-        <v>207</v>
+        <v>110</v>
       </c>
       <c r="D875" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E875" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="876" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A876" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B876" s="21">
+        <v>42767</v>
+      </c>
+      <c r="C876" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="D876" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="E875" s="19" t="s">
-        <v>279</v>
-      </c>
-      <c r="F875" s="20" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="876" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A876" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B876" s="21">
-        <v>42766</v>
-      </c>
-      <c r="C876" s="17" t="s">
-        <v>103</v>
-      </c>
-      <c r="D876" s="18" t="s">
-        <v>57</v>
-      </c>
       <c r="E876" s="19" t="s">
-        <v>246</v>
+        <v>466</v>
       </c>
       <c r="F876" s="20" t="s">
-        <v>530</v>
+        <v>533</v>
       </c>
     </row>
     <row r="877" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A877" s="10" t="s">
-        <v>13</v>
+        <v>80</v>
       </c>
       <c r="B877" s="21">
-        <v>42766</v>
+        <v>42767</v>
       </c>
       <c r="C877" s="17" t="s">
-        <v>110</v>
+        <v>225</v>
       </c>
       <c r="D877" s="18" t="s">
         <v>59</v>
@@ -18751,44 +19049,2766 @@
         <v>106</v>
       </c>
     </row>
-    <row r="878" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="878" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A878" s="10" t="s">
-        <v>13</v>
+        <v>80</v>
       </c>
       <c r="B878" s="21">
-        <v>42766</v>
+        <v>42767</v>
       </c>
       <c r="C878" s="17" t="s">
-        <v>253</v>
+        <v>129</v>
       </c>
       <c r="D878" s="18" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="E878" s="19" t="s">
-        <v>275</v>
+        <v>149</v>
       </c>
       <c r="F878" s="20" t="s">
-        <v>531</v>
+        <v>395</v>
       </c>
     </row>
     <row r="879" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A879" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B879" s="34">
-        <v>42766</v>
-      </c>
-      <c r="C879" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="B879" s="21">
+        <v>42767</v>
+      </c>
+      <c r="C879" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="D879" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E879" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="F879" s="20" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="880" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A880" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="B880" s="34">
+        <v>42767</v>
+      </c>
+      <c r="C880" s="35" t="s">
+        <v>226</v>
+      </c>
+      <c r="D880" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="E880" s="37" t="s">
+        <v>275</v>
+      </c>
+      <c r="F880" s="39" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="881" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A881" s="6"/>
+      <c r="B881" s="23"/>
+      <c r="C881" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="D881" s="6"/>
+      <c r="E881" s="27"/>
+      <c r="F881" s="29"/>
+    </row>
+    <row r="882" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A882" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B882" s="21">
+        <v>42768</v>
+      </c>
+      <c r="C882" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D882" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E882" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="883" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A883" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B883" s="21">
+        <v>42768</v>
+      </c>
+      <c r="C883" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D883" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E883" s="19" t="s">
+        <v>403</v>
+      </c>
+      <c r="F883" s="20" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="884" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A884" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B884" s="21">
+        <v>42768</v>
+      </c>
+      <c r="C884" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D884" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E884" s="19" t="s">
+        <v>177</v>
+      </c>
+      <c r="F884" s="20" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="885" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A885" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B885" s="21">
+        <v>42768</v>
+      </c>
+      <c r="C885" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D885" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E885" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="F885" s="20" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="886" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A886" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B886" s="21">
+        <v>42768</v>
+      </c>
+      <c r="C886" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D886" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E886" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F886" s="20" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="887" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A887" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B887" s="21">
+        <v>42768</v>
+      </c>
+      <c r="C887" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D887" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E887" s="19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="888" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A888" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="B888" s="41">
+        <v>42768</v>
+      </c>
+      <c r="C888" s="42" t="s">
+        <v>225</v>
+      </c>
+      <c r="D888" s="43" t="s">
+        <v>51</v>
+      </c>
+      <c r="E888" s="44" t="s">
+        <v>275</v>
+      </c>
+      <c r="F888" s="39" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="889" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A889" s="6"/>
+      <c r="B889" s="23"/>
+      <c r="C889" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="D889" s="6"/>
+      <c r="E889" s="27"/>
+      <c r="F889" s="29"/>
+    </row>
+    <row r="890" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A890" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B890" s="21">
+        <v>42769</v>
+      </c>
+      <c r="C890" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="D890" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E890" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="F890" s="20" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="891" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A891" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="B891" s="21">
+        <v>42769</v>
+      </c>
+      <c r="C891" s="42" t="s">
+        <v>110</v>
+      </c>
+      <c r="D891" s="43" t="s">
+        <v>51</v>
+      </c>
+      <c r="E891" s="44" t="s">
+        <v>275</v>
+      </c>
+      <c r="F891" s="39" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="892" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A892" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="B892" s="21">
+        <v>42769</v>
+      </c>
+      <c r="C892" s="17" t="s">
+        <v>362</v>
+      </c>
+      <c r="D892" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E892" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="F892" s="20" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="893" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A893" s="6"/>
+      <c r="B893" s="23"/>
+      <c r="C893" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D893" s="6"/>
+      <c r="E893" s="27"/>
+      <c r="F893" s="29"/>
+    </row>
+    <row r="894" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A894" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B894" s="21">
+        <v>42772</v>
+      </c>
+      <c r="C894" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D894" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E894" s="19" t="s">
+        <v>381</v>
+      </c>
+      <c r="F894" s="20" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="895" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A895" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B895" s="21">
+        <v>42772</v>
+      </c>
+      <c r="C895" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D895" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E895" s="19" t="s">
+        <v>381</v>
+      </c>
+      <c r="F895" s="20" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="896" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A896" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B896" s="21">
+        <v>42772</v>
+      </c>
+      <c r="C896" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D896" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E896" s="19" t="s">
+        <v>279</v>
+      </c>
+      <c r="F896" s="20" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="897" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A897" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B897" s="21">
+        <v>42772</v>
+      </c>
+      <c r="C897" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D897" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E897" s="19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="898" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A898" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B898" s="21">
+        <v>42772</v>
+      </c>
+      <c r="C898" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="D898" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E898" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="899" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A899" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B899" s="21">
+        <v>42772</v>
+      </c>
+      <c r="C899" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="D899" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E899" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F899" s="20" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="900" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A900" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="B900" s="34">
+        <v>42772</v>
+      </c>
+      <c r="C900" s="35" t="s">
+        <v>226</v>
+      </c>
+      <c r="D900" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="E900" s="37" t="s">
+        <v>275</v>
+      </c>
+      <c r="F900" s="39" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="901" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A901" s="6"/>
+      <c r="B901" s="23"/>
+      <c r="C901" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="D901" s="6"/>
+      <c r="E901" s="27"/>
+      <c r="F901" s="29"/>
+    </row>
+    <row r="902" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A902" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B902" s="21">
+        <v>42773</v>
+      </c>
+      <c r="C902" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D902" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E902" s="19" t="s">
+        <v>277</v>
+      </c>
+      <c r="F902" s="20" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="903" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A903" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B903" s="21">
+        <v>42773</v>
+      </c>
+      <c r="C903" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D903" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E903" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="F903" s="20" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="904" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A904" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B904" s="21">
+        <v>42773</v>
+      </c>
+      <c r="C904" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D904" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E904" s="19" t="s">
+        <v>279</v>
+      </c>
+      <c r="F904" s="20" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="905" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A905" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B905" s="21">
+        <v>42773</v>
+      </c>
+      <c r="C905" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="D905" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="E905" s="19" t="s">
+        <v>246</v>
+      </c>
+      <c r="F905" s="20" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="906" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A906" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B906" s="21">
+        <v>42773</v>
+      </c>
+      <c r="C906" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D906" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E906" s="19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="907" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A907" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B907" s="21">
+        <v>42773</v>
+      </c>
+      <c r="C907" s="17" t="s">
+        <v>253</v>
+      </c>
+      <c r="D907" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E907" s="19" t="s">
+        <v>275</v>
+      </c>
+      <c r="F907" s="20" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="908" spans="1:6" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A908" s="40" t="s">
+        <v>80</v>
+      </c>
+      <c r="B908" s="41">
+        <v>42773</v>
+      </c>
+      <c r="C908" s="42" t="s">
+        <v>225</v>
+      </c>
+      <c r="D908" s="43" t="s">
+        <v>59</v>
+      </c>
+      <c r="E908" s="44" t="s">
+        <v>136</v>
+      </c>
+      <c r="F908" s="39" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="909" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A909" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B909" s="41">
+        <v>42773</v>
+      </c>
+      <c r="C909" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="D909" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E909" s="19" t="s">
+        <v>177</v>
+      </c>
+      <c r="F909" s="20" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="910" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A910" s="6"/>
+      <c r="B910" s="23"/>
+      <c r="C910" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D910" s="6"/>
+      <c r="E910" s="27"/>
+      <c r="F910" s="29"/>
+    </row>
+    <row r="911" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A911" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B911" s="21">
+        <v>42774</v>
+      </c>
+      <c r="C911" s="17" t="s">
+        <v>368</v>
+      </c>
+      <c r="D911" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="E911" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="F911" s="20" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="912" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A912" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B912" s="21">
+        <v>42774</v>
+      </c>
+      <c r="C912" s="17" t="s">
+        <v>368</v>
+      </c>
+      <c r="D912" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="E912" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="F912" s="20" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="913" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A913" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B913" s="21">
+        <v>42774</v>
+      </c>
+      <c r="C913" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D913" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="E913" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="F913" s="20" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="914" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A914" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B914" s="21">
+        <v>42774</v>
+      </c>
+      <c r="C914" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D914" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E914" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F914" s="20" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="915" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A915" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B915" s="21">
+        <v>42774</v>
+      </c>
+      <c r="C915" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D915" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E915" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="916" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A916" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B916" s="21">
+        <v>42774</v>
+      </c>
+      <c r="C916" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="D916" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E916" s="19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="917" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A917" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="B917" s="34">
+        <v>42774</v>
+      </c>
+      <c r="C917" s="35" t="s">
+        <v>226</v>
+      </c>
+      <c r="D917" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="E917" s="37" t="s">
+        <v>275</v>
+      </c>
+      <c r="F917" s="39" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="918" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A918" s="6"/>
+      <c r="B918" s="23"/>
+      <c r="C918" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="D918" s="6"/>
+      <c r="E918" s="27"/>
+      <c r="F918" s="29"/>
+    </row>
+    <row r="919" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A919" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B919" s="21">
+        <v>42775</v>
+      </c>
+      <c r="C919" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D919" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E919" s="19" t="s">
+        <v>277</v>
+      </c>
+      <c r="F919" s="20" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="920" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A920" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B920" s="21">
+        <v>42775</v>
+      </c>
+      <c r="C920" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D920" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E920" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F920" s="20" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="921" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A921" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B921" s="21">
+        <v>42775</v>
+      </c>
+      <c r="C921" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="D921" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E921" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="F921" s="20" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="922" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A922" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B922" s="21">
+        <v>42775</v>
+      </c>
+      <c r="C922" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D922" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E922" s="19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="923" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A923" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B923" s="21">
+        <v>42775</v>
+      </c>
+      <c r="C923" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D923" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E923" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="924" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A924" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="B924" s="21">
+        <v>42775</v>
+      </c>
+      <c r="C924" s="42" t="s">
+        <v>225</v>
+      </c>
+      <c r="D924" s="43" t="s">
+        <v>51</v>
+      </c>
+      <c r="E924" s="44" t="s">
+        <v>275</v>
+      </c>
+      <c r="F924" s="39" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="925" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A925" s="6"/>
+      <c r="B925" s="23"/>
+      <c r="C925" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="D925" s="6"/>
+      <c r="E925" s="27"/>
+      <c r="F925" s="29"/>
+    </row>
+    <row r="926" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A926" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="B926" s="21">
+        <v>42776</v>
+      </c>
+      <c r="C926" s="42" t="s">
+        <v>110</v>
+      </c>
+      <c r="D926" s="43" t="s">
+        <v>51</v>
+      </c>
+      <c r="E926" s="44" t="s">
+        <v>275</v>
+      </c>
+      <c r="F926" s="39" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="927" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A927" s="6"/>
+      <c r="B927" s="23"/>
+      <c r="C927" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D927" s="6"/>
+      <c r="E927" s="27"/>
+      <c r="F927" s="29"/>
+    </row>
+    <row r="928" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A928" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B928" s="21">
+        <v>42779</v>
+      </c>
+      <c r="C928" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D928" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E928" s="19" t="s">
+        <v>279</v>
+      </c>
+      <c r="F928" s="20" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="929" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A929" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B929" s="21">
+        <v>42779</v>
+      </c>
+      <c r="C929" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D929" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E929" s="19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="930" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A930" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B930" s="21">
+        <v>42779</v>
+      </c>
+      <c r="C930" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="D930" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E930" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="F930" s="20" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="931" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A931" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B931" s="21">
+        <v>42779</v>
+      </c>
+      <c r="C931" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="D931" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E931" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="932" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A932" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B932" s="21">
+        <v>42779</v>
+      </c>
+      <c r="C932" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="D932" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E932" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F932" s="20" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="933" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A933" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="B933" s="34">
+        <v>42779</v>
+      </c>
+      <c r="C933" s="35" t="s">
+        <v>226</v>
+      </c>
+      <c r="D933" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="E933" s="37" t="s">
+        <v>275</v>
+      </c>
+      <c r="F933" s="39" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="934" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A934" s="6"/>
+      <c r="B934" s="23"/>
+      <c r="C934" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="D934" s="6"/>
+      <c r="E934" s="27"/>
+      <c r="F934" s="29"/>
+    </row>
+    <row r="935" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A935" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B935" s="21">
+        <v>42780</v>
+      </c>
+      <c r="C935" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D935" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E935" s="19" t="s">
+        <v>277</v>
+      </c>
+      <c r="F935" s="20" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="936" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A936" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B936" s="21">
+        <v>42780</v>
+      </c>
+      <c r="C936" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D936" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E936" s="19" t="s">
+        <v>279</v>
+      </c>
+      <c r="F936" s="20" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="937" spans="1:6" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A937" s="40" t="s">
+        <v>80</v>
+      </c>
+      <c r="B937" s="21">
+        <v>42780</v>
+      </c>
+      <c r="C937" s="42" t="s">
+        <v>240</v>
+      </c>
+      <c r="D937" s="43" t="s">
+        <v>59</v>
+      </c>
+      <c r="E937" s="44" t="s">
+        <v>136</v>
+      </c>
+      <c r="F937" s="39" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="938" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A938" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B938" s="21">
+        <v>42780</v>
+      </c>
+      <c r="C938" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D938" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E938" s="19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="939" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A939" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B939" s="21">
+        <v>42780</v>
+      </c>
+      <c r="C939" s="17" t="s">
+        <v>253</v>
+      </c>
+      <c r="D939" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E939" s="19" t="s">
+        <v>275</v>
+      </c>
+      <c r="F939" s="39" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="940" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A940" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B940" s="21">
+        <v>42780</v>
+      </c>
+      <c r="C940" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="D940" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E940" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F940" s="20" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="941" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A941" s="6"/>
+      <c r="B941" s="23"/>
+      <c r="C941" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D941" s="6"/>
+      <c r="E941" s="27"/>
+      <c r="F941" s="29"/>
+    </row>
+    <row r="942" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A942" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B942" s="21">
+        <v>42781</v>
+      </c>
+      <c r="C942" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="D942" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E942" s="19" t="s">
+        <v>277</v>
+      </c>
+      <c r="F942" s="20" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="943" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A943" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B943" s="21">
+        <v>42781</v>
+      </c>
+      <c r="C943" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D943" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E943" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F943" s="20" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="944" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A944" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B944" s="21">
+        <v>42781</v>
+      </c>
+      <c r="C944" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D944" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E944" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="945" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A945" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B945" s="21">
+        <v>42781</v>
+      </c>
+      <c r="C945" s="17" t="s">
+        <v>324</v>
+      </c>
+      <c r="D945" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E945" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="F945" s="20" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="946" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A946" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B946" s="21">
+        <v>42781</v>
+      </c>
+      <c r="C946" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="D946" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E946" s="19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="947" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A947" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="B947" s="34">
+        <v>42781</v>
+      </c>
+      <c r="C947" s="35" t="s">
+        <v>226</v>
+      </c>
+      <c r="D947" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="E947" s="37" t="s">
+        <v>275</v>
+      </c>
+      <c r="F947" s="39" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="948" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A948" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="B948" s="34">
+        <v>42779</v>
+      </c>
+      <c r="C948" s="35" t="s">
+        <v>226</v>
+      </c>
+      <c r="D948" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="E948" s="37" t="s">
+        <v>187</v>
+      </c>
+      <c r="F948" s="20" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="949" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A949" s="6"/>
+      <c r="B949" s="23"/>
+      <c r="C949" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="D949" s="6"/>
+      <c r="E949" s="27"/>
+      <c r="F949" s="29"/>
+    </row>
+    <row r="950" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A950" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B950" s="21">
+        <v>42782</v>
+      </c>
+      <c r="C950" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D950" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E950" s="19" t="s">
+        <v>277</v>
+      </c>
+      <c r="F950" s="20" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="951" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A951" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B951" s="21">
+        <v>42782</v>
+      </c>
+      <c r="C951" s="17" t="s">
+        <v>269</v>
+      </c>
+      <c r="D951" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E951" s="19" t="s">
+        <v>202</v>
+      </c>
+      <c r="F951" s="20" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="952" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A952" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B952" s="21">
+        <v>42782</v>
+      </c>
+      <c r="C952" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="D952" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E952" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="F952" s="20" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="953" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A953" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B953" s="21">
+        <v>42782</v>
+      </c>
+      <c r="C953" s="17" t="s">
+        <v>284</v>
+      </c>
+      <c r="D953" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="E953" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="F953" s="20" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="954" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A954" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B954" s="21">
+        <v>42782</v>
+      </c>
+      <c r="C954" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D954" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E954" s="19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="955" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A955" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B955" s="21">
+        <v>42782</v>
+      </c>
+      <c r="C955" s="17" t="s">
+        <v>253</v>
+      </c>
+      <c r="D955" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E955" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="956" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A956" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B956" s="21">
+        <v>42782</v>
+      </c>
+      <c r="C956" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="D956" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="E956" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="F956" s="20" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="957" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A957" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="B957" s="21">
+        <v>42782</v>
+      </c>
+      <c r="C957" s="42" t="s">
+        <v>225</v>
+      </c>
+      <c r="D957" s="43" t="s">
+        <v>51</v>
+      </c>
+      <c r="E957" s="44" t="s">
+        <v>275</v>
+      </c>
+      <c r="F957" s="39" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="958" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A958" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="B958" s="34">
+        <v>42782</v>
+      </c>
+      <c r="C958" s="35" t="s">
+        <v>226</v>
+      </c>
+      <c r="D958" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="E958" s="37" t="s">
+        <v>136</v>
+      </c>
+      <c r="F958" s="20" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="959" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A959" s="6"/>
+      <c r="B959" s="23"/>
+      <c r="C959" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="D959" s="6"/>
+      <c r="E959" s="27"/>
+      <c r="F959" s="29"/>
+    </row>
+    <row r="960" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A960" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B960" s="21">
+        <v>42783</v>
+      </c>
+      <c r="C960" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D960" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E960" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="F960" s="20" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="961" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A961" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B961" s="21">
+        <v>42783</v>
+      </c>
+      <c r="C961" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D961" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E961" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="F961" s="20" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="962" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A962" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="B962" s="21">
+        <v>42783</v>
+      </c>
+      <c r="C962" s="42" t="s">
+        <v>110</v>
+      </c>
+      <c r="D962" s="43" t="s">
+        <v>51</v>
+      </c>
+      <c r="E962" s="44" t="s">
+        <v>275</v>
+      </c>
+      <c r="F962" s="39" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="963" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A963" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="B963" s="34">
+        <v>42783</v>
+      </c>
+      <c r="C963" s="35" t="s">
+        <v>226</v>
+      </c>
+      <c r="D963" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="E963" s="37" t="s">
+        <v>142</v>
+      </c>
+      <c r="F963" s="20" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="964" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A964" s="6"/>
+      <c r="B964" s="23"/>
+      <c r="C964" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D964" s="6"/>
+      <c r="E964" s="27"/>
+      <c r="F964" s="29"/>
+    </row>
+    <row r="965" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A965" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B965" s="21">
+        <v>42793</v>
+      </c>
+      <c r="C965" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D965" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E965" s="19" t="s">
+        <v>381</v>
+      </c>
+      <c r="F965" s="20" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="966" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A966" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B966" s="21">
+        <v>42793</v>
+      </c>
+      <c r="C966" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D966" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E966" s="19" t="s">
+        <v>381</v>
+      </c>
+      <c r="F966" s="20" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="967" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A967" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B967" s="21">
+        <v>42793</v>
+      </c>
+      <c r="C967" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D967" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E967" s="19" t="s">
+        <v>279</v>
+      </c>
+      <c r="F967" s="20" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="968" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A968" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B968" s="21">
+        <v>42793</v>
+      </c>
+      <c r="C968" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="D968" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E968" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="F968" s="20" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="969" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A969" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B969" s="21">
+        <v>42793</v>
+      </c>
+      <c r="C969" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D969" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E969" s="19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="970" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A970" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B970" s="21">
+        <v>42793</v>
+      </c>
+      <c r="C970" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="D970" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E970" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="971" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A971" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B971" s="21">
+        <v>42793</v>
+      </c>
+      <c r="C971" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="D971" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E971" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F971" s="20" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="972" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A972" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B972" s="21">
+        <v>42793</v>
+      </c>
+      <c r="C972" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="D972" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E972" s="19" t="s">
+        <v>257</v>
+      </c>
+      <c r="F972" s="20" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="973" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A973" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="B973" s="34">
+        <v>42793</v>
+      </c>
+      <c r="C973" s="35" t="s">
+        <v>226</v>
+      </c>
+      <c r="D973" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="E973" s="37" t="s">
+        <v>275</v>
+      </c>
+      <c r="F973" s="39" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="974" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A974" s="6"/>
+      <c r="B974" s="23"/>
+      <c r="C974" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="D974" s="6"/>
+      <c r="E974" s="27"/>
+      <c r="F974" s="29"/>
+    </row>
+    <row r="975" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A975" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B975" s="21">
+        <v>42794</v>
+      </c>
+      <c r="C975" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D975" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E975" s="19" t="s">
+        <v>381</v>
+      </c>
+      <c r="F975" s="20" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="976" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A976" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B976" s="21">
+        <v>42794</v>
+      </c>
+      <c r="C976" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D976" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E976" s="19" t="s">
+        <v>381</v>
+      </c>
+      <c r="F976" s="20" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="977" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A977" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B977" s="21">
+        <v>42794</v>
+      </c>
+      <c r="C977" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D977" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E977" s="19" t="s">
+        <v>381</v>
+      </c>
+      <c r="F977" s="20" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="978" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A978" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B978" s="21">
+        <v>42794</v>
+      </c>
+      <c r="C978" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D978" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E978" s="19" t="s">
+        <v>277</v>
+      </c>
+      <c r="F978" s="20" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="979" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A979" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B979" s="21">
+        <v>42794</v>
+      </c>
+      <c r="C979" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D979" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E979" s="19" t="s">
+        <v>277</v>
+      </c>
+      <c r="F979" s="20" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="980" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A980" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B980" s="21">
+        <v>42794</v>
+      </c>
+      <c r="C980" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D980" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E980" s="19" t="s">
+        <v>403</v>
+      </c>
+      <c r="F980" s="20" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="981" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A981" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B981" s="21">
+        <v>42794</v>
+      </c>
+      <c r="C981" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D981" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E981" s="19" t="s">
+        <v>279</v>
+      </c>
+      <c r="F981" s="20" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="982" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A982" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B982" s="21">
+        <v>42794</v>
+      </c>
+      <c r="C982" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D982" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E982" s="19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="983" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A983" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B983" s="21">
+        <v>42794</v>
+      </c>
+      <c r="C983" s="17" t="s">
+        <v>253</v>
+      </c>
+      <c r="D983" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E983" s="19" t="s">
+        <v>275</v>
+      </c>
+      <c r="F983" s="20" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="984" spans="1:6" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A984" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="B984" s="34">
+        <v>42794</v>
+      </c>
+      <c r="C984" s="35" t="s">
         <v>529</v>
       </c>
-      <c r="D879" s="36" t="s">
-        <v>59</v>
-      </c>
-      <c r="E879" s="37" t="s">
+      <c r="D984" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="E984" s="37" t="s">
         <v>136</v>
       </c>
-      <c r="F879" s="38" t="s">
+      <c r="F984" s="39" t="s">
         <v>271</v>
+      </c>
+    </row>
+    <row r="985" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A985" s="6"/>
+      <c r="B985" s="23"/>
+      <c r="C985" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D985" s="6"/>
+      <c r="E985" s="27"/>
+      <c r="F985" s="29"/>
+    </row>
+    <row r="986" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A986" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B986" s="21">
+        <v>42795</v>
+      </c>
+      <c r="C986" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D986" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E986" s="19" t="s">
+        <v>277</v>
+      </c>
+      <c r="F986" s="20" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="987" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A987" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B987" s="21">
+        <v>42795</v>
+      </c>
+      <c r="C987" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D987" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E987" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="F987" s="20" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="988" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A988" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B988" s="21">
+        <v>42795</v>
+      </c>
+      <c r="C988" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D988" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E988" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="F988" s="20" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="989" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A989" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B989" s="21">
+        <v>42795</v>
+      </c>
+      <c r="C989" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="D989" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E989" s="19" t="s">
+        <v>466</v>
+      </c>
+      <c r="F989" s="20" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="990" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A990" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B990" s="21">
+        <v>42795</v>
+      </c>
+      <c r="C990" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="D990" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E990" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="F990" s="20" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="991" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A991" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B991" s="21">
+        <v>42795</v>
+      </c>
+      <c r="C991" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="D991" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E991" s="19" t="s">
+        <v>381</v>
+      </c>
+      <c r="F991" s="20" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="992" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A992" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B992" s="21">
+        <v>42795</v>
+      </c>
+      <c r="C992" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="D992" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E992" s="19" t="s">
+        <v>381</v>
+      </c>
+      <c r="F992" s="20" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="993" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A993" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B993" s="21">
+        <v>42795</v>
+      </c>
+      <c r="C993" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="D993" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E993" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="F993" s="20" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="994" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A994" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B994" s="21">
+        <v>42795</v>
+      </c>
+      <c r="C994" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="D994" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E994" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="F994" s="20" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="995" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A995" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B995" s="21">
+        <v>42795</v>
+      </c>
+      <c r="C995" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D995" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E995" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F995" s="20" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="996" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A996" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B996" s="21">
+        <v>42795</v>
+      </c>
+      <c r="C996" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D996" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E996" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="997" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A997" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B997" s="21">
+        <v>42795</v>
+      </c>
+      <c r="C997" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="D997" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E997" s="19" t="s">
+        <v>466</v>
+      </c>
+      <c r="F997" s="20" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="998" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A998" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B998" s="21">
+        <v>42795</v>
+      </c>
+      <c r="C998" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="D998" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E998" s="19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="999" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A999" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="B999" s="34">
+        <v>42795</v>
+      </c>
+      <c r="C999" s="35" t="s">
+        <v>226</v>
+      </c>
+      <c r="D999" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="E999" s="37" t="s">
+        <v>275</v>
+      </c>
+      <c r="F999" s="39" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="1000" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1000" s="6"/>
+      <c r="B1000" s="23"/>
+      <c r="C1000" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="D1000" s="6"/>
+      <c r="E1000" s="27"/>
+      <c r="F1000" s="29"/>
+    </row>
+    <row r="1001" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1001" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1001" s="21">
+        <v>42796</v>
+      </c>
+      <c r="C1001" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="D1001" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1001" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="F1001" s="20" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="1002" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1002" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1002" s="21">
+        <v>42796</v>
+      </c>
+      <c r="C1002" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="D1002" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1002" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="F1002" s="20" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="1003" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1003" s="40" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1003" s="41">
+        <v>42796</v>
+      </c>
+      <c r="C1003" s="42" t="s">
+        <v>207</v>
+      </c>
+      <c r="D1003" s="43" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1003" s="44" t="s">
+        <v>136</v>
+      </c>
+      <c r="F1003" s="20" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="1004" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1004" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1004" s="21">
+        <v>42796</v>
+      </c>
+      <c r="C1004" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D1004" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1004" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="F1004" s="20" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="1005" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1005" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1005" s="21">
+        <v>42796</v>
+      </c>
+      <c r="C1005" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1005" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1005" s="19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="1006" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1006" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1006" s="21">
+        <v>42796</v>
+      </c>
+      <c r="C1006" s="17" t="s">
+        <v>324</v>
+      </c>
+      <c r="D1006" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1006" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="1007" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1007" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1007" s="21">
+        <v>42796</v>
+      </c>
+      <c r="C1007" s="42" t="s">
+        <v>225</v>
+      </c>
+      <c r="D1007" s="43" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1007" s="44" t="s">
+        <v>275</v>
+      </c>
+      <c r="F1007" s="39" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="1008" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1008" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1008" s="21">
+        <v>42796</v>
+      </c>
+      <c r="C1008" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="D1008" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1008" s="19" t="s">
+        <v>381</v>
+      </c>
+      <c r="F1008" s="20" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="1009" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1009" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1009" s="21">
+        <v>42796</v>
+      </c>
+      <c r="C1009" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="D1009" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1009" s="19" t="s">
+        <v>381</v>
+      </c>
+      <c r="F1009" s="20" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="1010" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1010" s="6"/>
+      <c r="B1010" s="23"/>
+      <c r="C1010" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="D1010" s="6"/>
+      <c r="E1010" s="27"/>
+      <c r="F1010" s="29"/>
+    </row>
+    <row r="1011" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1011" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1011" s="21">
+        <v>42797</v>
+      </c>
+      <c r="C1011" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1011" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1011" s="19" t="s">
+        <v>277</v>
+      </c>
+      <c r="F1011" s="20" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="1012" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1012" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1012" s="21">
+        <v>42797</v>
+      </c>
+      <c r="C1012" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1012" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1012" s="19" t="s">
+        <v>277</v>
+      </c>
+      <c r="F1012" s="20" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="1013" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1013" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1013" s="21">
+        <v>42797</v>
+      </c>
+      <c r="C1013" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1013" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1013" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="F1013" s="20" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="1014" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1014" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1014" s="21">
+        <v>42796</v>
+      </c>
+      <c r="C1014" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1014" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1014" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="1015" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1015" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1015" s="21">
+        <v>42797</v>
+      </c>
+      <c r="C1015" s="42" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1015" s="43" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1015" s="44" t="s">
+        <v>275</v>
+      </c>
+      <c r="F1015" s="39" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="1016" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1016" s="6"/>
+      <c r="B1016" s="23"/>
+      <c r="C1016" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D1016" s="6"/>
+      <c r="E1016" s="27"/>
+      <c r="F1016" s="29"/>
+    </row>
+    <row r="1017" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1017" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1017" s="21">
+        <v>42800</v>
+      </c>
+      <c r="C1017" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1017" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1017" s="19" t="s">
+        <v>279</v>
+      </c>
+      <c r="F1017" s="20" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="1018" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1018" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1018" s="21">
+        <v>42795</v>
+      </c>
+      <c r="C1018" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1018" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1018" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="F1018" s="20" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="1019" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1019" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1019" s="21">
+        <v>42800</v>
+      </c>
+      <c r="C1019" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1019" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1019" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="1020" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1020" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1020" s="21">
+        <v>42795</v>
+      </c>
+      <c r="C1020" s="17" t="s">
+        <v>284</v>
+      </c>
+      <c r="D1020" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1020" s="19" t="s">
+        <v>381</v>
+      </c>
+      <c r="F1020" s="20" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="1021" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1021" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1021" s="21">
+        <v>42795</v>
+      </c>
+      <c r="C1021" s="17" t="s">
+        <v>284</v>
+      </c>
+      <c r="D1021" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1021" s="19" t="s">
+        <v>381</v>
+      </c>
+      <c r="F1021" s="20" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="1022" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1022" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1022" s="21">
+        <v>42800</v>
+      </c>
+      <c r="C1022" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D1022" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1022" s="19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="1023" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1023" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1023" s="41">
+        <v>42800</v>
+      </c>
+      <c r="C1023" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="D1023" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1023" s="19" t="s">
+        <v>277</v>
+      </c>
+      <c r="F1023" s="20" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="1024" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1024" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1024" s="21">
+        <v>42800</v>
+      </c>
+      <c r="C1024" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="D1024" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1024" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F1024" s="20" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="1025" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1025" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1025" s="41">
+        <v>42800</v>
+      </c>
+      <c r="C1025" s="42" t="s">
+        <v>324</v>
+      </c>
+      <c r="D1025" s="43" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1025" s="44" t="s">
+        <v>419</v>
+      </c>
+      <c r="F1025" s="39" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="1026" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1026" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1026" s="34">
+        <v>42795</v>
+      </c>
+      <c r="C1026" s="35" t="s">
+        <v>188</v>
+      </c>
+      <c r="D1026" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1026" s="37" t="s">
+        <v>381</v>
+      </c>
+      <c r="F1026" s="20" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="1027" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1027" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1027" s="34">
+        <v>42795</v>
+      </c>
+      <c r="C1027" s="35" t="s">
+        <v>188</v>
+      </c>
+      <c r="D1027" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1027" s="37" t="s">
+        <v>381</v>
+      </c>
+      <c r="F1027" s="20" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="1028" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1028" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1028" s="34">
+        <v>42800</v>
+      </c>
+      <c r="C1028" s="35" t="s">
+        <v>226</v>
+      </c>
+      <c r="D1028" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1028" s="37" t="s">
+        <v>275</v>
+      </c>
+      <c r="F1028" s="39" t="s">
+        <v>535</v>
       </c>
     </row>
   </sheetData>
@@ -18798,10 +21818,10 @@
     <sortCondition ref="D427:D515"/>
   </sortState>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A22:A23 B6 B2 A7:A8 B9 A10:A16 B17 A18:A20 B21 A3:A5 B24 A25:A27 B28 B32 A29:A31 A33:A34 B35 A36:A37 B38 A39:A53 B54 A55:A57 B58 A59:A63 B64 A65:A80 B81 A82:A85 B86 A87:A104 B105 A106:A109 B110 A111:A120 B121 A122:A133 B134 A135:A145 B146 A147:A176 B177 A178:A195 B196 A197:A203 B204 A205:A219 B220 A221:A227 B228 A229:A246 B247 A248:A264 B265 A266:A272 B273 A274:A278 B279 A280:A1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A22:A23 B6 B2 A7:A8 B9 A10:A16 B17 A18:A20 B21 A3:A5 B24 A25:A27 B28 B32 A29:A31 A33:A34 B35 A36:A37 B38 A39:A53 B54 A55:A57 B58 A59:A63 B64 A65:A80 B81 A82:A85 B86 A87:A104 B105 A106:A109 B110 A111:A120 B121 A122:A133 B134 A135:A145 B146 A147:A176 B177 A178:A195 B196 A197:A203 B204 A205:A219 B220 A221:A227 B228 A229:A246 B247 A248:A264 B265 A266:A272 B273 A274:A278 B279 A280:A1028 A1029:A1048576">
       <formula1>Task_type</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6 E2 D22:D23 D7:D8 E9 D10:D16 E17 D18:D20 E21 D3:D5 E24 D25:D27 E28 E32 D29:D31 D33:D34 E35 D36:D37 E38 D39:D53 E54 D55:D57 E58 D59:D63 E64 D65:D80 E81 D82:D85 E86 D87:D104 E105 D106:D109 E110 D111:D120 E121 D122:D133 E134 D135:D145 E146 D147:D176 E177 D178:D195 E196 D197:D203 E204 D205:D219 E220 D221:D227 E228 D229:D246 E247 D248:D264 E265 D266:D272 E273 D274:D278 E279 D280:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6 E2 D22:D23 D7:D8 E9 D10:D16 E17 D18:D20 E21 D3:D5 E24 D25:D27 E28 E32 D29:D31 D33:D34 E35 D36:D37 E38 D39:D53 E54 D55:D57 E58 D59:D63 E64 D65:D80 E81 D82:D85 E86 D87:D104 E105 D106:D109 E110 D111:D120 E121 D122:D133 E134 D135:D145 E146 D147:D176 E177 D178:D195 E196 D197:D203 E204 D205:D219 E220 D221:D227 E228 D229:D246 E247 D248:D264 E265 D266:D272 E273 D274:D278 E279 D280:D1028 D1029:D1048576">
       <formula1>Building</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 A2 A9 A17 A21 A24 A28 A32 A35 A38 A54 A58 A64 A81 A86 A105 A110 A121 A134 A146 A177 A196 A204 A220 A228 A247 A265 A273 A279">

</xml_diff>

<commit_message>
Updated the Saturday and Sunday
</commit_message>
<xml_diff>
--- a/CLASSOPS/Derek/Derek's Log.xlsx
+++ b/CLASSOPS/Derek/Derek's Log.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4561" uniqueCount="573">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4756" uniqueCount="592">
   <si>
     <t>Staff Name</t>
   </si>
@@ -2450,6 +2450,86 @@
   </si>
   <si>
     <t>Includes projector. Leave their network cable and portable screen. Lock room. To Vanier 040 store.</t>
+  </si>
+  <si>
+    <t>Return lectern mic, 2 audience mics, neck mic, stands, projector remote and presentation remote to back booth. Lock room-both entrances.</t>
+  </si>
+  <si>
+    <t>Send tech support person to assist with their presentation.</t>
+  </si>
+  <si>
+    <t>Lectern mic, stand, neck mic and small PA under projector cart, carpets etc. To Vanier 040 store.</t>
+  </si>
+  <si>
+    <t>PC and projector, no screen. Lock room. To Vanier 040 store.</t>
+  </si>
+  <si>
+    <t>Additional DLP TV. To Vanier 132 store.</t>
+  </si>
+  <si>
+    <t>DLP TV and computer, wireless keyboard and TV remote. To Vanier 132 store.</t>
+  </si>
+  <si>
+    <t>2101</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">TOA neck mic and receiver with small PA to Vari 1019.  This room is in the </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>second floor offices section</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> at the extreme south end of the building. Enter the area via the door marked SOCIOLOGY just down from Vari D.</t>
+    </r>
+  </si>
+  <si>
+    <t>152 A-Hall</t>
+  </si>
+  <si>
+    <t>5 mics, stands, cables, and 4 channel mixer to FDRS 156A. Leave lectern cable and carpet for it in place. Turn off PA system and lock the assembly hall.</t>
+  </si>
+  <si>
+    <t>Meet instructor Gail Vanstone in the cinema.</t>
+  </si>
+  <si>
+    <t>4 stand mics on stage for a choir and one boom stand mic overtop of a piano.  Small 4 channel mixer is already on stage for the choir mics. Lectern mic is in place from earlier today. Reposition this stand and mic for the piano. Get remaining mics and cables etc. from FDRS 156A storeroom.</t>
+  </si>
+  <si>
+    <t>Pickup Skype web cam and tripod.  To FDRS 164 store.</t>
+  </si>
+  <si>
+    <t>Meet instructor Brenda Blondeau.</t>
+  </si>
+  <si>
+    <t>If room is locked use the Ross N203 key to access.</t>
+  </si>
+  <si>
+    <t>DLP TV and computer. Leave their network cable and portable screen. Lock room with key from FDRS 164. To Vanier 132 store.</t>
+  </si>
+  <si>
+    <t>Turn off PC and projector. Leave all in and lock room with key from FDRS 164.</t>
+  </si>
+  <si>
+    <t>PC and projector, no screen. Lock room with key from FDRS 164. To Vanier 040 store.</t>
+  </si>
+  <si>
+    <t>Lectern mic, stand, and small PA under projector cart, carpets etc. Lock room with key from FDRS 164. To Vanier 040 store.</t>
   </si>
 </sst>
 </file>
@@ -3042,11 +3122,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I1034"/>
+  <dimension ref="A1:I1081"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1020" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1038" sqref="E1038"/>
+      <pane ySplit="1" topLeftCell="A1071" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F1097" sqref="F1097"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21921,6 +22001,842 @@
         <v>106</v>
       </c>
     </row>
+    <row r="1035" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1035" s="6"/>
+      <c r="B1035" s="23"/>
+      <c r="C1035" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D1035" s="6"/>
+      <c r="E1035" s="27"/>
+      <c r="F1035" s="29"/>
+    </row>
+    <row r="1036" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1036" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1036" s="21">
+        <v>42802</v>
+      </c>
+      <c r="C1036" s="17" t="s">
+        <v>210</v>
+      </c>
+      <c r="D1036" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1036" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="F1036" s="20" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="1037" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1037" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1037" s="21">
+        <v>42802</v>
+      </c>
+      <c r="C1037" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="D1037" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1037" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="F1037" s="20" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="1038" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1038" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1038" s="21">
+        <v>42802</v>
+      </c>
+      <c r="C1038" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1038" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1038" s="19" t="s">
+        <v>277</v>
+      </c>
+      <c r="F1038" s="20" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="1039" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1039" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1039" s="21">
+        <v>42802</v>
+      </c>
+      <c r="C1039" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1039" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1039" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="1040" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1040" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1040" s="21">
+        <v>42802</v>
+      </c>
+      <c r="C1040" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="D1040" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1040" s="19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="1041" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1041" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1041" s="34">
+        <v>42802</v>
+      </c>
+      <c r="C1041" s="35" t="s">
+        <v>529</v>
+      </c>
+      <c r="D1041" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1041" s="37" t="s">
+        <v>136</v>
+      </c>
+      <c r="F1041" s="20" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="1042" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1042" s="6"/>
+      <c r="B1042" s="23"/>
+      <c r="C1042" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="D1042" s="6"/>
+      <c r="E1042" s="27"/>
+      <c r="F1042" s="29"/>
+    </row>
+    <row r="1043" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1043" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1043" s="21">
+        <v>42803</v>
+      </c>
+      <c r="C1043" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D1043" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1043" s="19" t="s">
+        <v>277</v>
+      </c>
+      <c r="F1043" s="20" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="1044" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1044" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1044" s="21">
+        <v>42803</v>
+      </c>
+      <c r="C1044" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1044" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1044" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="F1044" s="20" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="1045" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1045" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1045" s="21">
+        <v>42803</v>
+      </c>
+      <c r="C1045" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1045" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1045" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="F1045" s="20" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="1046" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1046" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1046" s="21">
+        <v>42803</v>
+      </c>
+      <c r="C1046" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1046" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1046" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="F1046" s="20" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="1047" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1047" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1047" s="21">
+        <v>42803</v>
+      </c>
+      <c r="C1047" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1047" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1047" s="19" t="s">
+        <v>177</v>
+      </c>
+      <c r="F1047" s="20" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="1048" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1048" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1048" s="21">
+        <v>42803</v>
+      </c>
+      <c r="C1048" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1048" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1048" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="1049" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1049" s="40" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1049" s="21">
+        <v>42803</v>
+      </c>
+      <c r="C1049" s="42" t="s">
+        <v>207</v>
+      </c>
+      <c r="D1049" s="43" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1049" s="44" t="s">
+        <v>136</v>
+      </c>
+      <c r="F1049" s="20" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="1050" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1050" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1050" s="21">
+        <v>42803</v>
+      </c>
+      <c r="C1050" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="D1050" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1050" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="F1050" s="20" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="1051" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1051" s="6"/>
+      <c r="B1051" s="23"/>
+      <c r="C1051" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="D1051" s="6"/>
+      <c r="E1051" s="27"/>
+      <c r="F1051" s="29"/>
+    </row>
+    <row r="1052" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1052" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1052" s="21">
+        <v>42804</v>
+      </c>
+      <c r="C1052" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="D1052" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1052" s="19" t="s">
+        <v>579</v>
+      </c>
+      <c r="F1052" s="20" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="1053" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1053" s="6"/>
+      <c r="B1053" s="23"/>
+      <c r="C1053" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D1053" s="6"/>
+      <c r="E1053" s="27"/>
+      <c r="F1053" s="29"/>
+    </row>
+    <row r="1054" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1054" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1054" s="21">
+        <v>42807</v>
+      </c>
+      <c r="C1054" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1054" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1054" s="19" t="s">
+        <v>279</v>
+      </c>
+      <c r="F1054" s="20" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="1055" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1055" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1055" s="21">
+        <v>42807</v>
+      </c>
+      <c r="C1055" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D1055" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1055" s="19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="1056" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1056" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1056" s="21">
+        <v>42807</v>
+      </c>
+      <c r="C1056" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="D1056" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1056" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F1056" s="20" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="1057" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1057" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1057" s="21">
+        <v>42807</v>
+      </c>
+      <c r="C1057" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="D1057" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1057" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="1058" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1058" s="6"/>
+      <c r="B1058" s="23"/>
+      <c r="C1058" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="D1058" s="6"/>
+      <c r="E1058" s="27"/>
+      <c r="F1058" s="29"/>
+    </row>
+    <row r="1059" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1059" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1059" s="41">
+        <v>42808</v>
+      </c>
+      <c r="C1059" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D1059" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1059" s="19" t="s">
+        <v>279</v>
+      </c>
+      <c r="F1059" s="20" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="1060" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1060" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1060" s="41">
+        <v>42808</v>
+      </c>
+      <c r="C1060" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="D1060" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1060" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F1060" s="20" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="1061" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1061" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1061" s="41">
+        <v>42808</v>
+      </c>
+      <c r="C1061" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1061" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1061" s="19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="1062" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1062" s="6"/>
+      <c r="B1062" s="23"/>
+      <c r="C1062" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D1062" s="6"/>
+      <c r="E1062" s="27"/>
+      <c r="F1062" s="29"/>
+    </row>
+    <row r="1063" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A1063" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1063" s="21">
+        <v>42809</v>
+      </c>
+      <c r="C1063" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1063" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1063" s="19" t="s">
+        <v>581</v>
+      </c>
+      <c r="F1063" s="20" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="1064" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1064" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1064" s="21">
+        <v>42809</v>
+      </c>
+      <c r="C1064" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="D1064" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1064" s="19" t="s">
+        <v>466</v>
+      </c>
+      <c r="F1064" s="20" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="1065" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1065" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1065" s="21">
+        <v>42809</v>
+      </c>
+      <c r="C1065" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="D1065" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1065" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F1065" s="20" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="1066" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1066" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1066" s="21">
+        <v>42809</v>
+      </c>
+      <c r="C1066" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1066" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1066" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="1067" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1067" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1067" s="21">
+        <v>42809</v>
+      </c>
+      <c r="C1067" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="D1067" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1067" s="19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="1068" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1068" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1068" s="21">
+        <v>42809</v>
+      </c>
+      <c r="C1068" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="D1068" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1068" s="19" t="s">
+        <v>581</v>
+      </c>
+      <c r="F1068" s="20" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="1069" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1069" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1069" s="21">
+        <v>42809</v>
+      </c>
+      <c r="C1069" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="D1069" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1069" s="19" t="s">
+        <v>466</v>
+      </c>
+      <c r="F1069" s="20" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="1070" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1070" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1070" s="34">
+        <v>42809</v>
+      </c>
+      <c r="C1070" s="35" t="s">
+        <v>226</v>
+      </c>
+      <c r="D1070" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1070" s="37" t="s">
+        <v>136</v>
+      </c>
+      <c r="F1070" s="20" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="1071" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1071" s="6"/>
+      <c r="B1071" s="23"/>
+      <c r="C1071" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="D1071" s="6"/>
+      <c r="E1071" s="27"/>
+      <c r="F1071" s="29"/>
+    </row>
+    <row r="1072" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1072" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1072" s="21">
+        <v>42810</v>
+      </c>
+      <c r="C1072" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1072" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1072" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="F1072" s="20" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="1073" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1073" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1073" s="21">
+        <v>42810</v>
+      </c>
+      <c r="C1073" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1073" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1073" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="F1073" s="20" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="1074" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1074" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1074" s="21">
+        <v>42810</v>
+      </c>
+      <c r="C1074" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1074" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1074" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="F1074" s="20" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="1075" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1075" s="40" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1075" s="21">
+        <v>42810</v>
+      </c>
+      <c r="C1075" s="42" t="s">
+        <v>207</v>
+      </c>
+      <c r="D1075" s="43" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1075" s="44" t="s">
+        <v>136</v>
+      </c>
+      <c r="F1075" s="20" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="1076" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1076" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1076" s="21">
+        <v>42810</v>
+      </c>
+      <c r="C1076" s="17" t="s">
+        <v>288</v>
+      </c>
+      <c r="D1076" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1076" s="19" t="s">
+        <v>403</v>
+      </c>
+      <c r="F1076" s="20" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="1077" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1077" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1077" s="21">
+        <v>42810</v>
+      </c>
+      <c r="C1077" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="D1077" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1077" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="F1077" s="20" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="1078" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1078" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1078" s="21">
+        <v>42810</v>
+      </c>
+      <c r="C1078" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1078" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1078" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="F1078" s="20" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="1079" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1079" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1079" s="21">
+        <v>42810</v>
+      </c>
+      <c r="C1079" s="17" t="s">
+        <v>253</v>
+      </c>
+      <c r="D1079" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1079" s="19" t="s">
+        <v>277</v>
+      </c>
+      <c r="F1079" s="20" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="1080" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1080" s="6"/>
+      <c r="B1080" s="23"/>
+      <c r="C1080" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="D1080" s="6"/>
+      <c r="E1080" s="27"/>
+      <c r="F1080" s="29"/>
+    </row>
+    <row r="1081" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1081" s="40" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1081" s="21">
+        <v>42811</v>
+      </c>
+      <c r="C1081" s="42" t="s">
+        <v>172</v>
+      </c>
+      <c r="D1081" s="43" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1081" s="44" t="s">
+        <v>136</v>
+      </c>
+      <c r="F1081" s="20" t="s">
+        <v>205</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0"/>
   <sortState ref="A427:G515">
@@ -21928,10 +22844,10 @@
     <sortCondition ref="D427:D515"/>
   </sortState>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A22:A23 B6 B2 A7:A8 B9 A10:A16 B17 A18:A20 B21 A3:A5 B24 A25:A27 B28 B32 A29:A31 A33:A34 B35 A36:A37 B38 A39:A53 B54 A55:A57 B58 A59:A63 B64 A65:A80 B81 A82:A85 B86 A87:A104 B105 A106:A109 B110 A111:A120 B121 A122:A133 B134 A135:A145 B146 A147:A176 B177 A178:A195 B196 A197:A203 B204 A205:A219 B220 A221:A227 B228 A229:A246 B247 A248:A264 B265 A266:A272 B273 A274:A278 B279 A280:A1034 A1035:A1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A22:A23 B6 B2 A7:A8 B9 A10:A16 B17 A18:A20 B21 A3:A5 B24 A25:A27 B28 B32 A29:A31 A33:A34 B35 A36:A37 B38 A39:A53 B54 A55:A57 B58 A59:A63 B64 A65:A80 B81 A82:A85 B86 A87:A104 B105 A106:A109 B110 A111:A120 B121 A122:A133 B134 A135:A145 B146 A147:A176 B177 A178:A195 B196 A197:A203 B204 A205:A219 B220 A221:A227 B228 A229:A246 B247 A248:A264 B265 A266:A272 B273 A274:A278 B279 A280:A1048576">
       <formula1>Task_type</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6 E2 D22:D23 D7:D8 E9 D10:D16 E17 D18:D20 E21 D3:D5 E24 D25:D27 E28 E32 D29:D31 D33:D34 E35 D36:D37 E38 D39:D53 E54 D55:D57 E58 D59:D63 E64 D65:D80 E81 D82:D85 E86 D87:D104 E105 D106:D109 E110 D111:D120 E121 D122:D133 E134 D135:D145 E146 D147:D176 E177 D178:D195 E196 D197:D203 E204 D205:D219 E220 D221:D227 E228 D229:D246 E247 D248:D264 E265 D266:D272 E273 D274:D278 E279 D280:D1034 D1035:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6 E2 D22:D23 D7:D8 E9 D10:D16 E17 D18:D20 E21 D3:D5 E24 D25:D27 E28 E32 D29:D31 D33:D34 E35 D36:D37 E38 D39:D53 E54 D55:D57 E58 D59:D63 E64 D65:D80 E81 D82:D85 E86 D87:D104 E105 D106:D109 E110 D111:D120 E121 D122:D133 E134 D135:D145 E146 D147:D176 E177 D178:D195 E196 D197:D203 E204 D205:D219 E220 D221:D227 E228 D229:D246 E247 D248:D264 E265 D266:D272 E273 D274:D278 E279 D280:D1048576">
       <formula1>Building</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 A2 A9 A17 A21 A24 A28 A32 A35 A38 A54 A58 A64 A81 A86 A105 A110 A121 A134 A146 A177 A196 A204 A220 A228 A247 A265 A273 A279">

</xml_diff>

<commit_message>
Update files and switching to Production mode. Added a lock to the Zone function
</commit_message>
<xml_diff>
--- a/CLASSOPS/Derek/Derek's Log.xlsx
+++ b/CLASSOPS/Derek/Derek's Log.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5199" uniqueCount="637">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5230" uniqueCount="642">
   <si>
     <t>Staff Name</t>
   </si>
@@ -2915,6 +2915,67 @@
   </si>
   <si>
     <t>No tasks today, only Crestron Logouts where applicable.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">No tasks today, only Crestron Logouts where applicable. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Please note: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Nat Taylor Cinema is not is use today.</t>
+    </r>
+  </si>
+  <si>
+    <t>Set out the neck microphone and test the batteries.</t>
+  </si>
+  <si>
+    <t>Login for the client--no codes. Event starts at 6pm but they want setup done at 5pm. Event ends at 7pm.</t>
+  </si>
+  <si>
+    <t>Return neck mic to drawer and log out of the PC and Crestron. I mention this because the event is not shown on the RAC report for today and would not have come up as a Crestron logout.</t>
+  </si>
+  <si>
+    <r>
+      <t>Return lectern mic, 2 desk mic, projector remote and presentation remote to back booth and lock it. Retract the electric screen and turn off all lights. Lock room (</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2 entrances</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) with N940 keys from Ross S120 store.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -3507,11 +3568,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I1187"/>
+  <dimension ref="A1:I1198"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1175" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1187" sqref="B1187"/>
+      <pane ySplit="1" topLeftCell="A1184" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C1199" sqref="C1199"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25111,6 +25172,162 @@
       </c>
       <c r="F1187" s="20" t="s">
         <v>636</v>
+      </c>
+    </row>
+    <row r="1188" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1188" s="6"/>
+      <c r="B1188" s="23"/>
+      <c r="C1188" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="D1188" s="6"/>
+      <c r="E1188" s="27"/>
+      <c r="F1188" s="29"/>
+    </row>
+    <row r="1189" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B1189" s="41">
+        <v>42836</v>
+      </c>
+      <c r="F1189" s="20" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1190" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1190" s="6"/>
+      <c r="B1190" s="23"/>
+      <c r="C1190" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D1190" s="6"/>
+      <c r="E1190" s="27"/>
+      <c r="F1190" s="29"/>
+    </row>
+    <row r="1191" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1191" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1191" s="41">
+        <v>42837</v>
+      </c>
+      <c r="C1191" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="D1191" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1191" s="19" t="s">
+        <v>411</v>
+      </c>
+      <c r="F1191" s="20" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="1192" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1192" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1192" s="41">
+        <v>42837</v>
+      </c>
+      <c r="C1192" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="D1192" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1192" s="19" t="s">
+        <v>411</v>
+      </c>
+      <c r="F1192" s="20" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="1193" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1193" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1193" s="41">
+        <v>42837</v>
+      </c>
+      <c r="C1193" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1193" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1193" s="19" t="s">
+        <v>411</v>
+      </c>
+      <c r="F1193" s="20" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="1194" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1194" s="6"/>
+      <c r="B1194" s="23"/>
+      <c r="C1194" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="D1194" s="6"/>
+      <c r="E1194" s="27"/>
+      <c r="F1194" s="29"/>
+    </row>
+    <row r="1195" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1195" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1195" s="41">
+        <v>42838</v>
+      </c>
+      <c r="C1195" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D1195" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1195" s="19" t="s">
+        <v>277</v>
+      </c>
+      <c r="F1195" s="20" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="1196" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1196" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1196" s="41">
+        <v>42838</v>
+      </c>
+      <c r="C1196" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="D1196" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1196" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="F1196" s="20" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="1197" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1197" s="6"/>
+      <c r="B1197" s="23"/>
+      <c r="C1197" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="D1197" s="6"/>
+      <c r="E1197" s="27"/>
+      <c r="F1197" s="29"/>
+    </row>
+    <row r="1198" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B1198" s="41">
+        <v>42843</v>
+      </c>
+      <c r="F1198" s="20" t="s">
+        <v>637</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Switch to DEBUG mode, demo functions.
</commit_message>
<xml_diff>
--- a/CLASSOPS/Derek/Derek's Log.xlsx
+++ b/CLASSOPS/Derek/Derek's Log.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5230" uniqueCount="642">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5309" uniqueCount="647">
   <si>
     <t>Staff Name</t>
   </si>
@@ -2976,6 +2976,67 @@
       </rPr>
       <t>) with N940 keys from Ross S120 store.</t>
     </r>
+  </si>
+  <si>
+    <t>2 audience mic, 2 desk mics, stands, cables, carpets and mixer, but leave lectern carpet and cable in place. Turn off PA system and lock room with key from FDRS 164. Equipment to FDRS 156A.</t>
+  </si>
+  <si>
+    <r>
+      <t>Return neck mic, projector remote and presentation remote to back booth and lock it. Retract the electric screen and turn off all lights. Lock room (</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2 entrances</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) with N940 keys from Ross S120 store.</t>
+    </r>
+  </si>
+  <si>
+    <t>Return web cam and tripod to Ross S120 store.</t>
+  </si>
+  <si>
+    <r>
+      <t>Leave mics and mixer in place (not Skype kit) for Saturday's continuation of this conference. Turn off projector, computer and audio rack in the back. Turn off all lights and lock room (</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2 entrances</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) with N940 keys from Ross S120 store.</t>
+    </r>
+  </si>
+  <si>
+    <t>1 audience mic, 1 neck mic, stand, cables, and carpets, but leave lectern carpet and cable in place. Turn off PA system and lock room with key from FDRS 164. Equipment to FDRS 156A.</t>
   </si>
 </sst>
 </file>
@@ -3568,11 +3629,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I1198"/>
+  <dimension ref="A1:I1217"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1184" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1199" sqref="C1199"/>
+      <pane ySplit="1" topLeftCell="A1202" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1214" sqref="A1214:F1217"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25328,6 +25389,346 @@
       </c>
       <c r="F1198" s="20" t="s">
         <v>637</v>
+      </c>
+    </row>
+    <row r="1199" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1199" s="6"/>
+      <c r="B1199" s="23"/>
+      <c r="C1199" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D1199" s="6"/>
+      <c r="E1199" s="27"/>
+      <c r="F1199" s="29"/>
+    </row>
+    <row r="1200" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1200" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1200" s="41">
+        <v>42844</v>
+      </c>
+      <c r="C1200" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="D1200" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1200" s="19" t="s">
+        <v>277</v>
+      </c>
+      <c r="F1200" s="20" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="1201" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1201" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1201" s="41">
+        <v>42844</v>
+      </c>
+      <c r="C1201" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="D1201" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1201" s="19" t="s">
+        <v>381</v>
+      </c>
+      <c r="F1201" s="20" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="1202" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1202" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1202" s="41">
+        <v>42844</v>
+      </c>
+      <c r="C1202" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="D1202" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1202" s="19" t="s">
+        <v>381</v>
+      </c>
+      <c r="F1202" s="20" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="1203" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1203" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1203" s="34">
+        <v>42844</v>
+      </c>
+      <c r="C1203" s="35" t="s">
+        <v>226</v>
+      </c>
+      <c r="D1203" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1203" s="37" t="s">
+        <v>136</v>
+      </c>
+      <c r="F1203" s="20" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="1204" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1204" s="6"/>
+      <c r="B1204" s="23"/>
+      <c r="C1204" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="D1204" s="6"/>
+      <c r="E1204" s="27"/>
+      <c r="F1204" s="29"/>
+    </row>
+    <row r="1205" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1205" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1205" s="41">
+        <v>42845</v>
+      </c>
+      <c r="C1205" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1205" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1205" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="F1205" s="20" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="1206" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1206" s="6"/>
+      <c r="B1206" s="23"/>
+      <c r="C1206" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="D1206" s="6"/>
+      <c r="E1206" s="27"/>
+      <c r="F1206" s="29"/>
+    </row>
+    <row r="1207" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1207" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1207" s="41">
+        <v>42846</v>
+      </c>
+      <c r="C1207" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D1207" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1207" s="19" t="s">
+        <v>277</v>
+      </c>
+      <c r="F1207" s="20" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="1208" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1208" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1208" s="41">
+        <v>42846</v>
+      </c>
+      <c r="C1208" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1208" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1208" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="F1208" s="20" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="1209" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1209" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1209" s="41">
+        <v>42846</v>
+      </c>
+      <c r="C1209" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1209" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1209" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="F1209" s="20" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="1210" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1210" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1210" s="41">
+        <v>42846</v>
+      </c>
+      <c r="C1210" s="17" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1210" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1210" s="19" t="s">
+        <v>381</v>
+      </c>
+      <c r="F1210" s="20" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="1211" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1211" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1211" s="41">
+        <v>42846</v>
+      </c>
+      <c r="C1211" s="17" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1211" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1211" s="19" t="s">
+        <v>381</v>
+      </c>
+      <c r="F1211" s="20" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="1212" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1212" s="6"/>
+      <c r="B1212" s="23"/>
+      <c r="C1212" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D1212" s="6"/>
+      <c r="E1212" s="27"/>
+      <c r="F1212" s="29"/>
+    </row>
+    <row r="1213" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1213" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1213" s="41">
+        <v>42849</v>
+      </c>
+      <c r="C1213" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D1213" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1213" s="19" t="s">
+        <v>277</v>
+      </c>
+      <c r="F1213" s="20" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="1214" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1214" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1214" s="41">
+        <v>42849</v>
+      </c>
+      <c r="C1214" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1214" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1214" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="F1214" s="20" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="1215" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1215" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1215" s="41">
+        <v>42849</v>
+      </c>
+      <c r="C1215" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1215" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1215" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="F1215" s="20" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="1216" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1216" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1216" s="41">
+        <v>42849</v>
+      </c>
+      <c r="C1216" s="17" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1216" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1216" s="19" t="s">
+        <v>381</v>
+      </c>
+      <c r="F1216" s="20" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="1217" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1217" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1217" s="41">
+        <v>42849</v>
+      </c>
+      <c r="C1217" s="17" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1217" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1217" s="19" t="s">
+        <v>381</v>
+      </c>
+      <c r="F1217" s="20" t="s">
+        <v>646</v>
       </c>
     </row>
   </sheetData>

</xml_diff>